<commit_message>
Fixed UI for new reports and show. Added an is_absent? method and also added a function for sick leave to be equal to 1 if employee is absent.
</commit_message>
<xml_diff>
--- a/exceltocsv/public/reports/DTRSUMMARY.xlsx
+++ b/exceltocsv/public/reports/DTRSUMMARY.xlsx
@@ -9,12 +9,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="169">
   <si>
     <t>iRipple, Inc.</t>
   </si>
   <si>
-    <t>DTR Summary Sheet for the period March 07, 2015 to March 20, 2015</t>
+    <t>DTR Summary Sheet for the period February 10, 2015 to February 20, 2015</t>
   </si>
   <si>
     <t> </t>
@@ -245,13 +245,10 @@
     <t>emp.department</t>
   </si>
   <si>
-    <t>0.1.30</t>
+    <t>0.0.15</t>
   </si>
   <si>
-    <t>0.1.15</t>
-  </si>
-  <si>
-    <t>2.0.0</t>
+    <t>0.0.0</t>
   </si>
   <si>
     <t>7.5.0</t>
@@ -260,16 +257,7 @@
     <t>1.0.0</t>
   </si>
   <si>
-    <t>6.5.0</t>
-  </si>
-  <si>
-    <t>0.4.30</t>
-  </si>
-  <si>
-    <t>0.6.30</t>
-  </si>
-  <si>
-    <t>0.0.0</t>
+    <t>1.0.00</t>
   </si>
   <si>
     <t>0.0.00</t>
@@ -287,16 +275,25 @@
     <t>Ardamoy,Ma. Rica Catherine</t>
   </si>
   <si>
+    <t>0.4.00</t>
+  </si>
+  <si>
     <t>Bacani,Eddie Marie</t>
   </si>
   <si>
     <t>Bagaindoc,Kjell</t>
   </si>
   <si>
+    <t>0.1.15</t>
+  </si>
+  <si>
     <t>Balingit,Barbara</t>
   </si>
   <si>
     <t>5.5.0</t>
+  </si>
+  <si>
+    <t>4.5.0</t>
   </si>
   <si>
     <t>Balino,Kamille Diane</t>
@@ -308,34 +305,28 @@
     <t>Bayogos,Charmaine</t>
   </si>
   <si>
-    <t>3.0.0</t>
+    <t>0.1.30</t>
   </si>
   <si>
     <t>Bonita,Reynaldo Jr</t>
   </si>
   <si>
-    <t>2.5.0</t>
+    <t>0.2.30</t>
+  </si>
+  <si>
+    <t>4.0.0</t>
   </si>
   <si>
     <t>Borlagdan,Aldrin</t>
   </si>
   <si>
-    <t>0.0.45</t>
-  </si>
-  <si>
     <t>Brayles,Janwil</t>
   </si>
   <si>
-    <t>1.0.45</t>
+    <t>Buena,Ian Christopher</t>
   </si>
   <si>
-    <t>0.1.0</t>
-  </si>
-  <si>
-    <t>4.5.0</t>
-  </si>
-  <si>
-    <t>Buena,Ian Christopher</t>
+    <t>2.5.0</t>
   </si>
   <si>
     <t>Buenafe,Rajiv</t>
@@ -344,13 +335,16 @@
     <t>Cataluna,Christian Gilbert</t>
   </si>
   <si>
+    <t>1.5.0</t>
+  </si>
+  <si>
     <t>CaÃ±ete,Carol Ann</t>
   </si>
   <si>
-    <t>0.6.45</t>
+    <t>0.3.0</t>
   </si>
   <si>
-    <t>0.4.45</t>
+    <t>0.0.30</t>
   </si>
   <si>
     <t>Cerbo,Jaycer</t>
@@ -359,13 +353,16 @@
     <t>Ching,Mark Angelo</t>
   </si>
   <si>
+    <t>0.1.45</t>
+  </si>
+  <si>
     <t>Cortez,Jomar</t>
   </si>
   <si>
-    <t>Cruz,Cesar</t>
+    <t>6.5.0</t>
   </si>
   <si>
-    <t>0.0.30</t>
+    <t>Cruz,Cesar</t>
   </si>
   <si>
     <t>Delfin,Jonathan</t>
@@ -374,28 +371,25 @@
     <t>Delos Reyes,Jeffrey</t>
   </si>
   <si>
-    <t>0.1.45</t>
+    <t>Dino,Arvin</t>
   </si>
   <si>
-    <t>Dino,Arvin</t>
+    <t>3.0.0</t>
   </si>
   <si>
     <t>Dy,Hubert</t>
   </si>
   <si>
+    <t>2.0.0</t>
+  </si>
+  <si>
     <t>Egamino,Ellen</t>
   </si>
   <si>
-    <t>0.3.00</t>
-  </si>
-  <si>
-    <t>0.4.00</t>
+    <t>1.5.00</t>
   </si>
   <si>
     <t>Enrique,Christian Dan</t>
-  </si>
-  <si>
-    <t>1.5.0</t>
   </si>
   <si>
     <t>Espiritu,Carl Philip</t>
@@ -404,16 +398,16 @@
     <t>Flores,Arianne Grace</t>
   </si>
   <si>
-    <t>Francisco,Roed Ronualdo </t>
+    <t>0.6.30</t>
   </si>
   <si>
-    <t>0.0.15</t>
+    <t>Francisco,Roed Ronualdo </t>
   </si>
   <si>
     <t>Gatan,Mario Haris Jr</t>
   </si>
   <si>
-    <t>4.0.0</t>
+    <t>1.4.00</t>
   </si>
   <si>
     <t>Javier,Victor </t>
@@ -428,7 +422,7 @@
     <t>Laroza,Baltazar</t>
   </si>
   <si>
-    <t>0.2.30</t>
+    <t>0.0.45</t>
   </si>
   <si>
     <t>Laude,Ted Marty</t>
@@ -437,19 +431,28 @@
     <t>Ledesma,Jesse</t>
   </si>
   <si>
-    <t>2.1.30</t>
+    <t>0.6.00</t>
+  </si>
+  <si>
+    <t>0.2.00</t>
   </si>
   <si>
     <t>Mangundayao,Mac Donald</t>
   </si>
   <si>
-    <t>1.6.00</t>
+    <t>1.2.45</t>
   </si>
   <si>
     <t>Matias,Ma. Jeremia Jetheth </t>
   </si>
   <si>
+    <t>0.6.45</t>
+  </si>
+  <si>
     <t>Mendoza,Diana</t>
+  </si>
+  <si>
+    <t>0.4.30</t>
   </si>
   <si>
     <t>Nagnal,Fracy</t>
@@ -467,9 +470,6 @@
     <t>Pendre,Contessa</t>
   </si>
   <si>
-    <t>7.0.0</t>
-  </si>
-  <si>
     <t>Ranes,Jonathan</t>
   </si>
   <si>
@@ -482,13 +482,7 @@
     <t>Sanoria,Samuel</t>
   </si>
   <si>
-    <t>0.2.0</t>
-  </si>
-  <si>
     <t>Santos,Patricia</t>
-  </si>
-  <si>
-    <t>1.5.00</t>
   </si>
   <si>
     <t>See,Jenilyn</t>
@@ -497,28 +491,19 @@
     <t>Solbita,Felmar</t>
   </si>
   <si>
-    <t>0.2.00</t>
+    <t>Soriano,Hans Josif</t>
   </si>
   <si>
-    <t>Soriano,Hans Josif</t>
+    <t>Suarez,Katrina </t>
   </si>
   <si>
     <t>0.2.45</t>
   </si>
   <si>
-    <t>6.0.0</t>
-  </si>
-  <si>
-    <t>Suarez,Katrina </t>
-  </si>
-  <si>
     <t>Tanqueco,Mikee Dorina</t>
   </si>
   <si>
-    <t>0.3.15</t>
-  </si>
-  <si>
-    <t>1.0.00</t>
+    <t>1.7.00</t>
   </si>
   <si>
     <t>Tesoro,Rose Natalie</t>
@@ -653,7 +638,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="87.13483146067415"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="93.73483146067416"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="21.789887640449443"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="21.134831460674157" hidden="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="17.834831460674156"/>
@@ -1433,16 +1418,16 @@
         <v>79</v>
       </c>
       <c r="G4" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>82</v>
-      </c>
       <c r="J4" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K4" s="5" t="str">
         <f>INT(LEFT(E4,1))</f>
@@ -1553,31 +1538,31 @@
         <f>FLOOR(AS4/8,1,1)&amp;"."&amp;FLOOR(MOD(AS4,8),1,1)&amp;"."&amp;(MOD(AS4,8)-FLOOR(MOD(AS4,8),1,1))*60</f>
       </c>
       <c r="AU4" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AV4" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AW4" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX4" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY4" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ4" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA4" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB4" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC4" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD4" s="5" t="str">
         <f>INT(LEFT(AU4,1))</f>
@@ -1741,7 +1726,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>77</v>
@@ -1750,22 +1735,22 @@
         <v>0</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="K5" s="5" t="str">
         <f>INT(LEFT(E5,1))</f>
@@ -1876,31 +1861,31 @@
         <f>FLOOR(AS5/8,1,1)&amp;"."&amp;FLOOR(MOD(AS5,8),1,1)&amp;"."&amp;(MOD(AS5,8)-FLOOR(MOD(AS5,8),1,1))*60</f>
       </c>
       <c r="AU5" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV5" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW5" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX5" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY5" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ5" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA5" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB5" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC5" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD5" s="5" t="str">
         <f>INT(LEFT(AU5,1))</f>
@@ -2064,7 +2049,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>77</v>
@@ -2073,22 +2058,22 @@
         <v>0</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K6" s="5" t="str">
         <f>INT(LEFT(E6,1))</f>
@@ -2199,31 +2184,31 @@
         <f>FLOOR(AS6/8,1,1)&amp;"."&amp;FLOOR(MOD(AS6,8),1,1)&amp;"."&amp;(MOD(AS6,8)-FLOOR(MOD(AS6,8),1,1))*60</f>
       </c>
       <c r="AU6" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AV6" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="AW6" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX6" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY6" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ6" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA6" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB6" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC6" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD6" s="5" t="str">
         <f>INT(LEFT(AU6,1))</f>
@@ -2387,7 +2372,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>77</v>
@@ -2396,22 +2381,22 @@
         <v>0</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K7" s="5" t="str">
         <f>INT(LEFT(E7,1))</f>
@@ -2522,31 +2507,31 @@
         <f>FLOOR(AS7/8,1,1)&amp;"."&amp;FLOOR(MOD(AS7,8),1,1)&amp;"."&amp;(MOD(AS7,8)-FLOOR(MOD(AS7,8),1,1))*60</f>
       </c>
       <c r="AU7" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV7" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW7" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX7" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY7" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ7" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA7" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB7" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC7" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD7" s="5" t="str">
         <f>INT(LEFT(AU7,1))</f>
@@ -2710,7 +2695,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>77</v>
@@ -2719,22 +2704,22 @@
         <v>0</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K8" s="5" t="str">
         <f>INT(LEFT(E8,1))</f>
@@ -2845,31 +2830,31 @@
         <f>FLOOR(AS8/8,1,1)&amp;"."&amp;FLOOR(MOD(AS8,8),1,1)&amp;"."&amp;(MOD(AS8,8)-FLOOR(MOD(AS8,8),1,1))*60</f>
       </c>
       <c r="AU8" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV8" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW8" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX8" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY8" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ8" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA8" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB8" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC8" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD8" s="5" t="str">
         <f>INT(LEFT(AU8,1))</f>
@@ -3033,7 +3018,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>77</v>
@@ -3042,22 +3027,22 @@
         <v>0</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="K9" s="5" t="str">
         <f>INT(LEFT(E9,1))</f>
@@ -3168,31 +3153,31 @@
         <f>FLOOR(AS9/8,1,1)&amp;"."&amp;FLOOR(MOD(AS9,8),1,1)&amp;"."&amp;(MOD(AS9,8)-FLOOR(MOD(AS9,8),1,1))*60</f>
       </c>
       <c r="AU9" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV9" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW9" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX9" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY9" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ9" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA9" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB9" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC9" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD9" s="5" t="str">
         <f>INT(LEFT(AU9,1))</f>
@@ -3356,7 +3341,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>77</v>
@@ -3365,22 +3350,22 @@
         <v>0</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K10" s="5" t="str">
         <f>INT(LEFT(E10,1))</f>
@@ -3491,31 +3476,31 @@
         <f>FLOOR(AS10/8,1,1)&amp;"."&amp;FLOOR(MOD(AS10,8),1,1)&amp;"."&amp;(MOD(AS10,8)-FLOOR(MOD(AS10,8),1,1))*60</f>
       </c>
       <c r="AU10" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV10" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW10" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX10" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY10" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ10" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA10" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB10" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC10" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD10" s="5" t="str">
         <f>INT(LEFT(AU10,1))</f>
@@ -3679,7 +3664,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>77</v>
@@ -3688,22 +3673,22 @@
         <v>0</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K11" s="5" t="str">
         <f>INT(LEFT(E11,1))</f>
@@ -3814,31 +3799,31 @@
         <f>FLOOR(AS11/8,1,1)&amp;"."&amp;FLOOR(MOD(AS11,8),1,1)&amp;"."&amp;(MOD(AS11,8)-FLOOR(MOD(AS11,8),1,1))*60</f>
       </c>
       <c r="AU11" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV11" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW11" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX11" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY11" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ11" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA11" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB11" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC11" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD11" s="5" t="str">
         <f>INT(LEFT(AU11,1))</f>
@@ -4002,31 +3987,31 @@
         <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D12" s="5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>86</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K12" s="5" t="str">
         <f>INT(LEFT(E12,1))</f>
@@ -4137,31 +4122,31 @@
         <f>FLOOR(AS12/8,1,1)&amp;"."&amp;FLOOR(MOD(AS12,8),1,1)&amp;"."&amp;(MOD(AS12,8)-FLOOR(MOD(AS12,8),1,1))*60</f>
       </c>
       <c r="AU12" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV12" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW12" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX12" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY12" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ12" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA12" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB12" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC12" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD12" s="5" t="str">
         <f>INT(LEFT(AU12,1))</f>
@@ -4325,31 +4310,31 @@
         <v>10</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>101</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K13" s="5" t="str">
         <f>INT(LEFT(E13,1))</f>
@@ -4460,31 +4445,31 @@
         <f>FLOOR(AS13/8,1,1)&amp;"."&amp;FLOOR(MOD(AS13,8),1,1)&amp;"."&amp;(MOD(AS13,8)-FLOOR(MOD(AS13,8),1,1))*60</f>
       </c>
       <c r="AU13" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV13" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW13" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX13" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY13" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ13" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA13" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB13" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC13" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD13" s="5" t="str">
         <f>INT(LEFT(AU13,1))</f>
@@ -4654,25 +4639,25 @@
         <v>77</v>
       </c>
       <c r="D14" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K14" s="5" t="str">
         <f>INT(LEFT(E14,1))</f>
@@ -4783,31 +4768,31 @@
         <f>FLOOR(AS14/8,1,1)&amp;"."&amp;FLOOR(MOD(AS14,8),1,1)&amp;"."&amp;(MOD(AS14,8)-FLOOR(MOD(AS14,8),1,1))*60</f>
       </c>
       <c r="AU14" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV14" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW14" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX14" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY14" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ14" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA14" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB14" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC14" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD14" s="5" t="str">
         <f>INT(LEFT(AU14,1))</f>
@@ -4971,31 +4956,31 @@
         <v>12</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D15" s="5" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="K15" s="5" t="str">
         <f>INT(LEFT(E15,1))</f>
@@ -5106,31 +5091,31 @@
         <f>FLOOR(AS15/8,1,1)&amp;"."&amp;FLOOR(MOD(AS15,8),1,1)&amp;"."&amp;(MOD(AS15,8)-FLOOR(MOD(AS15,8),1,1))*60</f>
       </c>
       <c r="AU15" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV15" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW15" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX15" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY15" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ15" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA15" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB15" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC15" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD15" s="5" t="str">
         <f>INT(LEFT(AU15,1))</f>
@@ -5294,31 +5279,31 @@
         <v>13</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D16" s="5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K16" s="5" t="str">
         <f>INT(LEFT(E16,1))</f>
@@ -5429,31 +5414,31 @@
         <f>FLOOR(AS16/8,1,1)&amp;"."&amp;FLOOR(MOD(AS16,8),1,1)&amp;"."&amp;(MOD(AS16,8)-FLOOR(MOD(AS16,8),1,1))*60</f>
       </c>
       <c r="AU16" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV16" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW16" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX16" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY16" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ16" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA16" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB16" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC16" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD16" s="5" t="str">
         <f>INT(LEFT(AU16,1))</f>
@@ -5617,7 +5602,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>77</v>
@@ -5626,22 +5611,22 @@
         <v>0</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="K17" s="5" t="str">
         <f>INT(LEFT(E17,1))</f>
@@ -5752,31 +5737,31 @@
         <f>FLOOR(AS17/8,1,1)&amp;"."&amp;FLOOR(MOD(AS17,8),1,1)&amp;"."&amp;(MOD(AS17,8)-FLOOR(MOD(AS17,8),1,1))*60</f>
       </c>
       <c r="AU17" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV17" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW17" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX17" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY17" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ17" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA17" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB17" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC17" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD17" s="5" t="str">
         <f>INT(LEFT(AU17,1))</f>
@@ -5940,7 +5925,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>77</v>
@@ -5949,22 +5934,22 @@
         <v>0</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="K18" s="5" t="str">
         <f>INT(LEFT(E18,1))</f>
@@ -6075,31 +6060,31 @@
         <f>FLOOR(AS18/8,1,1)&amp;"."&amp;FLOOR(MOD(AS18,8),1,1)&amp;"."&amp;(MOD(AS18,8)-FLOOR(MOD(AS18,8),1,1))*60</f>
       </c>
       <c r="AU18" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV18" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW18" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX18" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY18" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ18" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA18" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB18" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC18" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD18" s="5" t="str">
         <f>INT(LEFT(AU18,1))</f>
@@ -6263,31 +6248,31 @@
         <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D19" s="5" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K19" s="5" t="str">
         <f>INT(LEFT(E19,1))</f>
@@ -6398,31 +6383,31 @@
         <f>FLOOR(AS19/8,1,1)&amp;"."&amp;FLOOR(MOD(AS19,8),1,1)&amp;"."&amp;(MOD(AS19,8)-FLOOR(MOD(AS19,8),1,1))*60</f>
       </c>
       <c r="AU19" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV19" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW19" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX19" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY19" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ19" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA19" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB19" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC19" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD19" s="5" t="str">
         <f>INT(LEFT(AU19,1))</f>
@@ -6586,7 +6571,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>77</v>
@@ -6595,22 +6580,22 @@
         <v>0</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K20" s="5" t="str">
         <f>INT(LEFT(E20,1))</f>
@@ -6721,31 +6706,31 @@
         <f>FLOOR(AS20/8,1,1)&amp;"."&amp;FLOOR(MOD(AS20,8),1,1)&amp;"."&amp;(MOD(AS20,8)-FLOOR(MOD(AS20,8),1,1))*60</f>
       </c>
       <c r="AU20" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV20" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW20" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX20" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY20" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ20" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA20" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB20" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC20" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD20" s="5" t="str">
         <f>INT(LEFT(AU20,1))</f>
@@ -6909,7 +6894,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>77</v>
@@ -6918,22 +6903,22 @@
         <v>0</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K21" s="5" t="str">
         <f>INT(LEFT(E21,1))</f>
@@ -7044,31 +7029,31 @@
         <f>FLOOR(AS21/8,1,1)&amp;"."&amp;FLOOR(MOD(AS21,8),1,1)&amp;"."&amp;(MOD(AS21,8)-FLOOR(MOD(AS21,8),1,1))*60</f>
       </c>
       <c r="AU21" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV21" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW21" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX21" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY21" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ21" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA21" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB21" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC21" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD21" s="5" t="str">
         <f>INT(LEFT(AU21,1))</f>
@@ -7232,7 +7217,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>77</v>
@@ -7241,22 +7226,22 @@
         <v>0</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="K22" s="5" t="str">
         <f>INT(LEFT(E22,1))</f>
@@ -7367,31 +7352,31 @@
         <f>FLOOR(AS22/8,1,1)&amp;"."&amp;FLOOR(MOD(AS22,8),1,1)&amp;"."&amp;(MOD(AS22,8)-FLOOR(MOD(AS22,8),1,1))*60</f>
       </c>
       <c r="AU22" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV22" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW22" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX22" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY22" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ22" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA22" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB22" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC22" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD22" s="5" t="str">
         <f>INT(LEFT(AU22,1))</f>
@@ -7564,22 +7549,22 @@
         <v>0</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>118</v>
+        <v>79</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="K23" s="5" t="str">
         <f>INT(LEFT(E23,1))</f>
@@ -7690,31 +7675,31 @@
         <f>FLOOR(AS23/8,1,1)&amp;"."&amp;FLOOR(MOD(AS23,8),1,1)&amp;"."&amp;(MOD(AS23,8)-FLOOR(MOD(AS23,8),1,1))*60</f>
       </c>
       <c r="AU23" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV23" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW23" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX23" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY23" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ23" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA23" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB23" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC23" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD23" s="5" t="str">
         <f>INT(LEFT(AU23,1))</f>
@@ -7878,31 +7863,31 @@
         <v>21</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D24" s="5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="K24" s="5" t="str">
         <f>INT(LEFT(E24,1))</f>
@@ -8013,31 +7998,31 @@
         <f>FLOOR(AS24/8,1,1)&amp;"."&amp;FLOOR(MOD(AS24,8),1,1)&amp;"."&amp;(MOD(AS24,8)-FLOOR(MOD(AS24,8),1,1))*60</f>
       </c>
       <c r="AU24" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV24" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW24" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX24" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY24" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ24" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA24" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB24" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC24" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD24" s="5" t="str">
         <f>INT(LEFT(AU24,1))</f>
@@ -8201,31 +8186,31 @@
         <v>22</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D25" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>121</v>
+        <v>78</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K25" s="5" t="str">
         <f>INT(LEFT(E25,1))</f>
@@ -8336,31 +8321,31 @@
         <f>FLOOR(AS25/8,1,1)&amp;"."&amp;FLOOR(MOD(AS25,8),1,1)&amp;"."&amp;(MOD(AS25,8)-FLOOR(MOD(AS25,8),1,1))*60</f>
       </c>
       <c r="AU25" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV25" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW25" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX25" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY25" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ25" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA25" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB25" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC25" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD25" s="5" t="str">
         <f>INT(LEFT(AU25,1))</f>
@@ -8524,7 +8509,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>77</v>
@@ -8533,22 +8518,22 @@
         <v>0</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>79</v>
+        <v>111</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>89</v>
+        <v>121</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="K26" s="5" t="str">
         <f>INT(LEFT(E26,1))</f>
@@ -8659,31 +8644,31 @@
         <f>FLOOR(AS26/8,1,1)&amp;"."&amp;FLOOR(MOD(AS26,8),1,1)&amp;"."&amp;(MOD(AS26,8)-FLOOR(MOD(AS26,8),1,1))*60</f>
       </c>
       <c r="AU26" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV26" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW26" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX26" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY26" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ26" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA26" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB26" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC26" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD26" s="5" t="str">
         <f>INT(LEFT(AU26,1))</f>
@@ -8847,7 +8832,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>77</v>
@@ -8856,22 +8841,22 @@
         <v>0</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K27" s="5" t="str">
         <f>INT(LEFT(E27,1))</f>
@@ -8982,31 +8967,31 @@
         <f>FLOOR(AS27/8,1,1)&amp;"."&amp;FLOOR(MOD(AS27,8),1,1)&amp;"."&amp;(MOD(AS27,8)-FLOOR(MOD(AS27,8),1,1))*60</f>
       </c>
       <c r="AU27" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV27" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW27" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX27" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY27" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ27" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA27" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB27" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC27" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD27" s="5" t="str">
         <f>INT(LEFT(AU27,1))</f>
@@ -9176,25 +9161,25 @@
         <v>77</v>
       </c>
       <c r="D28" s="5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="I28" s="5" t="s">
         <v>86</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="K28" s="5" t="str">
         <f>INT(LEFT(E28,1))</f>
@@ -9305,31 +9290,31 @@
         <f>FLOOR(AS28/8,1,1)&amp;"."&amp;FLOOR(MOD(AS28,8),1,1)&amp;"."&amp;(MOD(AS28,8)-FLOOR(MOD(AS28,8),1,1))*60</f>
       </c>
       <c r="AU28" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AV28" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AW28" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="AV28" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="AW28" s="5" t="s">
-        <v>86</v>
-      </c>
       <c r="AX28" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY28" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ28" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA28" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB28" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC28" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD28" s="5" t="str">
         <f>INT(LEFT(AU28,1))</f>
@@ -9493,7 +9478,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>77</v>
@@ -9502,22 +9487,22 @@
         <v>0</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>121</v>
+        <v>79</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K29" s="5" t="str">
         <f>INT(LEFT(E29,1))</f>
@@ -9628,31 +9613,31 @@
         <f>FLOOR(AS29/8,1,1)&amp;"."&amp;FLOOR(MOD(AS29,8),1,1)&amp;"."&amp;(MOD(AS29,8)-FLOOR(MOD(AS29,8),1,1))*60</f>
       </c>
       <c r="AU29" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV29" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW29" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX29" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY29" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ29" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA29" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB29" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC29" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD29" s="5" t="str">
         <f>INT(LEFT(AU29,1))</f>
@@ -9816,31 +9801,31 @@
         <v>27</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D30" s="5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="K30" s="5" t="str">
         <f>INT(LEFT(E30,1))</f>
@@ -9951,31 +9936,31 @@
         <f>FLOOR(AS30/8,1,1)&amp;"."&amp;FLOOR(MOD(AS30,8),1,1)&amp;"."&amp;(MOD(AS30,8)-FLOOR(MOD(AS30,8),1,1))*60</f>
       </c>
       <c r="AU30" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV30" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW30" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX30" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY30" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ30" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA30" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB30" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC30" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD30" s="5" t="str">
         <f>INT(LEFT(AU30,1))</f>
@@ -10139,7 +10124,7 @@
         <v>28</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>77</v>
@@ -10148,22 +10133,22 @@
         <v>2</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="F31" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="G31" s="5" t="s">
-        <v>90</v>
-      </c>
       <c r="H31" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K31" s="5" t="str">
         <f>INT(LEFT(E31,1))</f>
@@ -10274,31 +10259,31 @@
         <f>FLOOR(AS31/8,1,1)&amp;"."&amp;FLOOR(MOD(AS31,8),1,1)&amp;"."&amp;(MOD(AS31,8)-FLOOR(MOD(AS31,8),1,1))*60</f>
       </c>
       <c r="AU31" s="5" t="s">
-        <v>87</v>
+        <v>129</v>
       </c>
       <c r="AV31" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW31" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX31" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY31" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ31" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA31" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB31" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC31" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD31" s="5" t="str">
         <f>INT(LEFT(AU31,1))</f>
@@ -10462,31 +10447,31 @@
         <v>29</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D32" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>132</v>
+        <v>79</v>
       </c>
       <c r="F32" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G32" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="G32" s="5" t="s">
-        <v>128</v>
-      </c>
       <c r="H32" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K32" s="5" t="str">
         <f>INT(LEFT(E32,1))</f>
@@ -10597,31 +10582,31 @@
         <f>FLOOR(AS32/8,1,1)&amp;"."&amp;FLOOR(MOD(AS32,8),1,1)&amp;"."&amp;(MOD(AS32,8)-FLOOR(MOD(AS32,8),1,1))*60</f>
       </c>
       <c r="AU32" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV32" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW32" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX32" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY32" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ32" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA32" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB32" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC32" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD32" s="5" t="str">
         <f>INT(LEFT(AU32,1))</f>
@@ -10785,31 +10770,31 @@
         <v>30</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D33" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>79</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>118</v>
+        <v>79</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>134</v>
+        <v>94</v>
       </c>
       <c r="K33" s="5" t="str">
         <f>INT(LEFT(E33,1))</f>
@@ -10920,31 +10905,31 @@
         <f>FLOOR(AS33/8,1,1)&amp;"."&amp;FLOOR(MOD(AS33,8),1,1)&amp;"."&amp;(MOD(AS33,8)-FLOOR(MOD(AS33,8),1,1))*60</f>
       </c>
       <c r="AU33" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AV33" s="5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="AW33" s="5" t="s">
-        <v>86</v>
+        <v>132</v>
       </c>
       <c r="AX33" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY33" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ33" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA33" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB33" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC33" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD33" s="5" t="str">
         <f>INT(LEFT(AU33,1))</f>
@@ -11108,7 +11093,7 @@
         <v>31</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>77</v>
@@ -11117,22 +11102,22 @@
         <v>0</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K34" s="5" t="str">
         <f>INT(LEFT(E34,1))</f>
@@ -11243,31 +11228,31 @@
         <f>FLOOR(AS34/8,1,1)&amp;"."&amp;FLOOR(MOD(AS34,8),1,1)&amp;"."&amp;(MOD(AS34,8)-FLOOR(MOD(AS34,8),1,1))*60</f>
       </c>
       <c r="AU34" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV34" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW34" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX34" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY34" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ34" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA34" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB34" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC34" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD34" s="5" t="str">
         <f>INT(LEFT(AU34,1))</f>
@@ -11431,7 +11416,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>77</v>
@@ -11440,22 +11425,22 @@
         <v>0</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I35" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J35" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="J35" s="5" t="s">
-        <v>81</v>
       </c>
       <c r="K35" s="5" t="str">
         <f>INT(LEFT(E35,1))</f>
@@ -11566,31 +11551,31 @@
         <f>FLOOR(AS35/8,1,1)&amp;"."&amp;FLOOR(MOD(AS35,8),1,1)&amp;"."&amp;(MOD(AS35,8)-FLOOR(MOD(AS35,8),1,1))*60</f>
       </c>
       <c r="AU35" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV35" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW35" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX35" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY35" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ35" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA35" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB35" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC35" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD35" s="5" t="str">
         <f>INT(LEFT(AU35,1))</f>
@@ -11754,7 +11739,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>77</v>
@@ -11763,22 +11748,22 @@
         <v>0</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K36" s="5" t="str">
         <f>INT(LEFT(E36,1))</f>
@@ -11889,31 +11874,31 @@
         <f>FLOOR(AS36/8,1,1)&amp;"."&amp;FLOOR(MOD(AS36,8),1,1)&amp;"."&amp;(MOD(AS36,8)-FLOOR(MOD(AS36,8),1,1))*60</f>
       </c>
       <c r="AU36" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV36" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW36" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX36" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY36" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ36" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA36" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB36" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC36" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD36" s="5" t="str">
         <f>INT(LEFT(AU36,1))</f>
@@ -12077,31 +12062,31 @@
         <v>34</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D37" s="5" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>132</v>
+        <v>79</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K37" s="5" t="str">
         <f>INT(LEFT(E37,1))</f>
@@ -12212,31 +12197,31 @@
         <f>FLOOR(AS37/8,1,1)&amp;"."&amp;FLOOR(MOD(AS37,8),1,1)&amp;"."&amp;(MOD(AS37,8)-FLOOR(MOD(AS37,8),1,1))*60</f>
       </c>
       <c r="AU37" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV37" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW37" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX37" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY37" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ37" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA37" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB37" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC37" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD37" s="5" t="str">
         <f>INT(LEFT(AU37,1))</f>
@@ -12400,7 +12385,7 @@
         <v>35</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>77</v>
@@ -12409,22 +12394,22 @@
         <v>0</v>
       </c>
       <c r="E38" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J38" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="J38" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="K38" s="5" t="str">
         <f>INT(LEFT(E38,1))</f>
@@ -12535,31 +12520,31 @@
         <f>FLOOR(AS38/8,1,1)&amp;"."&amp;FLOOR(MOD(AS38,8),1,1)&amp;"."&amp;(MOD(AS38,8)-FLOOR(MOD(AS38,8),1,1))*60</f>
       </c>
       <c r="AU38" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV38" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW38" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX38" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY38" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ38" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA38" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB38" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC38" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD38" s="5" t="str">
         <f>INT(LEFT(AU38,1))</f>
@@ -12723,31 +12708,31 @@
         <v>36</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D39" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>132</v>
+        <v>79</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="K39" s="5" t="str">
         <f>INT(LEFT(E39,1))</f>
@@ -12858,31 +12843,31 @@
         <f>FLOOR(AS39/8,1,1)&amp;"."&amp;FLOOR(MOD(AS39,8),1,1)&amp;"."&amp;(MOD(AS39,8)-FLOOR(MOD(AS39,8),1,1))*60</f>
       </c>
       <c r="AU39" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="AV39" s="5" t="s">
-        <v>87</v>
+        <v>141</v>
       </c>
       <c r="AW39" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX39" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY39" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ39" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA39" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB39" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC39" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD39" s="5" t="str">
         <f>INT(LEFT(AU39,1))</f>
@@ -13046,31 +13031,31 @@
         <v>37</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D40" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K40" s="5" t="str">
         <f>INT(LEFT(E40,1))</f>
@@ -13181,31 +13166,31 @@
         <f>FLOOR(AS40/8,1,1)&amp;"."&amp;FLOOR(MOD(AS40,8),1,1)&amp;"."&amp;(MOD(AS40,8)-FLOOR(MOD(AS40,8),1,1))*60</f>
       </c>
       <c r="AU40" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AV40" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW40" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX40" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY40" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ40" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA40" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB40" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC40" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD40" s="5" t="str">
         <f>INT(LEFT(AU40,1))</f>
@@ -13369,7 +13354,7 @@
         <v>38</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>77</v>
@@ -13378,22 +13363,22 @@
         <v>6</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>112</v>
+        <v>145</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="K41" s="5" t="str">
         <f>INT(LEFT(E41,1))</f>
@@ -13504,31 +13489,31 @@
         <f>FLOOR(AS41/8,1,1)&amp;"."&amp;FLOOR(MOD(AS41,8),1,1)&amp;"."&amp;(MOD(AS41,8)-FLOOR(MOD(AS41,8),1,1))*60</f>
       </c>
       <c r="AU41" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV41" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW41" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX41" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY41" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ41" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA41" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB41" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC41" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD41" s="5" t="str">
         <f>INT(LEFT(AU41,1))</f>
@@ -13698,25 +13683,25 @@
         <v>77</v>
       </c>
       <c r="D42" s="5" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>85</v>
+        <v>147</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>132</v>
+        <v>79</v>
       </c>
       <c r="G42" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="H42" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="H42" s="5" t="s">
-        <v>81</v>
-      </c>
       <c r="I42" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K42" s="5" t="str">
         <f>INT(LEFT(E42,1))</f>
@@ -13827,31 +13812,31 @@
         <f>FLOOR(AS42/8,1,1)&amp;"."&amp;FLOOR(MOD(AS42,8),1,1)&amp;"."&amp;(MOD(AS42,8)-FLOOR(MOD(AS42,8),1,1))*60</f>
       </c>
       <c r="AU42" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV42" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW42" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX42" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY42" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ42" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA42" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB42" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC42" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD42" s="5" t="str">
         <f>INT(LEFT(AU42,1))</f>
@@ -14015,7 +14000,7 @@
         <v>40</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>77</v>
@@ -14024,22 +14009,22 @@
         <v>0</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="K43" s="5" t="str">
         <f>INT(LEFT(E43,1))</f>
@@ -14150,31 +14135,31 @@
         <f>FLOOR(AS43/8,1,1)&amp;"."&amp;FLOOR(MOD(AS43,8),1,1)&amp;"."&amp;(MOD(AS43,8)-FLOOR(MOD(AS43,8),1,1))*60</f>
       </c>
       <c r="AU43" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV43" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW43" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX43" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY43" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ43" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA43" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB43" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC43" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD43" s="5" t="str">
         <f>INT(LEFT(AU43,1))</f>
@@ -14338,7 +14323,7 @@
         <v>41</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>77</v>
@@ -14347,22 +14332,22 @@
         <v>0</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>86</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K44" s="5" t="str">
         <f>INT(LEFT(E44,1))</f>
@@ -14473,31 +14458,31 @@
         <f>FLOOR(AS44/8,1,1)&amp;"."&amp;FLOOR(MOD(AS44,8),1,1)&amp;"."&amp;(MOD(AS44,8)-FLOOR(MOD(AS44,8),1,1))*60</f>
       </c>
       <c r="AU44" s="5" t="s">
-        <v>87</v>
+        <v>140</v>
       </c>
       <c r="AV44" s="5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="AW44" s="5" t="s">
-        <v>86</v>
+        <v>132</v>
       </c>
       <c r="AX44" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY44" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ44" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA44" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB44" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC44" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD44" s="5" t="str">
         <f>INT(LEFT(AU44,1))</f>
@@ -14661,31 +14646,31 @@
         <v>42</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D45" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="K45" s="5" t="str">
         <f>INT(LEFT(E45,1))</f>
@@ -14796,31 +14781,31 @@
         <f>FLOOR(AS45/8,1,1)&amp;"."&amp;FLOOR(MOD(AS45,8),1,1)&amp;"."&amp;(MOD(AS45,8)-FLOOR(MOD(AS45,8),1,1))*60</f>
       </c>
       <c r="AU45" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV45" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW45" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX45" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY45" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ45" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA45" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB45" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC45" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD45" s="5" t="str">
         <f>INT(LEFT(AU45,1))</f>
@@ -14984,31 +14969,31 @@
         <v>43</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D46" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>132</v>
+        <v>79</v>
       </c>
       <c r="F46" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H46" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="G46" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="H46" s="5" t="s">
-        <v>90</v>
-      </c>
       <c r="I46" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K46" s="5" t="str">
         <f>INT(LEFT(E46,1))</f>
@@ -15119,31 +15104,31 @@
         <f>FLOOR(AS46/8,1,1)&amp;"."&amp;FLOOR(MOD(AS46,8),1,1)&amp;"."&amp;(MOD(AS46,8)-FLOOR(MOD(AS46,8),1,1))*60</f>
       </c>
       <c r="AU46" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV46" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW46" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX46" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY46" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ46" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA46" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB46" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC46" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD46" s="5" t="str">
         <f>INT(LEFT(AU46,1))</f>
@@ -15307,7 +15292,7 @@
         <v>44</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>77</v>
@@ -15316,22 +15301,22 @@
         <v>0</v>
       </c>
       <c r="E47" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G47" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="F47" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>82</v>
-      </c>
       <c r="H47" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>152</v>
+        <v>80</v>
       </c>
       <c r="K47" s="5" t="str">
         <f>INT(LEFT(E47,1))</f>
@@ -15442,31 +15427,31 @@
         <f>FLOOR(AS47/8,1,1)&amp;"."&amp;FLOOR(MOD(AS47,8),1,1)&amp;"."&amp;(MOD(AS47,8)-FLOOR(MOD(AS47,8),1,1))*60</f>
       </c>
       <c r="AU47" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV47" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW47" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX47" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY47" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ47" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA47" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB47" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC47" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD47" s="5" t="str">
         <f>INT(LEFT(AU47,1))</f>
@@ -15639,22 +15624,22 @@
         <v>0</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K48" s="5" t="str">
         <f>INT(LEFT(E48,1))</f>
@@ -15765,31 +15750,31 @@
         <f>FLOOR(AS48/8,1,1)&amp;"."&amp;FLOOR(MOD(AS48,8),1,1)&amp;"."&amp;(MOD(AS48,8)-FLOOR(MOD(AS48,8),1,1))*60</f>
       </c>
       <c r="AU48" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV48" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW48" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX48" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY48" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ48" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA48" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB48" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC48" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD48" s="5" t="str">
         <f>INT(LEFT(AU48,1))</f>
@@ -15959,25 +15944,25 @@
         <v>77</v>
       </c>
       <c r="D49" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>86</v>
+        <v>137</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K49" s="5" t="str">
         <f>INT(LEFT(E49,1))</f>
@@ -16088,31 +16073,31 @@
         <f>FLOOR(AS49/8,1,1)&amp;"."&amp;FLOOR(MOD(AS49,8),1,1)&amp;"."&amp;(MOD(AS49,8)-FLOOR(MOD(AS49,8),1,1))*60</f>
       </c>
       <c r="AU49" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="AV49" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW49" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX49" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY49" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ49" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA49" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB49" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC49" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD49" s="5" t="str">
         <f>INT(LEFT(AU49,1))</f>
@@ -16282,25 +16267,25 @@
         <v>77</v>
       </c>
       <c r="D50" s="5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>132</v>
+        <v>91</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>128</v>
+        <v>86</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K50" s="5" t="str">
         <f>INT(LEFT(E50,1))</f>
@@ -16411,31 +16396,31 @@
         <f>FLOOR(AS50/8,1,1)&amp;"."&amp;FLOOR(MOD(AS50,8),1,1)&amp;"."&amp;(MOD(AS50,8)-FLOOR(MOD(AS50,8),1,1))*60</f>
       </c>
       <c r="AU50" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV50" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW50" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX50" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY50" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ50" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA50" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB50" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC50" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD50" s="5" t="str">
         <f>INT(LEFT(AU50,1))</f>
@@ -16605,25 +16590,25 @@
         <v>77</v>
       </c>
       <c r="D51" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>157</v>
+        <v>78</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K51" s="5" t="str">
         <f>INT(LEFT(E51,1))</f>
@@ -16734,31 +16719,31 @@
         <f>FLOOR(AS51/8,1,1)&amp;"."&amp;FLOOR(MOD(AS51,8),1,1)&amp;"."&amp;(MOD(AS51,8)-FLOOR(MOD(AS51,8),1,1))*60</f>
       </c>
       <c r="AU51" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV51" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW51" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX51" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY51" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ51" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA51" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB51" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC51" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD51" s="5" t="str">
         <f>INT(LEFT(AU51,1))</f>
@@ -16922,31 +16907,31 @@
         <v>49</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D52" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>118</v>
+        <v>79</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="K52" s="5" t="str">
         <f>INT(LEFT(E52,1))</f>
@@ -17057,31 +17042,31 @@
         <f>FLOOR(AS52/8,1,1)&amp;"."&amp;FLOOR(MOD(AS52,8),1,1)&amp;"."&amp;(MOD(AS52,8)-FLOOR(MOD(AS52,8),1,1))*60</f>
       </c>
       <c r="AU52" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV52" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AW52" s="5" t="s">
-        <v>159</v>
+        <v>79</v>
       </c>
       <c r="AX52" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY52" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ52" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA52" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB52" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC52" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD52" s="5" t="str">
         <f>INT(LEFT(AU52,1))</f>
@@ -17245,7 +17230,7 @@
         <v>50</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>77</v>
@@ -17254,22 +17239,22 @@
         <v>0</v>
       </c>
       <c r="E53" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G53" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="F53" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="G53" s="5" t="s">
-        <v>128</v>
-      </c>
       <c r="H53" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K53" s="5" t="str">
         <f>INT(LEFT(E53,1))</f>
@@ -17380,31 +17365,31 @@
         <f>FLOOR(AS53/8,1,1)&amp;"."&amp;FLOOR(MOD(AS53,8),1,1)&amp;"."&amp;(MOD(AS53,8)-FLOOR(MOD(AS53,8),1,1))*60</f>
       </c>
       <c r="AU53" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV53" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW53" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX53" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY53" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ53" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA53" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB53" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC53" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD53" s="5" t="str">
         <f>INT(LEFT(AU53,1))</f>
@@ -17568,7 +17553,7 @@
         <v>51</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>77</v>
@@ -17577,22 +17562,22 @@
         <v>0</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K54" s="5" t="str">
         <f>INT(LEFT(E54,1))</f>
@@ -17703,31 +17688,31 @@
         <f>FLOOR(AS54/8,1,1)&amp;"."&amp;FLOOR(MOD(AS54,8),1,1)&amp;"."&amp;(MOD(AS54,8)-FLOOR(MOD(AS54,8),1,1))*60</f>
       </c>
       <c r="AU54" s="5" t="s">
-        <v>162</v>
+        <v>83</v>
       </c>
       <c r="AV54" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW54" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX54" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY54" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ54" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA54" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB54" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC54" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD54" s="5" t="str">
         <f>INT(LEFT(AU54,1))</f>
@@ -17891,31 +17876,31 @@
         <v>52</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D55" s="5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>164</v>
+        <v>78</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>165</v>
+        <v>116</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K55" s="5" t="str">
         <f>INT(LEFT(E55,1))</f>
@@ -18026,31 +18011,31 @@
         <f>FLOOR(AS55/8,1,1)&amp;"."&amp;FLOOR(MOD(AS55,8),1,1)&amp;"."&amp;(MOD(AS55,8)-FLOOR(MOD(AS55,8),1,1))*60</f>
       </c>
       <c r="AU55" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="AV55" s="5" t="s">
-        <v>126</v>
+        <v>83</v>
       </c>
       <c r="AW55" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX55" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY55" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ55" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA55" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB55" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC55" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD55" s="5" t="str">
         <f>INT(LEFT(AU55,1))</f>
@@ -18214,31 +18199,31 @@
         <v>53</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D56" s="5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>86</v>
+        <v>162</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>86</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="K56" s="5" t="str">
         <f>INT(LEFT(E56,1))</f>
@@ -18349,31 +18334,31 @@
         <f>FLOOR(AS56/8,1,1)&amp;"."&amp;FLOOR(MOD(AS56,8),1,1)&amp;"."&amp;(MOD(AS56,8)-FLOOR(MOD(AS56,8),1,1))*60</f>
       </c>
       <c r="AU56" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV56" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW56" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX56" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY56" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ56" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA56" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB56" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC56" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD56" s="5" t="str">
         <f>INT(LEFT(AU56,1))</f>
@@ -18537,7 +18522,7 @@
         <v>54</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>77</v>
@@ -18546,22 +18531,22 @@
         <v>0</v>
       </c>
       <c r="E57" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H57" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="F57" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="G57" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="H57" s="5" t="s">
-        <v>90</v>
-      </c>
       <c r="I57" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K57" s="5" t="str">
         <f>INT(LEFT(E57,1))</f>
@@ -18672,31 +18657,31 @@
         <f>FLOOR(AS57/8,1,1)&amp;"."&amp;FLOOR(MOD(AS57,8),1,1)&amp;"."&amp;(MOD(AS57,8)-FLOOR(MOD(AS57,8),1,1))*60</f>
       </c>
       <c r="AU57" s="5" t="s">
-        <v>87</v>
+        <v>164</v>
       </c>
       <c r="AV57" s="5" t="s">
-        <v>169</v>
+        <v>83</v>
       </c>
       <c r="AW57" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX57" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY57" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ57" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA57" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB57" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC57" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD57" s="5" t="str">
         <f>INT(LEFT(AU57,1))</f>
@@ -18860,7 +18845,7 @@
         <v>55</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>77</v>
@@ -18869,22 +18854,22 @@
         <v>0</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="K58" s="5" t="str">
         <f>INT(LEFT(E58,1))</f>
@@ -18995,31 +18980,31 @@
         <f>FLOOR(AS58/8,1,1)&amp;"."&amp;FLOOR(MOD(AS58,8),1,1)&amp;"."&amp;(MOD(AS58,8)-FLOOR(MOD(AS58,8),1,1))*60</f>
       </c>
       <c r="AU58" s="5" t="s">
-        <v>162</v>
+        <v>83</v>
       </c>
       <c r="AV58" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW58" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX58" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY58" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ58" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA58" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB58" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC58" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD58" s="5" t="str">
         <f>INT(LEFT(AU58,1))</f>
@@ -19183,7 +19168,7 @@
         <v>56</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>77</v>
@@ -19192,22 +19177,22 @@
         <v>0</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K59" s="5" t="str">
         <f>INT(LEFT(E59,1))</f>
@@ -19318,31 +19303,31 @@
         <f>FLOOR(AS59/8,1,1)&amp;"."&amp;FLOOR(MOD(AS59,8),1,1)&amp;"."&amp;(MOD(AS59,8)-FLOOR(MOD(AS59,8),1,1))*60</f>
       </c>
       <c r="AU59" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV59" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW59" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX59" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY59" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ59" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA59" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB59" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC59" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD59" s="5" t="str">
         <f>INT(LEFT(AU59,1))</f>
@@ -19506,7 +19491,7 @@
         <v>57</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>77</v>
@@ -19515,22 +19500,22 @@
         <v>0</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>128</v>
+        <v>81</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K60" s="5" t="str">
         <f>INT(LEFT(E60,1))</f>
@@ -19641,31 +19626,31 @@
         <f>FLOOR(AS60/8,1,1)&amp;"."&amp;FLOOR(MOD(AS60,8),1,1)&amp;"."&amp;(MOD(AS60,8)-FLOOR(MOD(AS60,8),1,1))*60</f>
       </c>
       <c r="AU60" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV60" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW60" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX60" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY60" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ60" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA60" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB60" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC60" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD60" s="5" t="str">
         <f>INT(LEFT(AU60,1))</f>
@@ -19829,7 +19814,7 @@
         <v>58</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>77</v>
@@ -19838,22 +19823,22 @@
         <v>0</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="K61" s="5" t="str">
         <f>INT(LEFT(E61,1))</f>
@@ -19964,31 +19949,31 @@
         <f>FLOOR(AS61/8,1,1)&amp;"."&amp;FLOOR(MOD(AS61,8),1,1)&amp;"."&amp;(MOD(AS61,8)-FLOOR(MOD(AS61,8),1,1))*60</f>
       </c>
       <c r="AU61" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AV61" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AW61" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AX61" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AY61" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AZ61" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BA61" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BB61" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="BC61" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="BD61" s="5" t="str">
         <f>INT(LEFT(AU61,1))</f>

</xml_diff>

<commit_message>
added colors to rows
</commit_message>
<xml_diff>
--- a/exceltocsv/public/reports/DTRSUMMARY.xlsx
+++ b/exceltocsv/public/reports/DTRSUMMARY.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="174">
   <si>
     <t>iRipple, Inc.</t>
   </si>
@@ -251,10 +251,10 @@
     <t>0.0.0</t>
   </si>
   <si>
-    <t>7.5.0</t>
+    <t>1.0.0</t>
   </si>
   <si>
-    <t>1.0.0</t>
+    <t>7.5.0</t>
   </si>
   <si>
     <t>1.0.00</t>
@@ -281,10 +281,16 @@
     <t>Bacani,Eddie Marie</t>
   </si>
   <si>
+    <t>9.0.0</t>
+  </si>
+  <si>
     <t>Bagaindoc,Kjell</t>
   </si>
   <si>
     <t>0.1.15</t>
+  </si>
+  <si>
+    <t>2.0.0</t>
   </si>
   <si>
     <t>Balingit,Barbara</t>
@@ -308,6 +314,9 @@
     <t>0.1.30</t>
   </si>
   <si>
+    <t>1.5.0</t>
+  </si>
+  <si>
     <t>Bonita,Reynaldo Jr</t>
   </si>
   <si>
@@ -326,16 +335,13 @@
     <t>Buena,Ian Christopher</t>
   </si>
   <si>
-    <t>2.5.0</t>
-  </si>
-  <si>
     <t>Buenafe,Rajiv</t>
   </si>
   <si>
     <t>Cataluna,Christian Gilbert</t>
   </si>
   <si>
-    <t>1.5.0</t>
+    <t>2.5.0</t>
   </si>
   <si>
     <t>CaÃ±ete,Carol Ann</t>
@@ -356,6 +362,9 @@
     <t>0.1.45</t>
   </si>
   <si>
+    <t>6.0.0</t>
+  </si>
+  <si>
     <t>Cortez,Jomar</t>
   </si>
   <si>
@@ -371,16 +380,16 @@
     <t>Delos Reyes,Jeffrey</t>
   </si>
   <si>
-    <t>Dino,Arvin</t>
+    <t>8.0.0</t>
   </si>
   <si>
-    <t>3.0.0</t>
+    <t>Dino,Arvin</t>
   </si>
   <si>
     <t>Dy,Hubert</t>
   </si>
   <si>
-    <t>2.0.0</t>
+    <t>3.0.0</t>
   </si>
   <si>
     <t>Egamino,Ellen</t>
@@ -413,10 +422,16 @@
     <t>Javier,Victor </t>
   </si>
   <si>
+    <t>7.0.0</t>
+  </si>
+  <si>
     <t>Joson,Alfonso Miguel</t>
   </si>
   <si>
     <t>Keng,Julie</t>
+  </si>
+  <si>
+    <t>8.5.0</t>
   </si>
   <si>
     <t>Laroza,Baltazar</t>
@@ -1418,16 +1433,16 @@
         <v>79</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="K4" s="5" t="str">
         <f>INT(LEFT(E4,1))</f>
@@ -1535,7 +1550,7 @@
         <f>AR4/60</f>
       </c>
       <c r="AT4" s="5" t="str">
-        <f>FLOOR(AS4/8,1,1)&amp;"."&amp;FLOOR(MOD(AS4,8),1,1)&amp;"."&amp;(MOD(AS4,8)-FLOOR(MOD(AS4,8),1,1))*60</f>
+        <f>FLOOR(AS4/8,1)&amp;"."&amp;FLOOR(MOD(AS4,8),1)&amp;"."&amp;(MOD(AS4,8)-FLOOR(MOD(AS4,8),1))*60</f>
       </c>
       <c r="AU4" s="5" t="s">
         <v>82</v>
@@ -1718,7 +1733,7 @@
         <v>0</v>
       </c>
       <c r="DC4" s="5" t="str">
-        <f>FLOOR(DA4/8,1,1)&amp;"."&amp;FLOOR(MOD(DA4,8),1,1)&amp;"."&amp;(MOD(DA4,8)-FLOOR(MOD(DA4,8),1,1))*60</f>
+        <f>FLOOR(DA4/8,1)&amp;"."&amp;FLOOR(MOD(DA4,8),1)&amp;"."&amp;(MOD(DA4,8)-FLOOR(MOD(DA4,8),1))*60</f>
       </c>
     </row>
     <row r="5">
@@ -1858,7 +1873,7 @@
         <f>AR5/60</f>
       </c>
       <c r="AT5" s="5" t="str">
-        <f>FLOOR(AS5/8,1,1)&amp;"."&amp;FLOOR(MOD(AS5,8),1,1)&amp;"."&amp;(MOD(AS5,8)-FLOOR(MOD(AS5,8),1,1))*60</f>
+        <f>FLOOR(AS5/8,1)&amp;"."&amp;FLOOR(MOD(AS5,8),1)&amp;"."&amp;(MOD(AS5,8)-FLOOR(MOD(AS5,8),1))*60</f>
       </c>
       <c r="AU5" s="5" t="s">
         <v>83</v>
@@ -2041,7 +2056,7 @@
         <v>0</v>
       </c>
       <c r="DC5" s="5" t="str">
-        <f>FLOOR(DA5/8,1,1)&amp;"."&amp;FLOOR(MOD(DA5,8),1,1)&amp;"."&amp;(MOD(DA5,8)-FLOOR(MOD(DA5,8),1,1))*60</f>
+        <f>FLOOR(DA5/8,1)&amp;"."&amp;FLOOR(MOD(DA5,8),1)&amp;"."&amp;(MOD(DA5,8)-FLOOR(MOD(DA5,8),1))*60</f>
       </c>
     </row>
     <row r="6">
@@ -2067,13 +2082,13 @@
         <v>79</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K6" s="5" t="str">
         <f>INT(LEFT(E6,1))</f>
@@ -2181,7 +2196,7 @@
         <f>AR6/60</f>
       </c>
       <c r="AT6" s="5" t="str">
-        <f>FLOOR(AS6/8,1,1)&amp;"."&amp;FLOOR(MOD(AS6,8),1,1)&amp;"."&amp;(MOD(AS6,8)-FLOOR(MOD(AS6,8),1,1))*60</f>
+        <f>FLOOR(AS6/8,1)&amp;"."&amp;FLOOR(MOD(AS6,8),1)&amp;"."&amp;(MOD(AS6,8)-FLOOR(MOD(AS6,8),1))*60</f>
       </c>
       <c r="AU6" s="5" t="s">
         <v>88</v>
@@ -2364,7 +2379,7 @@
         <v>0</v>
       </c>
       <c r="DC6" s="5" t="str">
-        <f>FLOOR(DA6/8,1,1)&amp;"."&amp;FLOOR(MOD(DA6,8),1,1)&amp;"."&amp;(MOD(DA6,8)-FLOOR(MOD(DA6,8),1,1))*60</f>
+        <f>FLOOR(DA6/8,1)&amp;"."&amp;FLOOR(MOD(DA6,8),1)&amp;"."&amp;(MOD(DA6,8)-FLOOR(MOD(DA6,8),1))*60</f>
       </c>
     </row>
     <row r="7">
@@ -2387,16 +2402,16 @@
         <v>79</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K7" s="5" t="str">
         <f>INT(LEFT(E7,1))</f>
@@ -2504,7 +2519,7 @@
         <f>AR7/60</f>
       </c>
       <c r="AT7" s="5" t="str">
-        <f>FLOOR(AS7/8,1,1)&amp;"."&amp;FLOOR(MOD(AS7,8),1,1)&amp;"."&amp;(MOD(AS7,8)-FLOOR(MOD(AS7,8),1,1))*60</f>
+        <f>FLOOR(AS7/8,1)&amp;"."&amp;FLOOR(MOD(AS7,8),1)&amp;"."&amp;(MOD(AS7,8)-FLOOR(MOD(AS7,8),1))*60</f>
       </c>
       <c r="AU7" s="5" t="s">
         <v>83</v>
@@ -2687,7 +2702,7 @@
         <v>0</v>
       </c>
       <c r="DC7" s="5" t="str">
-        <f>FLOOR(DA7/8,1,1)&amp;"."&amp;FLOOR(MOD(DA7,8),1,1)&amp;"."&amp;(MOD(DA7,8)-FLOOR(MOD(DA7,8),1,1))*60</f>
+        <f>FLOOR(DA7/8,1)&amp;"."&amp;FLOOR(MOD(DA7,8),1)&amp;"."&amp;(MOD(DA7,8)-FLOOR(MOD(DA7,8),1))*60</f>
       </c>
     </row>
     <row r="8">
@@ -2695,7 +2710,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>77</v>
@@ -2707,19 +2722,19 @@
         <v>79</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G8" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>80</v>
-      </c>
       <c r="I8" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K8" s="5" t="str">
         <f>INT(LEFT(E8,1))</f>
@@ -2827,7 +2842,7 @@
         <f>AR8/60</f>
       </c>
       <c r="AT8" s="5" t="str">
-        <f>FLOOR(AS8/8,1,1)&amp;"."&amp;FLOOR(MOD(AS8,8),1,1)&amp;"."&amp;(MOD(AS8,8)-FLOOR(MOD(AS8,8),1,1))*60</f>
+        <f>FLOOR(AS8/8,1)&amp;"."&amp;FLOOR(MOD(AS8,8),1)&amp;"."&amp;(MOD(AS8,8)-FLOOR(MOD(AS8,8),1))*60</f>
       </c>
       <c r="AU8" s="5" t="s">
         <v>83</v>
@@ -3010,7 +3025,7 @@
         <v>0</v>
       </c>
       <c r="DC8" s="5" t="str">
-        <f>FLOOR(DA8/8,1,1)&amp;"."&amp;FLOOR(MOD(DA8,8),1,1)&amp;"."&amp;(MOD(DA8,8)-FLOOR(MOD(DA8,8),1,1))*60</f>
+        <f>FLOOR(DA8/8,1)&amp;"."&amp;FLOOR(MOD(DA8,8),1)&amp;"."&amp;(MOD(DA8,8)-FLOOR(MOD(DA8,8),1))*60</f>
       </c>
     </row>
     <row r="9">
@@ -3018,7 +3033,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>77</v>
@@ -3033,16 +3048,16 @@
         <v>79</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K9" s="5" t="str">
         <f>INT(LEFT(E9,1))</f>
@@ -3150,7 +3165,7 @@
         <f>AR9/60</f>
       </c>
       <c r="AT9" s="5" t="str">
-        <f>FLOOR(AS9/8,1,1)&amp;"."&amp;FLOOR(MOD(AS9,8),1,1)&amp;"."&amp;(MOD(AS9,8)-FLOOR(MOD(AS9,8),1,1))*60</f>
+        <f>FLOOR(AS9/8,1)&amp;"."&amp;FLOOR(MOD(AS9,8),1)&amp;"."&amp;(MOD(AS9,8)-FLOOR(MOD(AS9,8),1))*60</f>
       </c>
       <c r="AU9" s="5" t="s">
         <v>83</v>
@@ -3333,7 +3348,7 @@
         <v>0</v>
       </c>
       <c r="DC9" s="5" t="str">
-        <f>FLOOR(DA9/8,1,1)&amp;"."&amp;FLOOR(MOD(DA9,8),1,1)&amp;"."&amp;(MOD(DA9,8)-FLOOR(MOD(DA9,8),1,1))*60</f>
+        <f>FLOOR(DA9/8,1)&amp;"."&amp;FLOOR(MOD(DA9,8),1)&amp;"."&amp;(MOD(DA9,8)-FLOOR(MOD(DA9,8),1))*60</f>
       </c>
     </row>
     <row r="10">
@@ -3341,7 +3356,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>77</v>
@@ -3356,16 +3371,16 @@
         <v>79</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K10" s="5" t="str">
         <f>INT(LEFT(E10,1))</f>
@@ -3473,7 +3488,7 @@
         <f>AR10/60</f>
       </c>
       <c r="AT10" s="5" t="str">
-        <f>FLOOR(AS10/8,1,1)&amp;"."&amp;FLOOR(MOD(AS10,8),1,1)&amp;"."&amp;(MOD(AS10,8)-FLOOR(MOD(AS10,8),1,1))*60</f>
+        <f>FLOOR(AS10/8,1)&amp;"."&amp;FLOOR(MOD(AS10,8),1)&amp;"."&amp;(MOD(AS10,8)-FLOOR(MOD(AS10,8),1))*60</f>
       </c>
       <c r="AU10" s="5" t="s">
         <v>83</v>
@@ -3656,7 +3671,7 @@
         <v>0</v>
       </c>
       <c r="DC10" s="5" t="str">
-        <f>FLOOR(DA10/8,1,1)&amp;"."&amp;FLOOR(MOD(DA10,8),1,1)&amp;"."&amp;(MOD(DA10,8)-FLOOR(MOD(DA10,8),1,1))*60</f>
+        <f>FLOOR(DA10/8,1)&amp;"."&amp;FLOOR(MOD(DA10,8),1)&amp;"."&amp;(MOD(DA10,8)-FLOOR(MOD(DA10,8),1))*60</f>
       </c>
     </row>
     <row r="11">
@@ -3664,7 +3679,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>77</v>
@@ -3679,16 +3694,16 @@
         <v>79</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K11" s="5" t="str">
         <f>INT(LEFT(E11,1))</f>
@@ -3796,7 +3811,7 @@
         <f>AR11/60</f>
       </c>
       <c r="AT11" s="5" t="str">
-        <f>FLOOR(AS11/8,1,1)&amp;"."&amp;FLOOR(MOD(AS11,8),1,1)&amp;"."&amp;(MOD(AS11,8)-FLOOR(MOD(AS11,8),1,1))*60</f>
+        <f>FLOOR(AS11/8,1)&amp;"."&amp;FLOOR(MOD(AS11,8),1)&amp;"."&amp;(MOD(AS11,8)-FLOOR(MOD(AS11,8),1))*60</f>
       </c>
       <c r="AU11" s="5" t="s">
         <v>83</v>
@@ -3979,7 +3994,7 @@
         <v>0</v>
       </c>
       <c r="DC11" s="5" t="str">
-        <f>FLOOR(DA11/8,1,1)&amp;"."&amp;FLOOR(MOD(DA11,8),1,1)&amp;"."&amp;(MOD(DA11,8)-FLOOR(MOD(DA11,8),1,1))*60</f>
+        <f>FLOOR(DA11/8,1)&amp;"."&amp;FLOOR(MOD(DA11,8),1)&amp;"."&amp;(MOD(DA11,8)-FLOOR(MOD(DA11,8),1))*60</f>
       </c>
     </row>
     <row r="12">
@@ -3987,7 +4002,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>77</v>
@@ -3996,22 +4011,22 @@
         <v>6</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K12" s="5" t="str">
         <f>INT(LEFT(E12,1))</f>
@@ -4119,7 +4134,7 @@
         <f>AR12/60</f>
       </c>
       <c r="AT12" s="5" t="str">
-        <f>FLOOR(AS12/8,1,1)&amp;"."&amp;FLOOR(MOD(AS12,8),1,1)&amp;"."&amp;(MOD(AS12,8)-FLOOR(MOD(AS12,8),1,1))*60</f>
+        <f>FLOOR(AS12/8,1)&amp;"."&amp;FLOOR(MOD(AS12,8),1)&amp;"."&amp;(MOD(AS12,8)-FLOOR(MOD(AS12,8),1))*60</f>
       </c>
       <c r="AU12" s="5" t="s">
         <v>83</v>
@@ -4302,7 +4317,7 @@
         <v>0</v>
       </c>
       <c r="DC12" s="5" t="str">
-        <f>FLOOR(DA12/8,1,1)&amp;"."&amp;FLOOR(MOD(DA12,8),1,1)&amp;"."&amp;(MOD(DA12,8)-FLOOR(MOD(DA12,8),1,1))*60</f>
+        <f>FLOOR(DA12/8,1)&amp;"."&amp;FLOOR(MOD(DA12,8),1)&amp;"."&amp;(MOD(DA12,8)-FLOOR(MOD(DA12,8),1))*60</f>
       </c>
     </row>
     <row r="13">
@@ -4310,7 +4325,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>77</v>
@@ -4319,22 +4334,22 @@
         <v>6</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K13" s="5" t="str">
         <f>INT(LEFT(E13,1))</f>
@@ -4442,7 +4457,7 @@
         <f>AR13/60</f>
       </c>
       <c r="AT13" s="5" t="str">
-        <f>FLOOR(AS13/8,1,1)&amp;"."&amp;FLOOR(MOD(AS13,8),1,1)&amp;"."&amp;(MOD(AS13,8)-FLOOR(MOD(AS13,8),1,1))*60</f>
+        <f>FLOOR(AS13/8,1)&amp;"."&amp;FLOOR(MOD(AS13,8),1)&amp;"."&amp;(MOD(AS13,8)-FLOOR(MOD(AS13,8),1))*60</f>
       </c>
       <c r="AU13" s="5" t="s">
         <v>83</v>
@@ -4625,7 +4640,7 @@
         <v>0</v>
       </c>
       <c r="DC13" s="5" t="str">
-        <f>FLOOR(DA13/8,1,1)&amp;"."&amp;FLOOR(MOD(DA13,8),1,1)&amp;"."&amp;(MOD(DA13,8)-FLOOR(MOD(DA13,8),1,1))*60</f>
+        <f>FLOOR(DA13/8,1)&amp;"."&amp;FLOOR(MOD(DA13,8),1)&amp;"."&amp;(MOD(DA13,8)-FLOOR(MOD(DA13,8),1))*60</f>
       </c>
     </row>
     <row r="14">
@@ -4633,7 +4648,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>77</v>
@@ -4648,16 +4663,16 @@
         <v>79</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K14" s="5" t="str">
         <f>INT(LEFT(E14,1))</f>
@@ -4765,7 +4780,7 @@
         <f>AR14/60</f>
       </c>
       <c r="AT14" s="5" t="str">
-        <f>FLOOR(AS14/8,1,1)&amp;"."&amp;FLOOR(MOD(AS14,8),1,1)&amp;"."&amp;(MOD(AS14,8)-FLOOR(MOD(AS14,8),1,1))*60</f>
+        <f>FLOOR(AS14/8,1)&amp;"."&amp;FLOOR(MOD(AS14,8),1)&amp;"."&amp;(MOD(AS14,8)-FLOOR(MOD(AS14,8),1))*60</f>
       </c>
       <c r="AU14" s="5" t="s">
         <v>83</v>
@@ -4948,7 +4963,7 @@
         <v>0</v>
       </c>
       <c r="DC14" s="5" t="str">
-        <f>FLOOR(DA14/8,1,1)&amp;"."&amp;FLOOR(MOD(DA14,8),1,1)&amp;"."&amp;(MOD(DA14,8)-FLOOR(MOD(DA14,8),1,1))*60</f>
+        <f>FLOOR(DA14/8,1)&amp;"."&amp;FLOOR(MOD(DA14,8),1)&amp;"."&amp;(MOD(DA14,8)-FLOOR(MOD(DA14,8),1))*60</f>
       </c>
     </row>
     <row r="15">
@@ -4956,7 +4971,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>77</v>
@@ -4974,13 +4989,13 @@
         <v>79</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K15" s="5" t="str">
         <f>INT(LEFT(E15,1))</f>
@@ -5088,7 +5103,7 @@
         <f>AR15/60</f>
       </c>
       <c r="AT15" s="5" t="str">
-        <f>FLOOR(AS15/8,1,1)&amp;"."&amp;FLOOR(MOD(AS15,8),1,1)&amp;"."&amp;(MOD(AS15,8)-FLOOR(MOD(AS15,8),1,1))*60</f>
+        <f>FLOOR(AS15/8,1)&amp;"."&amp;FLOOR(MOD(AS15,8),1)&amp;"."&amp;(MOD(AS15,8)-FLOOR(MOD(AS15,8),1))*60</f>
       </c>
       <c r="AU15" s="5" t="s">
         <v>83</v>
@@ -5271,7 +5286,7 @@
         <v>0</v>
       </c>
       <c r="DC15" s="5" t="str">
-        <f>FLOOR(DA15/8,1,1)&amp;"."&amp;FLOOR(MOD(DA15,8),1,1)&amp;"."&amp;(MOD(DA15,8)-FLOOR(MOD(DA15,8),1,1))*60</f>
+        <f>FLOOR(DA15/8,1)&amp;"."&amp;FLOOR(MOD(DA15,8),1)&amp;"."&amp;(MOD(DA15,8)-FLOOR(MOD(DA15,8),1))*60</f>
       </c>
     </row>
     <row r="16">
@@ -5279,7 +5294,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>77</v>
@@ -5288,22 +5303,22 @@
         <v>3</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>78</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K16" s="5" t="str">
         <f>INT(LEFT(E16,1))</f>
@@ -5411,7 +5426,7 @@
         <f>AR16/60</f>
       </c>
       <c r="AT16" s="5" t="str">
-        <f>FLOOR(AS16/8,1,1)&amp;"."&amp;FLOOR(MOD(AS16,8),1,1)&amp;"."&amp;(MOD(AS16,8)-FLOOR(MOD(AS16,8),1,1))*60</f>
+        <f>FLOOR(AS16/8,1)&amp;"."&amp;FLOOR(MOD(AS16,8),1)&amp;"."&amp;(MOD(AS16,8)-FLOOR(MOD(AS16,8),1))*60</f>
       </c>
       <c r="AU16" s="5" t="s">
         <v>83</v>
@@ -5594,7 +5609,7 @@
         <v>0</v>
       </c>
       <c r="DC16" s="5" t="str">
-        <f>FLOOR(DA16/8,1,1)&amp;"."&amp;FLOOR(MOD(DA16,8),1,1)&amp;"."&amp;(MOD(DA16,8)-FLOOR(MOD(DA16,8),1,1))*60</f>
+        <f>FLOOR(DA16/8,1)&amp;"."&amp;FLOOR(MOD(DA16,8),1)&amp;"."&amp;(MOD(DA16,8)-FLOOR(MOD(DA16,8),1))*60</f>
       </c>
     </row>
     <row r="17">
@@ -5602,7 +5617,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>77</v>
@@ -5620,13 +5635,13 @@
         <v>79</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K17" s="5" t="str">
         <f>INT(LEFT(E17,1))</f>
@@ -5734,7 +5749,7 @@
         <f>AR17/60</f>
       </c>
       <c r="AT17" s="5" t="str">
-        <f>FLOOR(AS17/8,1,1)&amp;"."&amp;FLOOR(MOD(AS17,8),1,1)&amp;"."&amp;(MOD(AS17,8)-FLOOR(MOD(AS17,8),1,1))*60</f>
+        <f>FLOOR(AS17/8,1)&amp;"."&amp;FLOOR(MOD(AS17,8),1)&amp;"."&amp;(MOD(AS17,8)-FLOOR(MOD(AS17,8),1))*60</f>
       </c>
       <c r="AU17" s="5" t="s">
         <v>83</v>
@@ -5917,7 +5932,7 @@
         <v>0</v>
       </c>
       <c r="DC17" s="5" t="str">
-        <f>FLOOR(DA17/8,1,1)&amp;"."&amp;FLOOR(MOD(DA17,8),1,1)&amp;"."&amp;(MOD(DA17,8)-FLOOR(MOD(DA17,8),1,1))*60</f>
+        <f>FLOOR(DA17/8,1)&amp;"."&amp;FLOOR(MOD(DA17,8),1)&amp;"."&amp;(MOD(DA17,8)-FLOOR(MOD(DA17,8),1))*60</f>
       </c>
     </row>
     <row r="18">
@@ -5925,7 +5940,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>77</v>
@@ -5940,16 +5955,16 @@
         <v>79</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="K18" s="5" t="str">
         <f>INT(LEFT(E18,1))</f>
@@ -6057,7 +6072,7 @@
         <f>AR18/60</f>
       </c>
       <c r="AT18" s="5" t="str">
-        <f>FLOOR(AS18/8,1,1)&amp;"."&amp;FLOOR(MOD(AS18,8),1,1)&amp;"."&amp;(MOD(AS18,8)-FLOOR(MOD(AS18,8),1,1))*60</f>
+        <f>FLOOR(AS18/8,1)&amp;"."&amp;FLOOR(MOD(AS18,8),1)&amp;"."&amp;(MOD(AS18,8)-FLOOR(MOD(AS18,8),1))*60</f>
       </c>
       <c r="AU18" s="5" t="s">
         <v>83</v>
@@ -6240,7 +6255,7 @@
         <v>0</v>
       </c>
       <c r="DC18" s="5" t="str">
-        <f>FLOOR(DA18/8,1,1)&amp;"."&amp;FLOOR(MOD(DA18,8),1,1)&amp;"."&amp;(MOD(DA18,8)-FLOOR(MOD(DA18,8),1,1))*60</f>
+        <f>FLOOR(DA18/8,1)&amp;"."&amp;FLOOR(MOD(DA18,8),1)&amp;"."&amp;(MOD(DA18,8)-FLOOR(MOD(DA18,8),1))*60</f>
       </c>
     </row>
     <row r="19">
@@ -6248,7 +6263,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>77</v>
@@ -6257,22 +6272,22 @@
         <v>4</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="I19" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J19" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="K19" s="5" t="str">
         <f>INT(LEFT(E19,1))</f>
@@ -6380,7 +6395,7 @@
         <f>AR19/60</f>
       </c>
       <c r="AT19" s="5" t="str">
-        <f>FLOOR(AS19/8,1,1)&amp;"."&amp;FLOOR(MOD(AS19,8),1,1)&amp;"."&amp;(MOD(AS19,8)-FLOOR(MOD(AS19,8),1,1))*60</f>
+        <f>FLOOR(AS19/8,1)&amp;"."&amp;FLOOR(MOD(AS19,8),1)&amp;"."&amp;(MOD(AS19,8)-FLOOR(MOD(AS19,8),1))*60</f>
       </c>
       <c r="AU19" s="5" t="s">
         <v>83</v>
@@ -6563,7 +6578,7 @@
         <v>0</v>
       </c>
       <c r="DC19" s="5" t="str">
-        <f>FLOOR(DA19/8,1,1)&amp;"."&amp;FLOOR(MOD(DA19,8),1,1)&amp;"."&amp;(MOD(DA19,8)-FLOOR(MOD(DA19,8),1,1))*60</f>
+        <f>FLOOR(DA19/8,1)&amp;"."&amp;FLOOR(MOD(DA19,8),1)&amp;"."&amp;(MOD(DA19,8)-FLOOR(MOD(DA19,8),1))*60</f>
       </c>
     </row>
     <row r="20">
@@ -6571,7 +6586,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>77</v>
@@ -6586,16 +6601,16 @@
         <v>79</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K20" s="5" t="str">
         <f>INT(LEFT(E20,1))</f>
@@ -6703,7 +6718,7 @@
         <f>AR20/60</f>
       </c>
       <c r="AT20" s="5" t="str">
-        <f>FLOOR(AS20/8,1,1)&amp;"."&amp;FLOOR(MOD(AS20,8),1,1)&amp;"."&amp;(MOD(AS20,8)-FLOOR(MOD(AS20,8),1,1))*60</f>
+        <f>FLOOR(AS20/8,1)&amp;"."&amp;FLOOR(MOD(AS20,8),1)&amp;"."&amp;(MOD(AS20,8)-FLOOR(MOD(AS20,8),1))*60</f>
       </c>
       <c r="AU20" s="5" t="s">
         <v>83</v>
@@ -6886,7 +6901,7 @@
         <v>0</v>
       </c>
       <c r="DC20" s="5" t="str">
-        <f>FLOOR(DA20/8,1,1)&amp;"."&amp;FLOOR(MOD(DA20,8),1,1)&amp;"."&amp;(MOD(DA20,8)-FLOOR(MOD(DA20,8),1,1))*60</f>
+        <f>FLOOR(DA20/8,1)&amp;"."&amp;FLOOR(MOD(DA20,8),1)&amp;"."&amp;(MOD(DA20,8)-FLOOR(MOD(DA20,8),1))*60</f>
       </c>
     </row>
     <row r="21">
@@ -6894,7 +6909,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>77</v>
@@ -6906,19 +6921,19 @@
         <v>79</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K21" s="5" t="str">
         <f>INT(LEFT(E21,1))</f>
@@ -7026,7 +7041,7 @@
         <f>AR21/60</f>
       </c>
       <c r="AT21" s="5" t="str">
-        <f>FLOOR(AS21/8,1,1)&amp;"."&amp;FLOOR(MOD(AS21,8),1,1)&amp;"."&amp;(MOD(AS21,8)-FLOOR(MOD(AS21,8),1,1))*60</f>
+        <f>FLOOR(AS21/8,1)&amp;"."&amp;FLOOR(MOD(AS21,8),1)&amp;"."&amp;(MOD(AS21,8)-FLOOR(MOD(AS21,8),1))*60</f>
       </c>
       <c r="AU21" s="5" t="s">
         <v>83</v>
@@ -7209,7 +7224,7 @@
         <v>0</v>
       </c>
       <c r="DC21" s="5" t="str">
-        <f>FLOOR(DA21/8,1,1)&amp;"."&amp;FLOOR(MOD(DA21,8),1,1)&amp;"."&amp;(MOD(DA21,8)-FLOOR(MOD(DA21,8),1,1))*60</f>
+        <f>FLOOR(DA21/8,1)&amp;"."&amp;FLOOR(MOD(DA21,8),1)&amp;"."&amp;(MOD(DA21,8)-FLOOR(MOD(DA21,8),1))*60</f>
       </c>
     </row>
     <row r="22">
@@ -7217,7 +7232,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>77</v>
@@ -7232,16 +7247,16 @@
         <v>79</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="K22" s="5" t="str">
         <f>INT(LEFT(E22,1))</f>
@@ -7349,7 +7364,7 @@
         <f>AR22/60</f>
       </c>
       <c r="AT22" s="5" t="str">
-        <f>FLOOR(AS22/8,1,1)&amp;"."&amp;FLOOR(MOD(AS22,8),1,1)&amp;"."&amp;(MOD(AS22,8)-FLOOR(MOD(AS22,8),1,1))*60</f>
+        <f>FLOOR(AS22/8,1)&amp;"."&amp;FLOOR(MOD(AS22,8),1)&amp;"."&amp;(MOD(AS22,8)-FLOOR(MOD(AS22,8),1))*60</f>
       </c>
       <c r="AU22" s="5" t="s">
         <v>83</v>
@@ -7532,7 +7547,7 @@
         <v>0</v>
       </c>
       <c r="DC22" s="5" t="str">
-        <f>FLOOR(DA22/8,1,1)&amp;"."&amp;FLOOR(MOD(DA22,8),1,1)&amp;"."&amp;(MOD(DA22,8)-FLOOR(MOD(DA22,8),1,1))*60</f>
+        <f>FLOOR(DA22/8,1)&amp;"."&amp;FLOOR(MOD(DA22,8),1)&amp;"."&amp;(MOD(DA22,8)-FLOOR(MOD(DA22,8),1))*60</f>
       </c>
     </row>
     <row r="23">
@@ -7540,7 +7555,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>77</v>
@@ -7555,16 +7570,16 @@
         <v>79</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>79</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="K23" s="5" t="str">
         <f>INT(LEFT(E23,1))</f>
@@ -7672,7 +7687,7 @@
         <f>AR23/60</f>
       </c>
       <c r="AT23" s="5" t="str">
-        <f>FLOOR(AS23/8,1,1)&amp;"."&amp;FLOOR(MOD(AS23,8),1,1)&amp;"."&amp;(MOD(AS23,8)-FLOOR(MOD(AS23,8),1,1))*60</f>
+        <f>FLOOR(AS23/8,1)&amp;"."&amp;FLOOR(MOD(AS23,8),1)&amp;"."&amp;(MOD(AS23,8)-FLOOR(MOD(AS23,8),1))*60</f>
       </c>
       <c r="AU23" s="5" t="s">
         <v>83</v>
@@ -7855,7 +7870,7 @@
         <v>0</v>
       </c>
       <c r="DC23" s="5" t="str">
-        <f>FLOOR(DA23/8,1,1)&amp;"."&amp;FLOOR(MOD(DA23,8),1,1)&amp;"."&amp;(MOD(DA23,8)-FLOOR(MOD(DA23,8),1,1))*60</f>
+        <f>FLOOR(DA23/8,1)&amp;"."&amp;FLOOR(MOD(DA23,8),1)&amp;"."&amp;(MOD(DA23,8)-FLOOR(MOD(DA23,8),1))*60</f>
       </c>
     </row>
     <row r="24">
@@ -7863,7 +7878,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>77</v>
@@ -7878,16 +7893,16 @@
         <v>79</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>79</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="K24" s="5" t="str">
         <f>INT(LEFT(E24,1))</f>
@@ -7995,7 +8010,7 @@
         <f>AR24/60</f>
       </c>
       <c r="AT24" s="5" t="str">
-        <f>FLOOR(AS24/8,1,1)&amp;"."&amp;FLOOR(MOD(AS24,8),1,1)&amp;"."&amp;(MOD(AS24,8)-FLOOR(MOD(AS24,8),1,1))*60</f>
+        <f>FLOOR(AS24/8,1)&amp;"."&amp;FLOOR(MOD(AS24,8),1)&amp;"."&amp;(MOD(AS24,8)-FLOOR(MOD(AS24,8),1))*60</f>
       </c>
       <c r="AU24" s="5" t="s">
         <v>83</v>
@@ -8178,7 +8193,7 @@
         <v>0</v>
       </c>
       <c r="DC24" s="5" t="str">
-        <f>FLOOR(DA24/8,1,1)&amp;"."&amp;FLOOR(MOD(DA24,8),1,1)&amp;"."&amp;(MOD(DA24,8)-FLOOR(MOD(DA24,8),1,1))*60</f>
+        <f>FLOOR(DA24/8,1)&amp;"."&amp;FLOOR(MOD(DA24,8),1)&amp;"."&amp;(MOD(DA24,8)-FLOOR(MOD(DA24,8),1))*60</f>
       </c>
     </row>
     <row r="25">
@@ -8186,7 +8201,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>77</v>
@@ -8201,16 +8216,16 @@
         <v>79</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>79</v>
+        <v>123</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K25" s="5" t="str">
         <f>INT(LEFT(E25,1))</f>
@@ -8318,7 +8333,7 @@
         <f>AR25/60</f>
       </c>
       <c r="AT25" s="5" t="str">
-        <f>FLOOR(AS25/8,1,1)&amp;"."&amp;FLOOR(MOD(AS25,8),1,1)&amp;"."&amp;(MOD(AS25,8)-FLOOR(MOD(AS25,8),1,1))*60</f>
+        <f>FLOOR(AS25/8,1)&amp;"."&amp;FLOOR(MOD(AS25,8),1)&amp;"."&amp;(MOD(AS25,8)-FLOOR(MOD(AS25,8),1))*60</f>
       </c>
       <c r="AU25" s="5" t="s">
         <v>83</v>
@@ -8501,7 +8516,7 @@
         <v>0</v>
       </c>
       <c r="DC25" s="5" t="str">
-        <f>FLOOR(DA25/8,1,1)&amp;"."&amp;FLOOR(MOD(DA25,8),1,1)&amp;"."&amp;(MOD(DA25,8)-FLOOR(MOD(DA25,8),1,1))*60</f>
+        <f>FLOOR(DA25/8,1)&amp;"."&amp;FLOOR(MOD(DA25,8),1)&amp;"."&amp;(MOD(DA25,8)-FLOOR(MOD(DA25,8),1))*60</f>
       </c>
     </row>
     <row r="26">
@@ -8509,7 +8524,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>77</v>
@@ -8521,19 +8536,19 @@
         <v>79</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K26" s="5" t="str">
         <f>INT(LEFT(E26,1))</f>
@@ -8641,7 +8656,7 @@
         <f>AR26/60</f>
       </c>
       <c r="AT26" s="5" t="str">
-        <f>FLOOR(AS26/8,1,1)&amp;"."&amp;FLOOR(MOD(AS26,8),1,1)&amp;"."&amp;(MOD(AS26,8)-FLOOR(MOD(AS26,8),1,1))*60</f>
+        <f>FLOOR(AS26/8,1)&amp;"."&amp;FLOOR(MOD(AS26,8),1)&amp;"."&amp;(MOD(AS26,8)-FLOOR(MOD(AS26,8),1))*60</f>
       </c>
       <c r="AU26" s="5" t="s">
         <v>83</v>
@@ -8824,7 +8839,7 @@
         <v>0</v>
       </c>
       <c r="DC26" s="5" t="str">
-        <f>FLOOR(DA26/8,1,1)&amp;"."&amp;FLOOR(MOD(DA26,8),1,1)&amp;"."&amp;(MOD(DA26,8)-FLOOR(MOD(DA26,8),1,1))*60</f>
+        <f>FLOOR(DA26/8,1)&amp;"."&amp;FLOOR(MOD(DA26,8),1)&amp;"."&amp;(MOD(DA26,8)-FLOOR(MOD(DA26,8),1))*60</f>
       </c>
     </row>
     <row r="27">
@@ -8832,7 +8847,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>77</v>
@@ -8844,19 +8859,19 @@
         <v>79</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K27" s="5" t="str">
         <f>INT(LEFT(E27,1))</f>
@@ -8964,7 +8979,7 @@
         <f>AR27/60</f>
       </c>
       <c r="AT27" s="5" t="str">
-        <f>FLOOR(AS27/8,1,1)&amp;"."&amp;FLOOR(MOD(AS27,8),1,1)&amp;"."&amp;(MOD(AS27,8)-FLOOR(MOD(AS27,8),1,1))*60</f>
+        <f>FLOOR(AS27/8,1)&amp;"."&amp;FLOOR(MOD(AS27,8),1)&amp;"."&amp;(MOD(AS27,8)-FLOOR(MOD(AS27,8),1))*60</f>
       </c>
       <c r="AU27" s="5" t="s">
         <v>83</v>
@@ -9147,7 +9162,7 @@
         <v>0</v>
       </c>
       <c r="DC27" s="5" t="str">
-        <f>FLOOR(DA27/8,1,1)&amp;"."&amp;FLOOR(MOD(DA27,8),1,1)&amp;"."&amp;(MOD(DA27,8)-FLOOR(MOD(DA27,8),1,1))*60</f>
+        <f>FLOOR(DA27/8,1)&amp;"."&amp;FLOOR(MOD(DA27,8),1)&amp;"."&amp;(MOD(DA27,8)-FLOOR(MOD(DA27,8),1))*60</f>
       </c>
     </row>
     <row r="28">
@@ -9155,7 +9170,7 @@
         <v>25</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>77</v>
@@ -9170,10 +9185,10 @@
         <v>79</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="I28" s="5" t="s">
         <v>86</v>
@@ -9287,16 +9302,16 @@
         <f>AR28/60</f>
       </c>
       <c r="AT28" s="5" t="str">
-        <f>FLOOR(AS28/8,1,1)&amp;"."&amp;FLOOR(MOD(AS28,8),1,1)&amp;"."&amp;(MOD(AS28,8)-FLOOR(MOD(AS28,8),1,1))*60</f>
+        <f>FLOOR(AS28/8,1)&amp;"."&amp;FLOOR(MOD(AS28,8),1)&amp;"."&amp;(MOD(AS28,8)-FLOOR(MOD(AS28,8),1))*60</f>
       </c>
       <c r="AU28" s="5" t="s">
         <v>88</v>
       </c>
       <c r="AV28" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AW28" s="5" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="AX28" s="5" t="s">
         <v>83</v>
@@ -9470,7 +9485,7 @@
         <v>0</v>
       </c>
       <c r="DC28" s="5" t="str">
-        <f>FLOOR(DA28/8,1,1)&amp;"."&amp;FLOOR(MOD(DA28,8),1,1)&amp;"."&amp;(MOD(DA28,8)-FLOOR(MOD(DA28,8),1,1))*60</f>
+        <f>FLOOR(DA28/8,1)&amp;"."&amp;FLOOR(MOD(DA28,8),1)&amp;"."&amp;(MOD(DA28,8)-FLOOR(MOD(DA28,8),1))*60</f>
       </c>
     </row>
     <row r="29">
@@ -9478,7 +9493,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>77</v>
@@ -9493,16 +9508,16 @@
         <v>79</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K29" s="5" t="str">
         <f>INT(LEFT(E29,1))</f>
@@ -9610,7 +9625,7 @@
         <f>AR29/60</f>
       </c>
       <c r="AT29" s="5" t="str">
-        <f>FLOOR(AS29/8,1,1)&amp;"."&amp;FLOOR(MOD(AS29,8),1,1)&amp;"."&amp;(MOD(AS29,8)-FLOOR(MOD(AS29,8),1,1))*60</f>
+        <f>FLOOR(AS29/8,1)&amp;"."&amp;FLOOR(MOD(AS29,8),1)&amp;"."&amp;(MOD(AS29,8)-FLOOR(MOD(AS29,8),1))*60</f>
       </c>
       <c r="AU29" s="5" t="s">
         <v>83</v>
@@ -9793,7 +9808,7 @@
         <v>0</v>
       </c>
       <c r="DC29" s="5" t="str">
-        <f>FLOOR(DA29/8,1,1)&amp;"."&amp;FLOOR(MOD(DA29,8),1,1)&amp;"."&amp;(MOD(DA29,8)-FLOOR(MOD(DA29,8),1,1))*60</f>
+        <f>FLOOR(DA29/8,1)&amp;"."&amp;FLOOR(MOD(DA29,8),1)&amp;"."&amp;(MOD(DA29,8)-FLOOR(MOD(DA29,8),1))*60</f>
       </c>
     </row>
     <row r="30">
@@ -9801,7 +9816,7 @@
         <v>27</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>77</v>
@@ -9825,7 +9840,7 @@
         <v>79</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="K30" s="5" t="str">
         <f>INT(LEFT(E30,1))</f>
@@ -9933,7 +9948,7 @@
         <f>AR30/60</f>
       </c>
       <c r="AT30" s="5" t="str">
-        <f>FLOOR(AS30/8,1,1)&amp;"."&amp;FLOOR(MOD(AS30,8),1,1)&amp;"."&amp;(MOD(AS30,8)-FLOOR(MOD(AS30,8),1,1))*60</f>
+        <f>FLOOR(AS30/8,1)&amp;"."&amp;FLOOR(MOD(AS30,8),1)&amp;"."&amp;(MOD(AS30,8)-FLOOR(MOD(AS30,8),1))*60</f>
       </c>
       <c r="AU30" s="5" t="s">
         <v>83</v>
@@ -10116,7 +10131,7 @@
         <v>0</v>
       </c>
       <c r="DC30" s="5" t="str">
-        <f>FLOOR(DA30/8,1,1)&amp;"."&amp;FLOOR(MOD(DA30,8),1,1)&amp;"."&amp;(MOD(DA30,8)-FLOOR(MOD(DA30,8),1,1))*60</f>
+        <f>FLOOR(DA30/8,1)&amp;"."&amp;FLOOR(MOD(DA30,8),1)&amp;"."&amp;(MOD(DA30,8)-FLOOR(MOD(DA30,8),1))*60</f>
       </c>
     </row>
     <row r="31">
@@ -10124,7 +10139,7 @@
         <v>28</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>77</v>
@@ -10133,22 +10148,22 @@
         <v>2</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K31" s="5" t="str">
         <f>INT(LEFT(E31,1))</f>
@@ -10256,10 +10271,10 @@
         <f>AR31/60</f>
       </c>
       <c r="AT31" s="5" t="str">
-        <f>FLOOR(AS31/8,1,1)&amp;"."&amp;FLOOR(MOD(AS31,8),1,1)&amp;"."&amp;(MOD(AS31,8)-FLOOR(MOD(AS31,8),1,1))*60</f>
+        <f>FLOOR(AS31/8,1)&amp;"."&amp;FLOOR(MOD(AS31,8),1)&amp;"."&amp;(MOD(AS31,8)-FLOOR(MOD(AS31,8),1))*60</f>
       </c>
       <c r="AU31" s="5" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AV31" s="5" t="s">
         <v>83</v>
@@ -10439,7 +10454,7 @@
         <v>0</v>
       </c>
       <c r="DC31" s="5" t="str">
-        <f>FLOOR(DA31/8,1,1)&amp;"."&amp;FLOOR(MOD(DA31,8),1,1)&amp;"."&amp;(MOD(DA31,8)-FLOOR(MOD(DA31,8),1,1))*60</f>
+        <f>FLOOR(DA31/8,1)&amp;"."&amp;FLOOR(MOD(DA31,8),1)&amp;"."&amp;(MOD(DA31,8)-FLOOR(MOD(DA31,8),1))*60</f>
       </c>
     </row>
     <row r="32">
@@ -10447,7 +10462,7 @@
         <v>29</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>77</v>
@@ -10462,16 +10477,16 @@
         <v>79</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I32" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K32" s="5" t="str">
         <f>INT(LEFT(E32,1))</f>
@@ -10579,7 +10594,7 @@
         <f>AR32/60</f>
       </c>
       <c r="AT32" s="5" t="str">
-        <f>FLOOR(AS32/8,1,1)&amp;"."&amp;FLOOR(MOD(AS32,8),1,1)&amp;"."&amp;(MOD(AS32,8)-FLOOR(MOD(AS32,8),1,1))*60</f>
+        <f>FLOOR(AS32/8,1)&amp;"."&amp;FLOOR(MOD(AS32,8),1)&amp;"."&amp;(MOD(AS32,8)-FLOOR(MOD(AS32,8),1))*60</f>
       </c>
       <c r="AU32" s="5" t="s">
         <v>83</v>
@@ -10762,7 +10777,7 @@
         <v>0</v>
       </c>
       <c r="DC32" s="5" t="str">
-        <f>FLOOR(DA32/8,1,1)&amp;"."&amp;FLOOR(MOD(DA32,8),1,1)&amp;"."&amp;(MOD(DA32,8)-FLOOR(MOD(DA32,8),1,1))*60</f>
+        <f>FLOOR(DA32/8,1)&amp;"."&amp;FLOOR(MOD(DA32,8),1)&amp;"."&amp;(MOD(DA32,8)-FLOOR(MOD(DA32,8),1))*60</f>
       </c>
     </row>
     <row r="33">
@@ -10770,7 +10785,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>77</v>
@@ -10788,13 +10803,13 @@
         <v>79</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="I33" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K33" s="5" t="str">
         <f>INT(LEFT(E33,1))</f>
@@ -10902,16 +10917,16 @@
         <f>AR33/60</f>
       </c>
       <c r="AT33" s="5" t="str">
-        <f>FLOOR(AS33/8,1,1)&amp;"."&amp;FLOOR(MOD(AS33,8),1,1)&amp;"."&amp;(MOD(AS33,8)-FLOOR(MOD(AS33,8),1,1))*60</f>
+        <f>FLOOR(AS33/8,1)&amp;"."&amp;FLOOR(MOD(AS33,8),1)&amp;"."&amp;(MOD(AS33,8)-FLOOR(MOD(AS33,8),1))*60</f>
       </c>
       <c r="AU33" s="5" t="s">
         <v>88</v>
       </c>
       <c r="AV33" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AW33" s="5" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="AX33" s="5" t="s">
         <v>83</v>
@@ -11085,7 +11100,7 @@
         <v>0</v>
       </c>
       <c r="DC33" s="5" t="str">
-        <f>FLOOR(DA33/8,1,1)&amp;"."&amp;FLOOR(MOD(DA33,8),1,1)&amp;"."&amp;(MOD(DA33,8)-FLOOR(MOD(DA33,8),1,1))*60</f>
+        <f>FLOOR(DA33/8,1)&amp;"."&amp;FLOOR(MOD(DA33,8),1)&amp;"."&amp;(MOD(DA33,8)-FLOOR(MOD(DA33,8),1))*60</f>
       </c>
     </row>
     <row r="34">
@@ -11093,7 +11108,7 @@
         <v>31</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>77</v>
@@ -11108,16 +11123,16 @@
         <v>78</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I34" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K34" s="5" t="str">
         <f>INT(LEFT(E34,1))</f>
@@ -11225,7 +11240,7 @@
         <f>AR34/60</f>
       </c>
       <c r="AT34" s="5" t="str">
-        <f>FLOOR(AS34/8,1,1)&amp;"."&amp;FLOOR(MOD(AS34,8),1,1)&amp;"."&amp;(MOD(AS34,8)-FLOOR(MOD(AS34,8),1,1))*60</f>
+        <f>FLOOR(AS34/8,1)&amp;"."&amp;FLOOR(MOD(AS34,8),1)&amp;"."&amp;(MOD(AS34,8)-FLOOR(MOD(AS34,8),1))*60</f>
       </c>
       <c r="AU34" s="5" t="s">
         <v>83</v>
@@ -11408,7 +11423,7 @@
         <v>0</v>
       </c>
       <c r="DC34" s="5" t="str">
-        <f>FLOOR(DA34/8,1,1)&amp;"."&amp;FLOOR(MOD(DA34,8),1,1)&amp;"."&amp;(MOD(DA34,8)-FLOOR(MOD(DA34,8),1,1))*60</f>
+        <f>FLOOR(DA34/8,1)&amp;"."&amp;FLOOR(MOD(DA34,8),1)&amp;"."&amp;(MOD(DA34,8)-FLOOR(MOD(DA34,8),1))*60</f>
       </c>
     </row>
     <row r="35">
@@ -11416,7 +11431,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>77</v>
@@ -11434,13 +11449,13 @@
         <v>79</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K35" s="5" t="str">
         <f>INT(LEFT(E35,1))</f>
@@ -11548,7 +11563,7 @@
         <f>AR35/60</f>
       </c>
       <c r="AT35" s="5" t="str">
-        <f>FLOOR(AS35/8,1,1)&amp;"."&amp;FLOOR(MOD(AS35,8),1,1)&amp;"."&amp;(MOD(AS35,8)-FLOOR(MOD(AS35,8),1,1))*60</f>
+        <f>FLOOR(AS35/8,1)&amp;"."&amp;FLOOR(MOD(AS35,8),1)&amp;"."&amp;(MOD(AS35,8)-FLOOR(MOD(AS35,8),1))*60</f>
       </c>
       <c r="AU35" s="5" t="s">
         <v>83</v>
@@ -11731,7 +11746,7 @@
         <v>0</v>
       </c>
       <c r="DC35" s="5" t="str">
-        <f>FLOOR(DA35/8,1,1)&amp;"."&amp;FLOOR(MOD(DA35,8),1,1)&amp;"."&amp;(MOD(DA35,8)-FLOOR(MOD(DA35,8),1,1))*60</f>
+        <f>FLOOR(DA35/8,1)&amp;"."&amp;FLOOR(MOD(DA35,8),1)&amp;"."&amp;(MOD(DA35,8)-FLOOR(MOD(DA35,8),1))*60</f>
       </c>
     </row>
     <row r="36">
@@ -11739,7 +11754,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>77</v>
@@ -11754,16 +11769,16 @@
         <v>79</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I36" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K36" s="5" t="str">
         <f>INT(LEFT(E36,1))</f>
@@ -11871,7 +11886,7 @@
         <f>AR36/60</f>
       </c>
       <c r="AT36" s="5" t="str">
-        <f>FLOOR(AS36/8,1,1)&amp;"."&amp;FLOOR(MOD(AS36,8),1,1)&amp;"."&amp;(MOD(AS36,8)-FLOOR(MOD(AS36,8),1,1))*60</f>
+        <f>FLOOR(AS36/8,1)&amp;"."&amp;FLOOR(MOD(AS36,8),1)&amp;"."&amp;(MOD(AS36,8)-FLOOR(MOD(AS36,8),1))*60</f>
       </c>
       <c r="AU36" s="5" t="s">
         <v>83</v>
@@ -12054,7 +12069,7 @@
         <v>0</v>
       </c>
       <c r="DC36" s="5" t="str">
-        <f>FLOOR(DA36/8,1,1)&amp;"."&amp;FLOOR(MOD(DA36,8),1,1)&amp;"."&amp;(MOD(DA36,8)-FLOOR(MOD(DA36,8),1,1))*60</f>
+        <f>FLOOR(DA36/8,1)&amp;"."&amp;FLOOR(MOD(DA36,8),1)&amp;"."&amp;(MOD(DA36,8)-FLOOR(MOD(DA36,8),1))*60</f>
       </c>
     </row>
     <row r="37">
@@ -12062,7 +12077,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>77</v>
@@ -12071,22 +12086,22 @@
         <v>1</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I37" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="K37" s="5" t="str">
         <f>INT(LEFT(E37,1))</f>
@@ -12194,7 +12209,7 @@
         <f>AR37/60</f>
       </c>
       <c r="AT37" s="5" t="str">
-        <f>FLOOR(AS37/8,1,1)&amp;"."&amp;FLOOR(MOD(AS37,8),1,1)&amp;"."&amp;(MOD(AS37,8)-FLOOR(MOD(AS37,8),1,1))*60</f>
+        <f>FLOOR(AS37/8,1)&amp;"."&amp;FLOOR(MOD(AS37,8),1)&amp;"."&amp;(MOD(AS37,8)-FLOOR(MOD(AS37,8),1))*60</f>
       </c>
       <c r="AU37" s="5" t="s">
         <v>83</v>
@@ -12377,7 +12392,7 @@
         <v>0</v>
       </c>
       <c r="DC37" s="5" t="str">
-        <f>FLOOR(DA37/8,1,1)&amp;"."&amp;FLOOR(MOD(DA37,8),1,1)&amp;"."&amp;(MOD(DA37,8)-FLOOR(MOD(DA37,8),1,1))*60</f>
+        <f>FLOOR(DA37/8,1)&amp;"."&amp;FLOOR(MOD(DA37,8),1)&amp;"."&amp;(MOD(DA37,8)-FLOOR(MOD(DA37,8),1))*60</f>
       </c>
     </row>
     <row r="38">
@@ -12385,7 +12400,7 @@
         <v>35</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>77</v>
@@ -12403,7 +12418,7 @@
         <v>79</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I38" s="5" t="s">
         <v>79</v>
@@ -12517,7 +12532,7 @@
         <f>AR38/60</f>
       </c>
       <c r="AT38" s="5" t="str">
-        <f>FLOOR(AS38/8,1,1)&amp;"."&amp;FLOOR(MOD(AS38,8),1,1)&amp;"."&amp;(MOD(AS38,8)-FLOOR(MOD(AS38,8),1,1))*60</f>
+        <f>FLOOR(AS38/8,1)&amp;"."&amp;FLOOR(MOD(AS38,8),1)&amp;"."&amp;(MOD(AS38,8)-FLOOR(MOD(AS38,8),1))*60</f>
       </c>
       <c r="AU38" s="5" t="s">
         <v>83</v>
@@ -12700,7 +12715,7 @@
         <v>0</v>
       </c>
       <c r="DC38" s="5" t="str">
-        <f>FLOOR(DA38/8,1,1)&amp;"."&amp;FLOOR(MOD(DA38,8),1,1)&amp;"."&amp;(MOD(DA38,8)-FLOOR(MOD(DA38,8),1,1))*60</f>
+        <f>FLOOR(DA38/8,1)&amp;"."&amp;FLOOR(MOD(DA38,8),1)&amp;"."&amp;(MOD(DA38,8)-FLOOR(MOD(DA38,8),1))*60</f>
       </c>
     </row>
     <row r="39">
@@ -12708,7 +12723,7 @@
         <v>36</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>77</v>
@@ -12723,10 +12738,10 @@
         <v>79</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>79</v>
@@ -12840,13 +12855,13 @@
         <f>AR39/60</f>
       </c>
       <c r="AT39" s="5" t="str">
-        <f>FLOOR(AS39/8,1,1)&amp;"."&amp;FLOOR(MOD(AS39,8),1,1)&amp;"."&amp;(MOD(AS39,8)-FLOOR(MOD(AS39,8),1,1))*60</f>
+        <f>FLOOR(AS39/8,1)&amp;"."&amp;FLOOR(MOD(AS39,8),1)&amp;"."&amp;(MOD(AS39,8)-FLOOR(MOD(AS39,8),1))*60</f>
       </c>
       <c r="AU39" s="5" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="AV39" s="5" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="AW39" s="5" t="s">
         <v>79</v>
@@ -13023,7 +13038,7 @@
         <v>0</v>
       </c>
       <c r="DC39" s="5" t="str">
-        <f>FLOOR(DA39/8,1,1)&amp;"."&amp;FLOOR(MOD(DA39,8),1,1)&amp;"."&amp;(MOD(DA39,8)-FLOOR(MOD(DA39,8),1,1))*60</f>
+        <f>FLOOR(DA39/8,1)&amp;"."&amp;FLOOR(MOD(DA39,8),1)&amp;"."&amp;(MOD(DA39,8)-FLOOR(MOD(DA39,8),1))*60</f>
       </c>
     </row>
     <row r="40">
@@ -13031,7 +13046,7 @@
         <v>37</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>77</v>
@@ -13046,16 +13061,16 @@
         <v>79</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="I40" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="K40" s="5" t="str">
         <f>INT(LEFT(E40,1))</f>
@@ -13163,10 +13178,10 @@
         <f>AR40/60</f>
       </c>
       <c r="AT40" s="5" t="str">
-        <f>FLOOR(AS40/8,1,1)&amp;"."&amp;FLOOR(MOD(AS40,8),1,1)&amp;"."&amp;(MOD(AS40,8)-FLOOR(MOD(AS40,8),1,1))*60</f>
+        <f>FLOOR(AS40/8,1)&amp;"."&amp;FLOOR(MOD(AS40,8),1)&amp;"."&amp;(MOD(AS40,8)-FLOOR(MOD(AS40,8),1))*60</f>
       </c>
       <c r="AU40" s="5" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="AV40" s="5" t="s">
         <v>83</v>
@@ -13346,7 +13361,7 @@
         <v>0</v>
       </c>
       <c r="DC40" s="5" t="str">
-        <f>FLOOR(DA40/8,1,1)&amp;"."&amp;FLOOR(MOD(DA40,8),1,1)&amp;"."&amp;(MOD(DA40,8)-FLOOR(MOD(DA40,8),1,1))*60</f>
+        <f>FLOOR(DA40/8,1)&amp;"."&amp;FLOOR(MOD(DA40,8),1)&amp;"."&amp;(MOD(DA40,8)-FLOOR(MOD(DA40,8),1))*60</f>
       </c>
     </row>
     <row r="41">
@@ -13354,7 +13369,7 @@
         <v>38</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>77</v>
@@ -13363,22 +13378,22 @@
         <v>6</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>79</v>
+        <v>126</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="I41" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="K41" s="5" t="str">
         <f>INT(LEFT(E41,1))</f>
@@ -13486,7 +13501,7 @@
         <f>AR41/60</f>
       </c>
       <c r="AT41" s="5" t="str">
-        <f>FLOOR(AS41/8,1,1)&amp;"."&amp;FLOOR(MOD(AS41,8),1,1)&amp;"."&amp;(MOD(AS41,8)-FLOOR(MOD(AS41,8),1,1))*60</f>
+        <f>FLOOR(AS41/8,1)&amp;"."&amp;FLOOR(MOD(AS41,8),1)&amp;"."&amp;(MOD(AS41,8)-FLOOR(MOD(AS41,8),1))*60</f>
       </c>
       <c r="AU41" s="5" t="s">
         <v>83</v>
@@ -13669,7 +13684,7 @@
         <v>0</v>
       </c>
       <c r="DC41" s="5" t="str">
-        <f>FLOOR(DA41/8,1,1)&amp;"."&amp;FLOOR(MOD(DA41,8),1,1)&amp;"."&amp;(MOD(DA41,8)-FLOOR(MOD(DA41,8),1,1))*60</f>
+        <f>FLOOR(DA41/8,1)&amp;"."&amp;FLOOR(MOD(DA41,8),1)&amp;"."&amp;(MOD(DA41,8)-FLOOR(MOD(DA41,8),1))*60</f>
       </c>
     </row>
     <row r="42">
@@ -13677,7 +13692,7 @@
         <v>39</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>77</v>
@@ -13686,22 +13701,22 @@
         <v>5</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I42" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K42" s="5" t="str">
         <f>INT(LEFT(E42,1))</f>
@@ -13809,7 +13824,7 @@
         <f>AR42/60</f>
       </c>
       <c r="AT42" s="5" t="str">
-        <f>FLOOR(AS42/8,1,1)&amp;"."&amp;FLOOR(MOD(AS42,8),1,1)&amp;"."&amp;(MOD(AS42,8)-FLOOR(MOD(AS42,8),1,1))*60</f>
+        <f>FLOOR(AS42/8,1)&amp;"."&amp;FLOOR(MOD(AS42,8),1)&amp;"."&amp;(MOD(AS42,8)-FLOOR(MOD(AS42,8),1))*60</f>
       </c>
       <c r="AU42" s="5" t="s">
         <v>83</v>
@@ -13992,7 +14007,7 @@
         <v>0</v>
       </c>
       <c r="DC42" s="5" t="str">
-        <f>FLOOR(DA42/8,1,1)&amp;"."&amp;FLOOR(MOD(DA42,8),1,1)&amp;"."&amp;(MOD(DA42,8)-FLOOR(MOD(DA42,8),1,1))*60</f>
+        <f>FLOOR(DA42/8,1)&amp;"."&amp;FLOOR(MOD(DA42,8),1)&amp;"."&amp;(MOD(DA42,8)-FLOOR(MOD(DA42,8),1))*60</f>
       </c>
     </row>
     <row r="43">
@@ -14000,7 +14015,7 @@
         <v>40</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>77</v>
@@ -14015,16 +14030,16 @@
         <v>79</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>79</v>
+        <v>123</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K43" s="5" t="str">
         <f>INT(LEFT(E43,1))</f>
@@ -14132,7 +14147,7 @@
         <f>AR43/60</f>
       </c>
       <c r="AT43" s="5" t="str">
-        <f>FLOOR(AS43/8,1,1)&amp;"."&amp;FLOOR(MOD(AS43,8),1,1)&amp;"."&amp;(MOD(AS43,8)-FLOOR(MOD(AS43,8),1,1))*60</f>
+        <f>FLOOR(AS43/8,1)&amp;"."&amp;FLOOR(MOD(AS43,8),1)&amp;"."&amp;(MOD(AS43,8)-FLOOR(MOD(AS43,8),1))*60</f>
       </c>
       <c r="AU43" s="5" t="s">
         <v>83</v>
@@ -14315,7 +14330,7 @@
         <v>0</v>
       </c>
       <c r="DC43" s="5" t="str">
-        <f>FLOOR(DA43/8,1,1)&amp;"."&amp;FLOOR(MOD(DA43,8),1,1)&amp;"."&amp;(MOD(DA43,8)-FLOOR(MOD(DA43,8),1,1))*60</f>
+        <f>FLOOR(DA43/8,1)&amp;"."&amp;FLOOR(MOD(DA43,8),1)&amp;"."&amp;(MOD(DA43,8)-FLOOR(MOD(DA43,8),1))*60</f>
       </c>
     </row>
     <row r="44">
@@ -14323,7 +14338,7 @@
         <v>41</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>77</v>
@@ -14341,13 +14356,13 @@
         <v>86</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I44" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K44" s="5" t="str">
         <f>INT(LEFT(E44,1))</f>
@@ -14455,16 +14470,16 @@
         <f>AR44/60</f>
       </c>
       <c r="AT44" s="5" t="str">
-        <f>FLOOR(AS44/8,1,1)&amp;"."&amp;FLOOR(MOD(AS44,8),1,1)&amp;"."&amp;(MOD(AS44,8)-FLOOR(MOD(AS44,8),1,1))*60</f>
+        <f>FLOOR(AS44/8,1)&amp;"."&amp;FLOOR(MOD(AS44,8),1)&amp;"."&amp;(MOD(AS44,8)-FLOOR(MOD(AS44,8),1))*60</f>
       </c>
       <c r="AU44" s="5" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="AV44" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AW44" s="5" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="AX44" s="5" t="s">
         <v>83</v>
@@ -14638,7 +14653,7 @@
         <v>0</v>
       </c>
       <c r="DC44" s="5" t="str">
-        <f>FLOOR(DA44/8,1,1)&amp;"."&amp;FLOOR(MOD(DA44,8),1,1)&amp;"."&amp;(MOD(DA44,8)-FLOOR(MOD(DA44,8),1,1))*60</f>
+        <f>FLOOR(DA44/8,1)&amp;"."&amp;FLOOR(MOD(DA44,8),1)&amp;"."&amp;(MOD(DA44,8)-FLOOR(MOD(DA44,8),1))*60</f>
       </c>
     </row>
     <row r="45">
@@ -14646,7 +14661,7 @@
         <v>42</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>77</v>
@@ -14655,13 +14670,13 @@
         <v>1</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>79</v>
@@ -14778,7 +14793,7 @@
         <f>AR45/60</f>
       </c>
       <c r="AT45" s="5" t="str">
-        <f>FLOOR(AS45/8,1,1)&amp;"."&amp;FLOOR(MOD(AS45,8),1,1)&amp;"."&amp;(MOD(AS45,8)-FLOOR(MOD(AS45,8),1,1))*60</f>
+        <f>FLOOR(AS45/8,1)&amp;"."&amp;FLOOR(MOD(AS45,8),1)&amp;"."&amp;(MOD(AS45,8)-FLOOR(MOD(AS45,8),1))*60</f>
       </c>
       <c r="AU45" s="5" t="s">
         <v>83</v>
@@ -14961,7 +14976,7 @@
         <v>0</v>
       </c>
       <c r="DC45" s="5" t="str">
-        <f>FLOOR(DA45/8,1,1)&amp;"."&amp;FLOOR(MOD(DA45,8),1,1)&amp;"."&amp;(MOD(DA45,8)-FLOOR(MOD(DA45,8),1,1))*60</f>
+        <f>FLOOR(DA45/8,1)&amp;"."&amp;FLOOR(MOD(DA45,8),1)&amp;"."&amp;(MOD(DA45,8)-FLOOR(MOD(DA45,8),1))*60</f>
       </c>
     </row>
     <row r="46">
@@ -14969,7 +14984,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>77</v>
@@ -14984,7 +14999,7 @@
         <v>79</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H46" s="5" t="s">
         <v>86</v>
@@ -14993,7 +15008,7 @@
         <v>79</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K46" s="5" t="str">
         <f>INT(LEFT(E46,1))</f>
@@ -15101,7 +15116,7 @@
         <f>AR46/60</f>
       </c>
       <c r="AT46" s="5" t="str">
-        <f>FLOOR(AS46/8,1,1)&amp;"."&amp;FLOOR(MOD(AS46,8),1,1)&amp;"."&amp;(MOD(AS46,8)-FLOOR(MOD(AS46,8),1,1))*60</f>
+        <f>FLOOR(AS46/8,1)&amp;"."&amp;FLOOR(MOD(AS46,8),1)&amp;"."&amp;(MOD(AS46,8)-FLOOR(MOD(AS46,8),1))*60</f>
       </c>
       <c r="AU46" s="5" t="s">
         <v>83</v>
@@ -15284,7 +15299,7 @@
         <v>0</v>
       </c>
       <c r="DC46" s="5" t="str">
-        <f>FLOOR(DA46/8,1,1)&amp;"."&amp;FLOOR(MOD(DA46,8),1,1)&amp;"."&amp;(MOD(DA46,8)-FLOOR(MOD(DA46,8),1,1))*60</f>
+        <f>FLOOR(DA46/8,1)&amp;"."&amp;FLOOR(MOD(DA46,8),1)&amp;"."&amp;(MOD(DA46,8)-FLOOR(MOD(DA46,8),1))*60</f>
       </c>
     </row>
     <row r="47">
@@ -15292,7 +15307,7 @@
         <v>44</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>77</v>
@@ -15307,16 +15322,16 @@
         <v>79</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>86</v>
+        <v>140</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I47" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K47" s="5" t="str">
         <f>INT(LEFT(E47,1))</f>
@@ -15424,7 +15439,7 @@
         <f>AR47/60</f>
       </c>
       <c r="AT47" s="5" t="str">
-        <f>FLOOR(AS47/8,1,1)&amp;"."&amp;FLOOR(MOD(AS47,8),1,1)&amp;"."&amp;(MOD(AS47,8)-FLOOR(MOD(AS47,8),1,1))*60</f>
+        <f>FLOOR(AS47/8,1)&amp;"."&amp;FLOOR(MOD(AS47,8),1)&amp;"."&amp;(MOD(AS47,8)-FLOOR(MOD(AS47,8),1))*60</f>
       </c>
       <c r="AU47" s="5" t="s">
         <v>83</v>
@@ -15607,7 +15622,7 @@
         <v>0</v>
       </c>
       <c r="DC47" s="5" t="str">
-        <f>FLOOR(DA47/8,1,1)&amp;"."&amp;FLOOR(MOD(DA47,8),1,1)&amp;"."&amp;(MOD(DA47,8)-FLOOR(MOD(DA47,8),1,1))*60</f>
+        <f>FLOOR(DA47/8,1)&amp;"."&amp;FLOOR(MOD(DA47,8),1)&amp;"."&amp;(MOD(DA47,8)-FLOOR(MOD(DA47,8),1))*60</f>
       </c>
     </row>
     <row r="48">
@@ -15615,7 +15630,7 @@
         <v>45</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>77</v>
@@ -15630,16 +15645,16 @@
         <v>79</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I48" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K48" s="5" t="str">
         <f>INT(LEFT(E48,1))</f>
@@ -15747,7 +15762,7 @@
         <f>AR48/60</f>
       </c>
       <c r="AT48" s="5" t="str">
-        <f>FLOOR(AS48/8,1,1)&amp;"."&amp;FLOOR(MOD(AS48,8),1,1)&amp;"."&amp;(MOD(AS48,8)-FLOOR(MOD(AS48,8),1,1))*60</f>
+        <f>FLOOR(AS48/8,1)&amp;"."&amp;FLOOR(MOD(AS48,8),1)&amp;"."&amp;(MOD(AS48,8)-FLOOR(MOD(AS48,8),1))*60</f>
       </c>
       <c r="AU48" s="5" t="s">
         <v>83</v>
@@ -15930,7 +15945,7 @@
         <v>0</v>
       </c>
       <c r="DC48" s="5" t="str">
-        <f>FLOOR(DA48/8,1,1)&amp;"."&amp;FLOOR(MOD(DA48,8),1,1)&amp;"."&amp;(MOD(DA48,8)-FLOOR(MOD(DA48,8),1,1))*60</f>
+        <f>FLOOR(DA48/8,1)&amp;"."&amp;FLOOR(MOD(DA48,8),1)&amp;"."&amp;(MOD(DA48,8)-FLOOR(MOD(DA48,8),1))*60</f>
       </c>
     </row>
     <row r="49">
@@ -15938,7 +15953,7 @@
         <v>46</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>77</v>
@@ -15947,22 +15962,22 @@
         <v>2</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>78</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I49" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K49" s="5" t="str">
         <f>INT(LEFT(E49,1))</f>
@@ -16070,7 +16085,7 @@
         <f>AR49/60</f>
       </c>
       <c r="AT49" s="5" t="str">
-        <f>FLOOR(AS49/8,1,1)&amp;"."&amp;FLOOR(MOD(AS49,8),1,1)&amp;"."&amp;(MOD(AS49,8)-FLOOR(MOD(AS49,8),1,1))*60</f>
+        <f>FLOOR(AS49/8,1)&amp;"."&amp;FLOOR(MOD(AS49,8),1)&amp;"."&amp;(MOD(AS49,8)-FLOOR(MOD(AS49,8),1))*60</f>
       </c>
       <c r="AU49" s="5" t="s">
         <v>82</v>
@@ -16253,7 +16268,7 @@
         <v>0</v>
       </c>
       <c r="DC49" s="5" t="str">
-        <f>FLOOR(DA49/8,1,1)&amp;"."&amp;FLOOR(MOD(DA49,8),1,1)&amp;"."&amp;(MOD(DA49,8)-FLOOR(MOD(DA49,8),1,1))*60</f>
+        <f>FLOOR(DA49/8,1)&amp;"."&amp;FLOOR(MOD(DA49,8),1)&amp;"."&amp;(MOD(DA49,8)-FLOOR(MOD(DA49,8),1))*60</f>
       </c>
     </row>
     <row r="50">
@@ -16261,7 +16276,7 @@
         <v>47</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>77</v>
@@ -16270,22 +16285,22 @@
         <v>3</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I50" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K50" s="5" t="str">
         <f>INT(LEFT(E50,1))</f>
@@ -16393,7 +16408,7 @@
         <f>AR50/60</f>
       </c>
       <c r="AT50" s="5" t="str">
-        <f>FLOOR(AS50/8,1,1)&amp;"."&amp;FLOOR(MOD(AS50,8),1,1)&amp;"."&amp;(MOD(AS50,8)-FLOOR(MOD(AS50,8),1,1))*60</f>
+        <f>FLOOR(AS50/8,1)&amp;"."&amp;FLOOR(MOD(AS50,8),1)&amp;"."&amp;(MOD(AS50,8)-FLOOR(MOD(AS50,8),1))*60</f>
       </c>
       <c r="AU50" s="5" t="s">
         <v>83</v>
@@ -16576,7 +16591,7 @@
         <v>0</v>
       </c>
       <c r="DC50" s="5" t="str">
-        <f>FLOOR(DA50/8,1,1)&amp;"."&amp;FLOOR(MOD(DA50,8),1,1)&amp;"."&amp;(MOD(DA50,8)-FLOOR(MOD(DA50,8),1,1))*60</f>
+        <f>FLOOR(DA50/8,1)&amp;"."&amp;FLOOR(MOD(DA50,8),1)&amp;"."&amp;(MOD(DA50,8)-FLOOR(MOD(DA50,8),1))*60</f>
       </c>
     </row>
     <row r="51">
@@ -16584,7 +16599,7 @@
         <v>48</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>77</v>
@@ -16599,16 +16614,16 @@
         <v>79</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I51" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="K51" s="5" t="str">
         <f>INT(LEFT(E51,1))</f>
@@ -16716,7 +16731,7 @@
         <f>AR51/60</f>
       </c>
       <c r="AT51" s="5" t="str">
-        <f>FLOOR(AS51/8,1,1)&amp;"."&amp;FLOOR(MOD(AS51,8),1,1)&amp;"."&amp;(MOD(AS51,8)-FLOOR(MOD(AS51,8),1,1))*60</f>
+        <f>FLOOR(AS51/8,1)&amp;"."&amp;FLOOR(MOD(AS51,8),1)&amp;"."&amp;(MOD(AS51,8)-FLOOR(MOD(AS51,8),1))*60</f>
       </c>
       <c r="AU51" s="5" t="s">
         <v>83</v>
@@ -16899,7 +16914,7 @@
         <v>0</v>
       </c>
       <c r="DC51" s="5" t="str">
-        <f>FLOOR(DA51/8,1,1)&amp;"."&amp;FLOOR(MOD(DA51,8),1,1)&amp;"."&amp;(MOD(DA51,8)-FLOOR(MOD(DA51,8),1,1))*60</f>
+        <f>FLOOR(DA51/8,1)&amp;"."&amp;FLOOR(MOD(DA51,8),1)&amp;"."&amp;(MOD(DA51,8)-FLOOR(MOD(DA51,8),1))*60</f>
       </c>
     </row>
     <row r="52">
@@ -16907,7 +16922,7 @@
         <v>49</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>77</v>
@@ -16916,22 +16931,22 @@
         <v>2</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I52" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K52" s="5" t="str">
         <f>INT(LEFT(E52,1))</f>
@@ -17039,7 +17054,7 @@
         <f>AR52/60</f>
       </c>
       <c r="AT52" s="5" t="str">
-        <f>FLOOR(AS52/8,1,1)&amp;"."&amp;FLOOR(MOD(AS52,8),1,1)&amp;"."&amp;(MOD(AS52,8)-FLOOR(MOD(AS52,8),1,1))*60</f>
+        <f>FLOOR(AS52/8,1)&amp;"."&amp;FLOOR(MOD(AS52,8),1)&amp;"."&amp;(MOD(AS52,8)-FLOOR(MOD(AS52,8),1))*60</f>
       </c>
       <c r="AU52" s="5" t="s">
         <v>83</v>
@@ -17222,7 +17237,7 @@
         <v>0</v>
       </c>
       <c r="DC52" s="5" t="str">
-        <f>FLOOR(DA52/8,1,1)&amp;"."&amp;FLOOR(MOD(DA52,8),1,1)&amp;"."&amp;(MOD(DA52,8)-FLOOR(MOD(DA52,8),1,1))*60</f>
+        <f>FLOOR(DA52/8,1)&amp;"."&amp;FLOOR(MOD(DA52,8),1)&amp;"."&amp;(MOD(DA52,8)-FLOOR(MOD(DA52,8),1))*60</f>
       </c>
     </row>
     <row r="53">
@@ -17230,7 +17245,7 @@
         <v>50</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>77</v>
@@ -17245,16 +17260,16 @@
         <v>78</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I53" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K53" s="5" t="str">
         <f>INT(LEFT(E53,1))</f>
@@ -17362,7 +17377,7 @@
         <f>AR53/60</f>
       </c>
       <c r="AT53" s="5" t="str">
-        <f>FLOOR(AS53/8,1,1)&amp;"."&amp;FLOOR(MOD(AS53,8),1,1)&amp;"."&amp;(MOD(AS53,8)-FLOOR(MOD(AS53,8),1,1))*60</f>
+        <f>FLOOR(AS53/8,1)&amp;"."&amp;FLOOR(MOD(AS53,8),1)&amp;"."&amp;(MOD(AS53,8)-FLOOR(MOD(AS53,8),1))*60</f>
       </c>
       <c r="AU53" s="5" t="s">
         <v>83</v>
@@ -17545,7 +17560,7 @@
         <v>0</v>
       </c>
       <c r="DC53" s="5" t="str">
-        <f>FLOOR(DA53/8,1,1)&amp;"."&amp;FLOOR(MOD(DA53,8),1,1)&amp;"."&amp;(MOD(DA53,8)-FLOOR(MOD(DA53,8),1,1))*60</f>
+        <f>FLOOR(DA53/8,1)&amp;"."&amp;FLOOR(MOD(DA53,8),1)&amp;"."&amp;(MOD(DA53,8)-FLOOR(MOD(DA53,8),1))*60</f>
       </c>
     </row>
     <row r="54">
@@ -17553,7 +17568,7 @@
         <v>51</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>77</v>
@@ -17568,16 +17583,16 @@
         <v>79</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I54" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K54" s="5" t="str">
         <f>INT(LEFT(E54,1))</f>
@@ -17685,7 +17700,7 @@
         <f>AR54/60</f>
       </c>
       <c r="AT54" s="5" t="str">
-        <f>FLOOR(AS54/8,1,1)&amp;"."&amp;FLOOR(MOD(AS54,8),1,1)&amp;"."&amp;(MOD(AS54,8)-FLOOR(MOD(AS54,8),1,1))*60</f>
+        <f>FLOOR(AS54/8,1)&amp;"."&amp;FLOOR(MOD(AS54,8),1)&amp;"."&amp;(MOD(AS54,8)-FLOOR(MOD(AS54,8),1))*60</f>
       </c>
       <c r="AU54" s="5" t="s">
         <v>83</v>
@@ -17868,7 +17883,7 @@
         <v>0</v>
       </c>
       <c r="DC54" s="5" t="str">
-        <f>FLOOR(DA54/8,1,1)&amp;"."&amp;FLOOR(MOD(DA54,8),1,1)&amp;"."&amp;(MOD(DA54,8)-FLOOR(MOD(DA54,8),1,1))*60</f>
+        <f>FLOOR(DA54/8,1)&amp;"."&amp;FLOOR(MOD(DA54,8),1)&amp;"."&amp;(MOD(DA54,8)-FLOOR(MOD(DA54,8),1))*60</f>
       </c>
     </row>
     <row r="55">
@@ -17876,7 +17891,7 @@
         <v>52</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>77</v>
@@ -17891,16 +17906,16 @@
         <v>79</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="K55" s="5" t="str">
         <f>INT(LEFT(E55,1))</f>
@@ -18008,7 +18023,7 @@
         <f>AR55/60</f>
       </c>
       <c r="AT55" s="5" t="str">
-        <f>FLOOR(AS55/8,1,1)&amp;"."&amp;FLOOR(MOD(AS55,8),1,1)&amp;"."&amp;(MOD(AS55,8)-FLOOR(MOD(AS55,8),1,1))*60</f>
+        <f>FLOOR(AS55/8,1)&amp;"."&amp;FLOOR(MOD(AS55,8),1)&amp;"."&amp;(MOD(AS55,8)-FLOOR(MOD(AS55,8),1))*60</f>
       </c>
       <c r="AU55" s="5" t="s">
         <v>82</v>
@@ -18191,7 +18206,7 @@
         <v>0</v>
       </c>
       <c r="DC55" s="5" t="str">
-        <f>FLOOR(DA55/8,1,1)&amp;"."&amp;FLOOR(MOD(DA55,8),1,1)&amp;"."&amp;(MOD(DA55,8)-FLOOR(MOD(DA55,8),1,1))*60</f>
+        <f>FLOOR(DA55/8,1)&amp;"."&amp;FLOOR(MOD(DA55,8),1)&amp;"."&amp;(MOD(DA55,8)-FLOOR(MOD(DA55,8),1))*60</f>
       </c>
     </row>
     <row r="56">
@@ -18199,7 +18214,7 @@
         <v>53</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>77</v>
@@ -18208,16 +18223,16 @@
         <v>5</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>79</v>
@@ -18331,7 +18346,7 @@
         <f>AR56/60</f>
       </c>
       <c r="AT56" s="5" t="str">
-        <f>FLOOR(AS56/8,1,1)&amp;"."&amp;FLOOR(MOD(AS56,8),1,1)&amp;"."&amp;(MOD(AS56,8)-FLOOR(MOD(AS56,8),1,1))*60</f>
+        <f>FLOOR(AS56/8,1)&amp;"."&amp;FLOOR(MOD(AS56,8),1)&amp;"."&amp;(MOD(AS56,8)-FLOOR(MOD(AS56,8),1))*60</f>
       </c>
       <c r="AU56" s="5" t="s">
         <v>83</v>
@@ -18514,7 +18529,7 @@
         <v>0</v>
       </c>
       <c r="DC56" s="5" t="str">
-        <f>FLOOR(DA56/8,1,1)&amp;"."&amp;FLOOR(MOD(DA56,8),1,1)&amp;"."&amp;(MOD(DA56,8)-FLOOR(MOD(DA56,8),1,1))*60</f>
+        <f>FLOOR(DA56/8,1)&amp;"."&amp;FLOOR(MOD(DA56,8),1)&amp;"."&amp;(MOD(DA56,8)-FLOOR(MOD(DA56,8),1))*60</f>
       </c>
     </row>
     <row r="57">
@@ -18522,7 +18537,7 @@
         <v>54</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>77</v>
@@ -18537,7 +18552,7 @@
         <v>78</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="H57" s="5" t="s">
         <v>86</v>
@@ -18546,7 +18561,7 @@
         <v>79</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K57" s="5" t="str">
         <f>INT(LEFT(E57,1))</f>
@@ -18654,10 +18669,10 @@
         <f>AR57/60</f>
       </c>
       <c r="AT57" s="5" t="str">
-        <f>FLOOR(AS57/8,1,1)&amp;"."&amp;FLOOR(MOD(AS57,8),1,1)&amp;"."&amp;(MOD(AS57,8)-FLOOR(MOD(AS57,8),1,1))*60</f>
+        <f>FLOOR(AS57/8,1)&amp;"."&amp;FLOOR(MOD(AS57,8),1)&amp;"."&amp;(MOD(AS57,8)-FLOOR(MOD(AS57,8),1))*60</f>
       </c>
       <c r="AU57" s="5" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="AV57" s="5" t="s">
         <v>83</v>
@@ -18837,7 +18852,7 @@
         <v>0</v>
       </c>
       <c r="DC57" s="5" t="str">
-        <f>FLOOR(DA57/8,1,1)&amp;"."&amp;FLOOR(MOD(DA57,8),1,1)&amp;"."&amp;(MOD(DA57,8)-FLOOR(MOD(DA57,8),1,1))*60</f>
+        <f>FLOOR(DA57/8,1)&amp;"."&amp;FLOOR(MOD(DA57,8),1)&amp;"."&amp;(MOD(DA57,8)-FLOOR(MOD(DA57,8),1))*60</f>
       </c>
     </row>
     <row r="58">
@@ -18845,7 +18860,7 @@
         <v>55</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>77</v>
@@ -18860,16 +18875,16 @@
         <v>79</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="K58" s="5" t="str">
         <f>INT(LEFT(E58,1))</f>
@@ -18977,7 +18992,7 @@
         <f>AR58/60</f>
       </c>
       <c r="AT58" s="5" t="str">
-        <f>FLOOR(AS58/8,1,1)&amp;"."&amp;FLOOR(MOD(AS58,8),1,1)&amp;"."&amp;(MOD(AS58,8)-FLOOR(MOD(AS58,8),1,1))*60</f>
+        <f>FLOOR(AS58/8,1)&amp;"."&amp;FLOOR(MOD(AS58,8),1)&amp;"."&amp;(MOD(AS58,8)-FLOOR(MOD(AS58,8),1))*60</f>
       </c>
       <c r="AU58" s="5" t="s">
         <v>83</v>
@@ -19160,7 +19175,7 @@
         <v>0</v>
       </c>
       <c r="DC58" s="5" t="str">
-        <f>FLOOR(DA58/8,1,1)&amp;"."&amp;FLOOR(MOD(DA58,8),1,1)&amp;"."&amp;(MOD(DA58,8)-FLOOR(MOD(DA58,8),1,1))*60</f>
+        <f>FLOOR(DA58/8,1)&amp;"."&amp;FLOOR(MOD(DA58,8),1)&amp;"."&amp;(MOD(DA58,8)-FLOOR(MOD(DA58,8),1))*60</f>
       </c>
     </row>
     <row r="59">
@@ -19168,7 +19183,7 @@
         <v>56</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>77</v>
@@ -19183,16 +19198,16 @@
         <v>79</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K59" s="5" t="str">
         <f>INT(LEFT(E59,1))</f>
@@ -19300,7 +19315,7 @@
         <f>AR59/60</f>
       </c>
       <c r="AT59" s="5" t="str">
-        <f>FLOOR(AS59/8,1,1)&amp;"."&amp;FLOOR(MOD(AS59,8),1,1)&amp;"."&amp;(MOD(AS59,8)-FLOOR(MOD(AS59,8),1,1))*60</f>
+        <f>FLOOR(AS59/8,1)&amp;"."&amp;FLOOR(MOD(AS59,8),1)&amp;"."&amp;(MOD(AS59,8)-FLOOR(MOD(AS59,8),1))*60</f>
       </c>
       <c r="AU59" s="5" t="s">
         <v>83</v>
@@ -19483,7 +19498,7 @@
         <v>0</v>
       </c>
       <c r="DC59" s="5" t="str">
-        <f>FLOOR(DA59/8,1,1)&amp;"."&amp;FLOOR(MOD(DA59,8),1,1)&amp;"."&amp;(MOD(DA59,8)-FLOOR(MOD(DA59,8),1,1))*60</f>
+        <f>FLOOR(DA59/8,1)&amp;"."&amp;FLOOR(MOD(DA59,8),1)&amp;"."&amp;(MOD(DA59,8)-FLOOR(MOD(DA59,8),1))*60</f>
       </c>
     </row>
     <row r="60">
@@ -19491,7 +19506,7 @@
         <v>57</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>77</v>
@@ -19506,16 +19521,16 @@
         <v>79</v>
       </c>
       <c r="G60" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H60" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="H60" s="5" t="s">
-        <v>80</v>
-      </c>
       <c r="I60" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K60" s="5" t="str">
         <f>INT(LEFT(E60,1))</f>
@@ -19623,7 +19638,7 @@
         <f>AR60/60</f>
       </c>
       <c r="AT60" s="5" t="str">
-        <f>FLOOR(AS60/8,1,1)&amp;"."&amp;FLOOR(MOD(AS60,8),1,1)&amp;"."&amp;(MOD(AS60,8)-FLOOR(MOD(AS60,8),1,1))*60</f>
+        <f>FLOOR(AS60/8,1)&amp;"."&amp;FLOOR(MOD(AS60,8),1)&amp;"."&amp;(MOD(AS60,8)-FLOOR(MOD(AS60,8),1))*60</f>
       </c>
       <c r="AU60" s="5" t="s">
         <v>83</v>
@@ -19806,7 +19821,7 @@
         <v>0</v>
       </c>
       <c r="DC60" s="5" t="str">
-        <f>FLOOR(DA60/8,1,1)&amp;"."&amp;FLOOR(MOD(DA60,8),1,1)&amp;"."&amp;(MOD(DA60,8)-FLOOR(MOD(DA60,8),1,1))*60</f>
+        <f>FLOOR(DA60/8,1)&amp;"."&amp;FLOOR(MOD(DA60,8),1)&amp;"."&amp;(MOD(DA60,8)-FLOOR(MOD(DA60,8),1))*60</f>
       </c>
     </row>
     <row r="61">
@@ -19814,7 +19829,7 @@
         <v>58</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>77</v>
@@ -19829,16 +19844,16 @@
         <v>79</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K61" s="5" t="str">
         <f>INT(LEFT(E61,1))</f>
@@ -19946,7 +19961,7 @@
         <f>AR61/60</f>
       </c>
       <c r="AT61" s="5" t="str">
-        <f>FLOOR(AS61/8,1,1)&amp;"."&amp;FLOOR(MOD(AS61,8),1,1)&amp;"."&amp;(MOD(AS61,8)-FLOOR(MOD(AS61,8),1,1))*60</f>
+        <f>FLOOR(AS61/8,1)&amp;"."&amp;FLOOR(MOD(AS61,8),1)&amp;"."&amp;(MOD(AS61,8)-FLOOR(MOD(AS61,8),1))*60</f>
       </c>
       <c r="AU61" s="5" t="s">
         <v>83</v>
@@ -20129,7 +20144,7 @@
         <v>0</v>
       </c>
       <c r="DC61" s="5" t="str">
-        <f>FLOOR(DA61/8,1,1)&amp;"."&amp;FLOOR(MOD(DA61,8),1,1)&amp;"."&amp;(MOD(DA61,8)-FLOOR(MOD(DA61,8),1,1))*60</f>
+        <f>FLOOR(DA61/8,1)&amp;"."&amp;FLOOR(MOD(DA61,8),1)&amp;"."&amp;(MOD(DA61,8)-FLOOR(MOD(DA61,8),1))*60</f>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed num hrs late computation
</commit_message>
<xml_diff>
--- a/exceltocsv/public/reports/DTRSUMMARY.xlsx
+++ b/exceltocsv/public/reports/DTRSUMMARY.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="175">
   <si>
     <t>iRipple, Inc.</t>
   </si>
@@ -245,7 +245,7 @@
     <t>emp.department</t>
   </si>
   <si>
-    <t>0.0.15</t>
+    <t>0.0.30</t>
   </si>
   <si>
     <t>0.0.0</t>
@@ -335,6 +335,9 @@
     <t>Buena,Ian Christopher</t>
   </si>
   <si>
+    <t>0.0.15</t>
+  </si>
+  <si>
     <t>Buenafe,Rajiv</t>
   </si>
   <si>
@@ -348,9 +351,6 @@
   </si>
   <si>
     <t>0.3.0</t>
-  </si>
-  <si>
-    <t>0.0.30</t>
   </si>
   <si>
     <t>Cerbo,Jaycer</t>
@@ -489,6 +489,9 @@
   </si>
   <si>
     <t>Reyes,Mark Gil</t>
+  </si>
+  <si>
+    <t>0.2.0</t>
   </si>
   <si>
     <t>Reyes,Salvador</t>
@@ -1424,7 +1427,7 @@
         <v>77</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>78</v>
@@ -5306,7 +5309,7 @@
         <v>103</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>85</v>
@@ -5617,7 +5620,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>77</v>
@@ -5940,7 +5943,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>77</v>
@@ -5964,7 +5967,7 @@
         <v>79</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K18" s="5" t="str">
         <f>INT(LEFT(E18,1))</f>
@@ -6263,7 +6266,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>77</v>
@@ -6272,10 +6275,10 @@
         <v>4</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>85</v>
@@ -8210,7 +8213,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>79</v>
@@ -8536,7 +8539,7 @@
         <v>79</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>117</v>
@@ -9188,7 +9191,7 @@
         <v>117</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I28" s="5" t="s">
         <v>86</v>
@@ -9508,7 +9511,7 @@
         <v>79</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>81</v>
@@ -9840,7 +9843,7 @@
         <v>79</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K30" s="5" t="str">
         <f>INT(LEFT(E30,1))</f>
@@ -10148,7 +10151,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>79</v>
@@ -10803,7 +10806,7 @@
         <v>79</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I33" s="5" t="s">
         <v>79</v>
@@ -11120,7 +11123,7 @@
         <v>79</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>137</v>
@@ -12729,10 +12732,10 @@
         <v>77</v>
       </c>
       <c r="D39" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>79</v>
+        <v>142</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>79</v>
@@ -13055,7 +13058,7 @@
         <v>1</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>79</v>
@@ -13393,7 +13396,7 @@
         <v>79</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K41" s="5" t="str">
         <f>INT(LEFT(E41,1))</f>
@@ -13707,7 +13710,7 @@
         <v>79</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>81</v>
@@ -14670,7 +14673,7 @@
         <v>1</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>79</v>
@@ -15959,13 +15962,13 @@
         <v>77</v>
       </c>
       <c r="D49" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>142</v>
+        <v>160</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>80</v>
@@ -16276,7 +16279,7 @@
         <v>47</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>77</v>
@@ -16599,7 +16602,7 @@
         <v>48</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>77</v>
@@ -16608,7 +16611,7 @@
         <v>1</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>79</v>
@@ -16922,7 +16925,7 @@
         <v>49</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>77</v>
@@ -16931,7 +16934,7 @@
         <v>2</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>79</v>
@@ -17245,7 +17248,7 @@
         <v>50</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>77</v>
@@ -17257,7 +17260,7 @@
         <v>79</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>101</v>
@@ -17568,7 +17571,7 @@
         <v>51</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>77</v>
@@ -17891,7 +17894,7 @@
         <v>52</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>77</v>
@@ -17900,7 +17903,7 @@
         <v>1</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>79</v>
@@ -18214,7 +18217,7 @@
         <v>53</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>77</v>
@@ -18223,7 +18226,7 @@
         <v>5</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>79</v>
@@ -18537,7 +18540,7 @@
         <v>54</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>77</v>
@@ -18549,7 +18552,7 @@
         <v>79</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>93</v>
@@ -18672,7 +18675,7 @@
         <f>FLOOR(AS57/8,1)&amp;"."&amp;FLOOR(MOD(AS57,8),1)&amp;"."&amp;(MOD(AS57,8)-FLOOR(MOD(AS57,8),1))*60</f>
       </c>
       <c r="AU57" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AV57" s="5" t="s">
         <v>83</v>
@@ -18860,7 +18863,7 @@
         <v>55</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>77</v>
@@ -19183,7 +19186,7 @@
         <v>56</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>77</v>
@@ -19506,7 +19509,7 @@
         <v>57</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>77</v>
@@ -19829,7 +19832,7 @@
         <v>58</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>77</v>

</xml_diff>

<commit_message>
made the border of the headers fat like me
</commit_message>
<xml_diff>
--- a/exceltocsv/public/reports/DTRSUMMARY.xlsx
+++ b/exceltocsv/public/reports/DTRSUMMARY.xlsx
@@ -630,16 +630,16 @@
       </bottom>
     </border>
     <border>
-      <left style="thin">
+      <left style="thick">
         <color rgb="00000000"/>
       </left>
-      <right style="thin">
+      <right style="thick">
         <color rgb="00000000"/>
       </right>
-      <top style="thin">
+      <top style="thick">
         <color rgb="00000000"/>
       </top>
-      <bottom style="thin">
+      <bottom style="thick">
         <color rgb="00000000"/>
       </bottom>
     </border>

</xml_diff>

<commit_message>
Fixed to_string methods and edited loading screen
</commit_message>
<xml_diff>
--- a/exceltocsv/public/reports/DTRSUMMARY.xlsx
+++ b/exceltocsv/public/reports/DTRSUMMARY.xlsx
@@ -9,9 +9,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="187" xml:space="preserve">
-  <si>
-    <t>iRipple, Inc. | DTR Summary Sheet for the period April 04, 2015 to April 24, 2015</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="184" xml:space="preserve">
+  <si>
+    <t>iRipple, Inc. | DTR Summary Sheet for the period April 25, 2015 to May 08, 2015</t>
   </si>
   <si>
     <t>Employee Information</t>
@@ -245,313 +245,304 @@
     <t>Barter Local - Support</t>
   </si>
   <si>
+    <t>0.4.3</t>
+  </si>
+  <si>
+    <t>0.0.0</t>
+  </si>
+  <si>
+    <t>2.4.0</t>
+  </si>
+  <si>
+    <t>7.4.0</t>
+  </si>
+  <si>
+    <t>Arceo,Arwin</t>
+  </si>
+  <si>
+    <t>International Business - Malaysia</t>
+  </si>
+  <si>
+    <t>9.0.0</t>
+  </si>
+  <si>
+    <t>6.4.0</t>
+  </si>
+  <si>
+    <t>0.5.0</t>
+  </si>
+  <si>
+    <t>Ardamoy,Ma. Rica Catherine</t>
+  </si>
+  <si>
+    <t>Enterprise - Petron</t>
+  </si>
+  <si>
+    <t>5.0.0</t>
+  </si>
+  <si>
+    <t>Bacani,Eddie Marie</t>
+  </si>
+  <si>
+    <t>International Business - Thailand</t>
+  </si>
+  <si>
+    <t>0.1.15</t>
+  </si>
+  <si>
+    <t>Balingit,Barbara</t>
+  </si>
+  <si>
+    <t>HR &amp;amp; Admin</t>
+  </si>
+  <si>
+    <t>Balino,Kamille Diane</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Barrion,Jane Katherine</t>
+  </si>
+  <si>
+    <t>0.0.3</t>
+  </si>
+  <si>
+    <t>1.4.0</t>
+  </si>
+  <si>
+    <t>Bayogos,Charmaine</t>
+  </si>
+  <si>
+    <t>Enterprise - Ayagold</t>
+  </si>
+  <si>
+    <t>2.0.0</t>
+  </si>
+  <si>
+    <t>Borlagdan,Aldrin</t>
+  </si>
+  <si>
+    <t>ATVI</t>
+  </si>
+  <si>
     <t>0.4.0</t>
   </si>
   <si>
-    <t>0.0.0</t>
+    <t>Buena,Ian Christopher</t>
+  </si>
+  <si>
+    <t>0.1.0</t>
+  </si>
+  <si>
+    <t>Buenafe,Rajiv</t>
+  </si>
+  <si>
+    <t>Cataluna,Christian Gilbert</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>CaÃ±ete,Carol Ann</t>
+  </si>
+  <si>
+    <t>0.0.45</t>
+  </si>
+  <si>
+    <t>Cerbo,Jaycer</t>
+  </si>
+  <si>
+    <t>Ching,Mark Angelo</t>
+  </si>
+  <si>
+    <t>Imaghine</t>
+  </si>
+  <si>
+    <t>0.3.0</t>
+  </si>
+  <si>
+    <t>6.0.0</t>
+  </si>
+  <si>
+    <t>Cortez,Jomar</t>
+  </si>
+  <si>
+    <t>Cruz,Cesar</t>
+  </si>
+  <si>
+    <t>7.0.0</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>Delfin,Jonathan</t>
+  </si>
+  <si>
+    <t>International Business - PNG</t>
+  </si>
+  <si>
+    <t>0.0.15</t>
+  </si>
+  <si>
+    <t>0.2.0</t>
+  </si>
+  <si>
+    <t>0.7.0</t>
+  </si>
+  <si>
+    <t>Dino,Arvin</t>
+  </si>
+  <si>
+    <t>8.0.0</t>
+  </si>
+  <si>
+    <t>Dy,Hubert</t>
+  </si>
+  <si>
+    <t>Executive</t>
+  </si>
+  <si>
+    <t>Egamino,Ellen</t>
+  </si>
+  <si>
+    <t>0.1.3</t>
+  </si>
+  <si>
+    <t>Enrique,Christian Dan</t>
+  </si>
+  <si>
+    <t>Barter Local - Project</t>
+  </si>
+  <si>
+    <t>Espiritu,Carl Philip</t>
+  </si>
+  <si>
+    <t>0.3.45</t>
+  </si>
+  <si>
+    <t>Flores,Arianne Grace</t>
+  </si>
+  <si>
+    <t>4.4.0</t>
+  </si>
+  <si>
+    <t>Francisco,Roed Ronualdo </t>
+  </si>
+  <si>
+    <t>Javier,Victor </t>
+  </si>
+  <si>
+    <t>3.0.0</t>
+  </si>
+  <si>
+    <t>Joson,Alfonso Miguel</t>
+  </si>
+  <si>
+    <t>0.1.45</t>
+  </si>
+  <si>
+    <t>Keng,Julie</t>
+  </si>
+  <si>
+    <t>8.4.0</t>
+  </si>
+  <si>
+    <t>Laude,Ted Marty</t>
+  </si>
+  <si>
+    <t>Ledesma,Jesse</t>
+  </si>
+  <si>
+    <t>Mangundayao,Mac Donald</t>
+  </si>
+  <si>
+    <t>Barter CX</t>
+  </si>
+  <si>
+    <t>0.2.15</t>
+  </si>
+  <si>
+    <t>0.6.0</t>
+  </si>
+  <si>
+    <t>Matias,Ma. Jeremia Jetheth </t>
+  </si>
+  <si>
+    <t>0.4.15</t>
+  </si>
+  <si>
+    <t>Mendoza,Diana</t>
+  </si>
+  <si>
+    <t>Nagnal,Fracy</t>
+  </si>
+  <si>
+    <t>Newsom,Jifferson</t>
+  </si>
+  <si>
+    <t>3.4.0</t>
+  </si>
+  <si>
+    <t>Pancho,Jona</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>Pechuanging,Ma. Antoinette</t>
+  </si>
+  <si>
+    <t>Pendre,Contessa</t>
+  </si>
+  <si>
+    <t>Ranes,Jonathan</t>
   </si>
   <si>
     <t>4.0.0</t>
   </si>
   <si>
-    <t>7.4.0</t>
-  </si>
-  <si>
-    <t>Arceo,Arwin</t>
-  </si>
-  <si>
-    <t>International Business - Malaysia</t>
-  </si>
-  <si>
-    <t>6.4.0</t>
-  </si>
-  <si>
-    <t>Ardamoy,Ma. Rica Catherine</t>
-  </si>
-  <si>
-    <t>Enterprise - Petron</t>
-  </si>
-  <si>
-    <t>0.1.15</t>
-  </si>
-  <si>
-    <t>1.0.0</t>
-  </si>
-  <si>
-    <t>2.4.0</t>
-  </si>
-  <si>
-    <t>0.2.0</t>
-  </si>
-  <si>
-    <t>0.1.0</t>
-  </si>
-  <si>
-    <t>Bacani,Eddie Marie</t>
-  </si>
-  <si>
-    <t>International Business - Thailand</t>
-  </si>
-  <si>
-    <t>Balingit,Barbara</t>
-  </si>
-  <si>
-    <t>HR &amp;amp; Admin</t>
-  </si>
-  <si>
-    <t>1.4.0</t>
-  </si>
-  <si>
-    <t>Balino,Kamille Diane</t>
-  </si>
-  <si>
-    <t>Product</t>
-  </si>
-  <si>
-    <t>12.0.0</t>
-  </si>
-  <si>
-    <t>Barrion,Jane Katherine</t>
-  </si>
-  <si>
-    <t>Bayogos,Charmaine</t>
-  </si>
-  <si>
-    <t>Enterprise - Ayagold</t>
-  </si>
-  <si>
-    <t>2.0.0</t>
-  </si>
-  <si>
-    <t>Borlagdan,Aldrin</t>
-  </si>
-  <si>
-    <t>ATVI</t>
-  </si>
-  <si>
-    <t>Buena,Ian Christopher</t>
-  </si>
-  <si>
-    <t>0.1.45</t>
-  </si>
-  <si>
-    <t>0.0.3</t>
-  </si>
-  <si>
-    <t>7.0.0</t>
-  </si>
-  <si>
-    <t>Buenafe,Rajiv</t>
-  </si>
-  <si>
-    <t>14.0.0</t>
-  </si>
-  <si>
-    <t>Cataluna,Christian Gilbert</t>
-  </si>
-  <si>
-    <t>Sales</t>
-  </si>
-  <si>
-    <t>6.0.0</t>
-  </si>
-  <si>
-    <t>CaÃ±ete,Carol Ann</t>
-  </si>
-  <si>
-    <t>0.2.15</t>
-  </si>
-  <si>
-    <t>Cerbo,Jaycer</t>
-  </si>
-  <si>
-    <t>Ching,Mark Angelo</t>
-  </si>
-  <si>
-    <t>Imaghine</t>
+    <t>Reyes,Mark Gil</t>
+  </si>
+  <si>
+    <t>5.4.0</t>
+  </si>
+  <si>
+    <t>Reyes,Salvador</t>
+  </si>
+  <si>
+    <t>1.2.0</t>
+  </si>
+  <si>
+    <t>Sanoria,Samuel</t>
+  </si>
+  <si>
+    <t>Santos,Patricia</t>
   </si>
   <si>
     <t>0.2.45</t>
   </si>
   <si>
-    <t>0.1.3</t>
-  </si>
-  <si>
-    <t>9.0.0</t>
-  </si>
-  <si>
-    <t>Cortez,Jomar</t>
-  </si>
-  <si>
-    <t>0.0.45</t>
-  </si>
-  <si>
-    <t>Cruz,Cesar</t>
-  </si>
-  <si>
-    <t>3.4.0</t>
-  </si>
-  <si>
-    <t>Delfin,Jonathan</t>
-  </si>
-  <si>
-    <t>International Business - PNG</t>
-  </si>
-  <si>
-    <t>Dino,Arvin</t>
-  </si>
-  <si>
-    <t>0.3.0</t>
-  </si>
-  <si>
-    <t>11.4.0</t>
-  </si>
-  <si>
-    <t>Dy,Hubert</t>
-  </si>
-  <si>
-    <t>Executive</t>
-  </si>
-  <si>
-    <t>Egamino,Ellen</t>
-  </si>
-  <si>
-    <t>8.4.0</t>
-  </si>
-  <si>
-    <t>Enrique,Christian Dan</t>
-  </si>
-  <si>
-    <t>Barter Local - Project</t>
-  </si>
-  <si>
-    <t>3.0.0</t>
-  </si>
-  <si>
-    <t>Espiritu,Carl Philip</t>
-  </si>
-  <si>
-    <t>0.7.0</t>
-  </si>
-  <si>
-    <t>Flores,Arianne Grace</t>
-  </si>
-  <si>
-    <t>Francisco,Roed Ronualdo </t>
-  </si>
-  <si>
-    <t>Javier,Victor </t>
-  </si>
-  <si>
-    <t>4.4.0</t>
-  </si>
-  <si>
-    <t>Joson,Alfonso Miguel</t>
-  </si>
-  <si>
-    <t>Keng,Julie</t>
-  </si>
-  <si>
-    <t>11.0.0</t>
-  </si>
-  <si>
-    <t>Laude,Ted Marty</t>
-  </si>
-  <si>
-    <t>Ledesma,Jesse</t>
-  </si>
-  <si>
-    <t>9.4.0</t>
-  </si>
-  <si>
-    <t>Mangundayao,Mac Donald</t>
-  </si>
-  <si>
-    <t>Barter CX</t>
+    <t>See,Jenilyn</t>
+  </si>
+  <si>
+    <t>Solbita,Felmar</t>
+  </si>
+  <si>
+    <t>Enterprise - Primer</t>
+  </si>
+  <si>
+    <t>Soriano,Josif Hans</t>
+  </si>
+  <si>
+    <t>0.3.3</t>
+  </si>
+  <si>
+    <t>Suarez,Katrina </t>
   </si>
   <si>
     <t>0.2.3</t>
-  </si>
-  <si>
-    <t>3.6.0</t>
-  </si>
-  <si>
-    <t>0.4.15</t>
-  </si>
-  <si>
-    <t>Matias,Ma. Jeremia Jetheth </t>
-  </si>
-  <si>
-    <t>0.3.15</t>
-  </si>
-  <si>
-    <t>Mendoza,Diana</t>
-  </si>
-  <si>
-    <t>1.1.3</t>
-  </si>
-  <si>
-    <t>Nagnal,Fracy</t>
-  </si>
-  <si>
-    <t>Newsom,Jifferson</t>
-  </si>
-  <si>
-    <t>Pancho,Jona</t>
-  </si>
-  <si>
-    <t>Finance</t>
-  </si>
-  <si>
-    <t>Pechuanging,Ma. Antoinette</t>
-  </si>
-  <si>
-    <t>Pendre,Contessa</t>
-  </si>
-  <si>
-    <t>Ranes,Jonathan</t>
-  </si>
-  <si>
-    <t>Reyes,Mark Gil</t>
-  </si>
-  <si>
-    <t>5.4.0</t>
-  </si>
-  <si>
-    <t>1.6.0</t>
-  </si>
-  <si>
-    <t>Reyes,Salvador</t>
-  </si>
-  <si>
-    <t>Sanoria,Samuel</t>
-  </si>
-  <si>
-    <t>Santos,Patricia</t>
-  </si>
-  <si>
-    <t>See,Jenilyn</t>
-  </si>
-  <si>
-    <t>0.0.15</t>
-  </si>
-  <si>
-    <t>Solbita,Felmar</t>
-  </si>
-  <si>
-    <t>Enterprise - Primer</t>
-  </si>
-  <si>
-    <t>Soriano,Josif Hans</t>
-  </si>
-  <si>
-    <t>0.6.0</t>
-  </si>
-  <si>
-    <t>Suarez,Katrina </t>
-  </si>
-  <si>
-    <t>1.2.0</t>
   </si>
   <si>
     <t>Tanqueco,Mikee Dorina</t>
@@ -1797,7 +1788,7 @@
         <v>79</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>81</v>
@@ -1806,7 +1797,7 @@
         <v>79</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K5" s="5" t="str">
         <f>INT(LEFT(E5,2))</f>
@@ -1920,7 +1911,7 @@
         <v>79</v>
       </c>
       <c r="AV5" s="5" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="AW5" s="5" t="s">
         <v>79</v>
@@ -2105,31 +2096,31 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J6" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>81</v>
       </c>
       <c r="K6" s="5" t="str">
         <f>INT(LEFT(E6,2))</f>
@@ -2240,13 +2231,13 @@
         <f>FLOOR(AS6/8,1)&amp;"."&amp;FLOOR(MOD(AS6,8),1)&amp;"."&amp;(MOD(AS6,8)-FLOOR(MOD(AS6,8),1))*60</f>
       </c>
       <c r="AU6" s="5" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AV6" s="5" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="AW6" s="5" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="AX6" s="5" t="s">
         <v>79</v>
@@ -2428,22 +2419,22 @@
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D7" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>79</v>
-      </c>
       <c r="F7" s="5" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>81</v>
@@ -2751,10 +2742,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>95</v>
       </c>
       <c r="D8" s="5" t="n">
         <v>0</v>
@@ -2763,10 +2754,10 @@
         <v>79</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>81</v>
@@ -3074,10 +3065,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D9" s="5" t="n">
         <v>0</v>
@@ -3086,10 +3077,10 @@
         <v>79</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>81</v>
@@ -3397,22 +3388,22 @@
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D10" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>81</v>
@@ -3720,10 +3711,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>102</v>
       </c>
       <c r="D11" s="5" t="n">
         <v>0</v>
@@ -3735,7 +3726,7 @@
         <v>79</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>81</v>
@@ -4043,22 +4034,22 @@
         <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="D12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="D12" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>79</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>81</v>
@@ -4369,19 +4360,19 @@
         <v>106</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D13" s="5" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>107</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>81</v>
@@ -4689,7 +4680,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>83</v>
@@ -4704,7 +4695,7 @@
         <v>79</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>81</v>
@@ -5012,10 +5003,10 @@
         <v>12</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D15" s="5" t="n">
         <v>0</v>
@@ -5027,7 +5018,7 @@
         <v>79</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>81</v>
@@ -5335,22 +5326,22 @@
         <v>13</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D16" s="5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>81</v>
@@ -5658,22 +5649,22 @@
         <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D17" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>81</v>
@@ -5981,22 +5972,22 @@
         <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D18" s="5" t="n">
         <v>2</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>81</v>
@@ -6304,22 +6295,22 @@
         <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D19" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>81</v>
@@ -6627,28 +6618,28 @@
         <v>17</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D20" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>81</v>
@@ -6950,22 +6941,22 @@
         <v>18</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D21" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>79</v>
+        <v>124</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>81</v>
@@ -7085,7 +7076,7 @@
         <f>FLOOR(AS21/8,1)&amp;"."&amp;FLOOR(MOD(AS21,8),1)&amp;"."&amp;(MOD(AS21,8)-FLOOR(MOD(AS21,8),1))*60</f>
       </c>
       <c r="AU21" s="5" t="s">
-        <v>79</v>
+        <v>125</v>
       </c>
       <c r="AV21" s="5" t="s">
         <v>79</v>
@@ -7100,7 +7091,7 @@
         <v>79</v>
       </c>
       <c r="AZ21" s="5" t="s">
-        <v>88</v>
+        <v>126</v>
       </c>
       <c r="BA21" s="5" t="s">
         <v>79</v>
@@ -7273,10 +7264,10 @@
         <v>19</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D22" s="5" t="n">
         <v>0</v>
@@ -7285,10 +7276,10 @@
         <v>79</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>81</v>
@@ -7596,10 +7587,10 @@
         <v>20</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D23" s="5" t="n">
         <v>0</v>
@@ -7608,10 +7599,10 @@
         <v>79</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>126</v>
+        <v>89</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>81</v>
@@ -7919,7 +7910,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>77</v>
@@ -7928,13 +7919,13 @@
         <v>2</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>81</v>
@@ -8242,10 +8233,10 @@
         <v>22</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D25" s="5" t="n">
         <v>0</v>
@@ -8254,10 +8245,10 @@
         <v>79</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>91</v>
+        <v>132</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>138</v>
+        <v>105</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>81</v>
@@ -8565,25 +8556,25 @@
         <v>23</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D26" s="5" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>79</v>
@@ -8888,31 +8879,31 @@
         <v>24</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D27" s="5" t="n">
         <v>3</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>81</v>
+        <v>117</v>
       </c>
       <c r="I27" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J27" s="5" t="s">
         <v>138</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>81</v>
       </c>
       <c r="K27" s="5" t="str">
         <f>INT(LEFT(E27,2))</f>
@@ -9026,7 +9017,7 @@
         <v>79</v>
       </c>
       <c r="AV27" s="5" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="AW27" s="5" t="s">
         <v>79</v>
@@ -9038,7 +9029,7 @@
         <v>79</v>
       </c>
       <c r="AZ27" s="5" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="BA27" s="5" t="s">
         <v>79</v>
@@ -9211,22 +9202,22 @@
         <v>25</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D28" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="H28" s="5" t="s">
         <v>81</v>
@@ -9534,10 +9525,10 @@
         <v>26</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D29" s="5" t="n">
         <v>0</v>
@@ -9546,10 +9537,10 @@
         <v>79</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>81</v>
@@ -9857,22 +9848,22 @@
         <v>27</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>83</v>
       </c>
       <c r="D30" s="5" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>81</v>
@@ -9992,7 +9983,7 @@
         <f>FLOOR(AS30/8,1)&amp;"."&amp;FLOOR(MOD(AS30,8),1)&amp;"."&amp;(MOD(AS30,8)-FLOOR(MOD(AS30,8),1))*60</f>
       </c>
       <c r="AU30" s="5" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="AV30" s="5" t="s">
         <v>79</v>
@@ -10180,10 +10171,10 @@
         <v>28</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D31" s="5" t="n">
         <v>0</v>
@@ -10192,10 +10183,10 @@
         <v>79</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>81</v>
@@ -10503,28 +10494,28 @@
         <v>29</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>83</v>
       </c>
       <c r="D32" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>79</v>
+        <v>124</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>81</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="J32" s="5" t="s">
         <v>81</v>
@@ -10826,22 +10817,22 @@
         <v>30</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D33" s="5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>81</v>
@@ -10976,10 +10967,10 @@
         <v>79</v>
       </c>
       <c r="AZ33" s="5" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="BA33" s="5" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="BB33" s="5" t="s">
         <v>79</v>
@@ -11149,22 +11140,22 @@
         <v>31</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D34" s="5" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>153</v>
+        <v>116</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>79</v>
+        <v>150</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>81</v>
@@ -11284,13 +11275,13 @@
         <f>FLOOR(AS34/8,1)&amp;"."&amp;FLOOR(MOD(AS34,8),1)&amp;"."&amp;(MOD(AS34,8)-FLOOR(MOD(AS34,8),1))*60</f>
       </c>
       <c r="AU34" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="AV34" s="5" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="AW34" s="5" t="s">
-        <v>155</v>
+        <v>79</v>
       </c>
       <c r="AX34" s="5" t="s">
         <v>79</v>
@@ -11472,22 +11463,22 @@
         <v>32</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D35" s="5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>124</v>
+        <v>79</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>138</v>
+        <v>102</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>81</v>
@@ -11795,22 +11786,22 @@
         <v>33</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D36" s="5" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>159</v>
+        <v>136</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="H36" s="5" t="s">
         <v>81</v>
@@ -12118,7 +12109,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>83</v>
@@ -12130,10 +12121,10 @@
         <v>79</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>79</v>
+        <v>124</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>135</v>
+        <v>99</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>81</v>
@@ -12441,10 +12432,10 @@
         <v>35</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D38" s="5" t="n">
         <v>0</v>
@@ -12456,7 +12447,7 @@
         <v>79</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>78</v>
+        <v>157</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>81</v>
@@ -12576,7 +12567,7 @@
         <f>FLOOR(AS38/8,1)&amp;"."&amp;FLOOR(MOD(AS38,8),1)&amp;"."&amp;(MOD(AS38,8)-FLOOR(MOD(AS38,8),1))*60</f>
       </c>
       <c r="AU38" s="5" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="AV38" s="5" t="s">
         <v>79</v>
@@ -12591,10 +12582,10 @@
         <v>79</v>
       </c>
       <c r="AZ38" s="5" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="BA38" s="5" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="BB38" s="5" t="s">
         <v>79</v>
@@ -12764,22 +12755,22 @@
         <v>36</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D39" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>81</v>
@@ -13087,10 +13078,10 @@
         <v>37</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D40" s="5" t="n">
         <v>0</v>
@@ -13102,7 +13093,7 @@
         <v>79</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>81</v>
@@ -13410,10 +13401,10 @@
         <v>38</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D41" s="5" t="n">
         <v>0</v>
@@ -13422,10 +13413,10 @@
         <v>79</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>81</v>
@@ -13733,22 +13724,22 @@
         <v>39</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D42" s="5" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>109</v>
+        <v>163</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>81</v>
@@ -14056,25 +14047,25 @@
         <v>40</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D43" s="5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>168</v>
+        <v>105</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>81</v>
+        <v>165</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>79</v>
@@ -14191,10 +14182,10 @@
         <f>FLOOR(AS43/8,1)&amp;"."&amp;FLOOR(MOD(AS43,8),1)&amp;"."&amp;(MOD(AS43,8)-FLOOR(MOD(AS43,8),1))*60</f>
       </c>
       <c r="AU43" s="5" t="s">
-        <v>169</v>
+        <v>79</v>
       </c>
       <c r="AV43" s="5" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="AW43" s="5" t="s">
         <v>79</v>
@@ -14379,22 +14370,22 @@
         <v>41</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D44" s="5" t="n">
         <v>4</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="H44" s="5" t="s">
         <v>81</v>
@@ -14514,7 +14505,7 @@
         <f>FLOOR(AS44/8,1)&amp;"."&amp;FLOOR(MOD(AS44,8),1)&amp;"."&amp;(MOD(AS44,8)-FLOOR(MOD(AS44,8),1))*60</f>
       </c>
       <c r="AU44" s="5" t="s">
-        <v>79</v>
+        <v>167</v>
       </c>
       <c r="AV44" s="5" t="s">
         <v>79</v>
@@ -14523,7 +14514,7 @@
         <v>79</v>
       </c>
       <c r="AX44" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AY44" s="5" t="s">
         <v>79</v>
@@ -14702,22 +14693,22 @@
         <v>42</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D45" s="5" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>138</v>
+        <v>102</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>81</v>
@@ -15025,22 +15016,22 @@
         <v>43</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D46" s="5" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>108</v>
+        <v>170</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>79</v>
+        <v>132</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>147</v>
+        <v>102</v>
       </c>
       <c r="H46" s="5" t="s">
         <v>81</v>
@@ -15163,10 +15154,10 @@
         <v>79</v>
       </c>
       <c r="AV46" s="5" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="AW46" s="5" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="AX46" s="5" t="s">
         <v>79</v>
@@ -15348,7 +15339,7 @@
         <v>44</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>77</v>
@@ -15360,10 +15351,10 @@
         <v>79</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>174</v>
+        <v>79</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>81</v>
@@ -15671,22 +15662,22 @@
         <v>45</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D48" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>81</v>
@@ -15994,22 +15985,22 @@
         <v>46</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D49" s="5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>107</v>
+        <v>175</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>124</v>
+        <v>79</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>81</v>
@@ -16132,7 +16123,7 @@
         <v>79</v>
       </c>
       <c r="AV49" s="5" t="s">
-        <v>178</v>
+        <v>79</v>
       </c>
       <c r="AW49" s="5" t="s">
         <v>79</v>
@@ -16317,31 +16308,31 @@
         <v>47</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D50" s="5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="H50" s="5" t="s">
         <v>81</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>81</v>
+        <v>165</v>
       </c>
       <c r="K50" s="5" t="str">
         <f>INT(LEFT(E50,2))</f>
@@ -16452,7 +16443,7 @@
         <f>FLOOR(AS50/8,1)&amp;"."&amp;FLOOR(MOD(AS50,8),1)&amp;"."&amp;(MOD(AS50,8)-FLOOR(MOD(AS50,8),1))*60</f>
       </c>
       <c r="AU50" s="5" t="s">
-        <v>180</v>
+        <v>79</v>
       </c>
       <c r="AV50" s="5" t="s">
         <v>79</v>
@@ -16467,7 +16458,7 @@
         <v>79</v>
       </c>
       <c r="AZ50" s="5" t="s">
-        <v>140</v>
+        <v>79</v>
       </c>
       <c r="BA50" s="5" t="s">
         <v>79</v>
@@ -16640,10 +16631,10 @@
         <v>48</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D51" s="5" t="n">
         <v>0</v>
@@ -16655,7 +16646,7 @@
         <v>79</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>78</v>
+        <v>121</v>
       </c>
       <c r="H51" s="5" t="s">
         <v>81</v>
@@ -16963,10 +16954,10 @@
         <v>49</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D52" s="5" t="n">
         <v>0</v>
@@ -16975,10 +16966,10 @@
         <v>79</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>174</v>
+        <v>79</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="H52" s="5" t="s">
         <v>81</v>
@@ -17286,10 +17277,10 @@
         <v>50</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D53" s="5" t="n">
         <v>0</v>
@@ -17301,7 +17292,7 @@
         <v>79</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>81</v>
@@ -17609,10 +17600,10 @@
         <v>51</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D54" s="5" t="n">
         <v>0</v>
@@ -17624,7 +17615,7 @@
         <v>79</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>80</v>
+        <v>157</v>
       </c>
       <c r="H54" s="5" t="s">
         <v>81</v>
@@ -17932,10 +17923,10 @@
         <v>52</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D55" s="5" t="n">
         <v>0</v>
@@ -17944,10 +17935,10 @@
         <v>79</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>126</v>
+        <v>80</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
Fixed biometrics import error
</commit_message>
<xml_diff>
--- a/exceltocsv/public/reports/DTRSUMMARY.xlsx
+++ b/exceltocsv/public/reports/DTRSUMMARY.xlsx
@@ -245,7 +245,7 @@
     <t>Barter Local - Support</t>
   </si>
   <si>
-    <t>0.4.3</t>
+    <t>0.4.30</t>
   </si>
   <si>
     <t>0.0.0</t>
@@ -305,7 +305,7 @@
     <t>Barrion,Jane Katherine</t>
   </si>
   <si>
-    <t>0.0.3</t>
+    <t>0.0.30</t>
   </si>
   <si>
     <t>1.4.0</t>
@@ -407,7 +407,7 @@
     <t>Egamino,Ellen</t>
   </si>
   <si>
-    <t>0.1.3</t>
+    <t>0.1.30</t>
   </si>
   <si>
     <t>Enrique,Christian Dan</t>
@@ -536,13 +536,13 @@
     <t>Soriano,Josif Hans</t>
   </si>
   <si>
-    <t>0.3.3</t>
+    <t>0.3.30</t>
   </si>
   <si>
     <t>Suarez,Katrina </t>
   </si>
   <si>
-    <t>0.2.3</t>
+    <t>0.2.30</t>
   </si>
   <si>
     <t>Tanqueco,Mikee Dorina</t>

</xml_diff>

<commit_message>
Fixed format time error and deleted some unnecessary comments
</commit_message>
<xml_diff>
--- a/exceltocsv/public/reports/DTRSUMMARY.xlsx
+++ b/exceltocsv/public/reports/DTRSUMMARY.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="187" xml:space="preserve">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="186" xml:space="preserve">
   <si>
     <t>iRipple, Inc. | DTR Summary Sheet for the period April 25, 2015 to May 08, 2015</t>
   </si>
@@ -290,6 +290,9 @@
     <t>International Business - Thailand</t>
   </si>
   <si>
+    <t>0.1.45</t>
+  </si>
+  <si>
     <t>Balingit,Barbara</t>
   </si>
   <si>
@@ -371,6 +374,9 @@
     <t>0.2.0</t>
   </si>
   <si>
+    <t>0.1.30</t>
+  </si>
+  <si>
     <t>6.0.0</t>
   </si>
   <si>
@@ -416,9 +422,6 @@
     <t>Barter Local - Project</t>
   </si>
   <si>
-    <t>0.1.30</t>
-  </si>
-  <si>
     <t>Espiritu,Carl Philip</t>
   </si>
   <si>
@@ -446,7 +449,7 @@
     <t>Joson,Alfonso Miguel</t>
   </si>
   <si>
-    <t>0.1.45</t>
+    <t>0.2.45</t>
   </si>
   <si>
     <t>Keng,Julie</t>
@@ -465,9 +468,6 @@
   </si>
   <si>
     <t>Barter CX</t>
-  </si>
-  <si>
-    <t>0.2.45</t>
   </si>
   <si>
     <t>0.6.0</t>
@@ -500,7 +500,7 @@
     <t>Finance</t>
   </si>
   <si>
-    <t>0.5.15</t>
+    <t>0.5.45</t>
   </si>
   <si>
     <t>Pechuanging,Ma. Antoinette</t>
@@ -510,6 +510,9 @@
   </si>
   <si>
     <t>Ranes,Jonathan</t>
+  </si>
+  <si>
+    <t>0.2.30</t>
   </si>
   <si>
     <t>4.0.0</t>
@@ -522,9 +525,6 @@
   </si>
   <si>
     <t>Reyes,Salvador</t>
-  </si>
-  <si>
-    <t>0.3.30</t>
   </si>
   <si>
     <t>1.2.0</t>
@@ -549,9 +549,6 @@
   </si>
   <si>
     <t>Suarez,Katrina </t>
-  </si>
-  <si>
-    <t>0.2.30</t>
   </si>
   <si>
     <t>Tanqueco,Mikee Dorina</t>
@@ -2440,7 +2437,7 @@
         <v>84</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>79</v>
@@ -2751,10 +2748,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D8" s="5" t="n">
         <v>0</v>
@@ -3074,16 +3071,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D9" s="5" t="n">
         <v>2</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>79</v>
@@ -3397,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>92</v>
@@ -3406,13 +3403,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>81</v>
@@ -3720,10 +3717,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D11" s="5" t="n">
         <v>0</v>
@@ -3735,7 +3732,7 @@
         <v>79</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>81</v>
@@ -4043,7 +4040,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>89</v>
@@ -4052,7 +4049,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>79</v>
@@ -4366,10 +4363,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D13" s="5" t="n">
         <v>0</v>
@@ -4381,7 +4378,7 @@
         <v>79</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>81</v>
@@ -4689,16 +4686,16 @@
         <v>11</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D14" s="5" t="n">
         <v>2</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>79</v>
@@ -5012,7 +5009,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>83</v>
@@ -5027,7 +5024,7 @@
         <v>79</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>81</v>
@@ -5335,10 +5332,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D16" s="5" t="n">
         <v>0</v>
@@ -5658,22 +5655,22 @@
         <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D17" s="5" t="n">
         <v>2</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>81</v>
@@ -5981,10 +5978,10 @@
         <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D18" s="5" t="n">
         <v>0</v>
@@ -6304,22 +6301,22 @@
         <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D19" s="5" t="n">
         <v>2</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>81</v>
@@ -6627,7 +6624,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>77</v>
@@ -6636,7 +6633,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>79</v>
@@ -6950,28 +6947,28 @@
         <v>18</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D21" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>81</v>
@@ -7273,16 +7270,16 @@
         <v>19</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D22" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>79</v>
@@ -7408,7 +7405,7 @@
         <f>FLOOR(AS22/8,1)&amp;"."&amp;FLOOR(MOD(AS22,8),1)&amp;"."&amp;(MOD(AS22,8)-FLOOR(MOD(AS22,8),1))*60</f>
       </c>
       <c r="AU22" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AV22" s="5" t="s">
         <v>79</v>
@@ -7423,7 +7420,7 @@
         <v>79</v>
       </c>
       <c r="AZ22" s="5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="BA22" s="5" t="s">
         <v>79</v>
@@ -7596,10 +7593,10 @@
         <v>20</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D23" s="5" t="n">
         <v>0</v>
@@ -7608,10 +7605,10 @@
         <v>79</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>81</v>
@@ -7919,10 +7916,10 @@
         <v>21</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D24" s="5" t="n">
         <v>0</v>
@@ -7931,7 +7928,7 @@
         <v>79</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>90</v>
@@ -8242,7 +8239,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>77</v>
@@ -8257,7 +8254,7 @@
         <v>79</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>81</v>
@@ -8565,10 +8562,10 @@
         <v>23</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D26" s="5" t="n">
         <v>0</v>
@@ -8577,10 +8574,10 @@
         <v>79</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H26" s="5" t="s">
         <v>81</v>
@@ -8888,22 +8885,22 @@
         <v>24</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D27" s="5" t="n">
         <v>7</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>86</v>
@@ -9211,10 +9208,10 @@
         <v>25</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D28" s="5" t="n">
         <v>0</v>
@@ -9226,7 +9223,7 @@
         <v>79</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H28" s="5" t="s">
         <v>81</v>
@@ -9534,7 +9531,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>89</v>
@@ -9543,16 +9540,16 @@
         <v>3</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>79</v>
@@ -9857,22 +9854,22 @@
         <v>27</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D30" s="5" t="n">
         <v>2</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>81</v>
@@ -10180,10 +10177,10 @@
         <v>28</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D31" s="5" t="n">
         <v>0</v>
@@ -10192,10 +10189,10 @@
         <v>79</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>81</v>
@@ -10503,7 +10500,7 @@
         <v>29</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>83</v>
@@ -10512,13 +10509,13 @@
         <v>7</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>81</v>
@@ -10826,10 +10823,10 @@
         <v>30</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D33" s="5" t="n">
         <v>0</v>
@@ -10841,7 +10838,7 @@
         <v>79</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>81</v>
@@ -11149,7 +11146,7 @@
         <v>31</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>83</v>
@@ -11158,19 +11155,19 @@
         <v>1</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>81</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="J34" s="5" t="s">
         <v>81</v>
@@ -11472,22 +11469,22 @@
         <v>32</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D35" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>147</v>
+        <v>85</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>81</v>
@@ -11795,22 +11792,22 @@
         <v>33</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D36" s="5" t="n">
         <v>5</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="H36" s="5" t="s">
         <v>81</v>
@@ -12121,7 +12118,7 @@
         <v>154</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D37" s="5" t="n">
         <v>7</v>
@@ -12133,7 +12130,7 @@
         <v>79</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>81</v>
@@ -12444,19 +12441,19 @@
         <v>156</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D38" s="5" t="n">
         <v>6</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>81</v>
@@ -12776,10 +12773,10 @@
         <v>79</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>81</v>
@@ -13090,7 +13087,7 @@
         <v>158</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D40" s="5" t="n">
         <v>0</v>
@@ -13413,7 +13410,7 @@
         <v>160</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D41" s="5" t="n">
         <v>0</v>
@@ -13425,7 +13422,7 @@
         <v>79</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>81</v>
@@ -13748,7 +13745,7 @@
         <v>79</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>81</v>
@@ -14382,7 +14379,7 @@
         <v>165</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D44" s="5" t="n">
         <v>0</v>
@@ -14705,19 +14702,19 @@
         <v>166</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D45" s="5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>129</v>
+        <v>167</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>84</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>81</v>
@@ -15025,25 +15022,25 @@
         <v>43</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D46" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I46" s="5" t="s">
         <v>79</v>
@@ -15348,22 +15345,22 @@
         <v>44</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D47" s="5" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>78</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>81</v>
@@ -15674,7 +15671,7 @@
         <v>173</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D48" s="5" t="n">
         <v>0</v>
@@ -15686,7 +15683,7 @@
         <v>79</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>81</v>
@@ -16003,13 +16000,13 @@
         <v>6</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>81</v>
@@ -16332,7 +16329,7 @@
         <v>79</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H50" s="5" t="s">
         <v>81</v>
@@ -16649,10 +16646,10 @@
         <v>1</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>79</v>
@@ -16966,19 +16963,19 @@
         <v>178</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D52" s="5" t="n">
         <v>4</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H52" s="5" t="s">
         <v>81</v>
@@ -17289,19 +17286,19 @@
         <v>179</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D53" s="5" t="n">
         <v>4</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>81</v>
@@ -17310,7 +17307,7 @@
         <v>79</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K53" s="5" t="str">
         <f>INT(LEFT(E53,2))</f>
@@ -17609,10 +17606,10 @@
         <v>51</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D54" s="5" t="n">
         <v>0</v>
@@ -17624,7 +17621,7 @@
         <v>79</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="H54" s="5" t="s">
         <v>81</v>
@@ -17932,7 +17929,7 @@
         <v>52</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>89</v>
@@ -18255,10 +18252,10 @@
         <v>53</v>
       </c>
       <c r="B56" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>183</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>184</v>
       </c>
       <c r="D56" s="5" t="n">
         <v>0</v>
@@ -18270,7 +18267,7 @@
         <v>79</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H56" s="5" t="s">
         <v>81</v>
@@ -18578,7 +18575,7 @@
         <v>54</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>89</v>
@@ -18590,7 +18587,7 @@
         <v>79</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>159</v>
@@ -18901,10 +18898,10 @@
         <v>55</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D58" s="5" t="n">
         <v>0</v>
@@ -18913,7 +18910,7 @@
         <v>79</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
fixed excel files formatting
</commit_message>
<xml_diff>
--- a/exceltocsv/public/reports/DTRSUMMARY.xlsx
+++ b/exceltocsv/public/reports/DTRSUMMARY.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="187" xml:space="preserve">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="175" xml:space="preserve">
   <si>
     <t>iRipple, Inc. | DTR Summary Sheet for the period April 25, 2015 to May 08, 2015</t>
   </si>
@@ -227,7 +227,7 @@
     <t>TOTAL</t>
   </si>
   <si>
-    <t>"Gatan, Jr.",Mario Haris</t>
+    <t>"Gatan, Jr.", Mario Haris</t>
   </si>
   <si>
     <t>Barter Local - Support</t>
@@ -236,7 +236,7 @@
     <t>0.4.30</t>
   </si>
   <si>
-    <t>0.4.45</t>
+    <t>0.2.0</t>
   </si>
   <si>
     <t>0.0.0</t>
@@ -245,13 +245,19 @@
     <t>7.4.0</t>
   </si>
   <si>
-    <t>Arceo,Arwin</t>
+    <t>Arceo, Arwin</t>
   </si>
   <si>
     <t>International Business - Malaysia</t>
   </si>
   <si>
-    <t>1.0.30</t>
+    <t>0.1.15</t>
+  </si>
+  <si>
+    <t>0.4.0</t>
+  </si>
+  <si>
+    <t>1.4.0</t>
   </si>
   <si>
     <t>6.4.0</t>
@@ -260,7 +266,7 @@
     <t>0.5.0</t>
   </si>
   <si>
-    <t>Ardamoy,Ma. Rica Catherine</t>
+    <t>Ardamoy, Ma. Rica Catherine</t>
   </si>
   <si>
     <t>Enterprise - Petron</t>
@@ -269,25 +275,22 @@
     <t>5.0.0</t>
   </si>
   <si>
-    <t>Bacani,Eddie Marie</t>
+    <t>Bacani, Eddie Marie</t>
   </si>
   <si>
     <t>International Business - Thailand</t>
   </si>
   <si>
-    <t>0.1.15</t>
-  </si>
-  <si>
     <t>0.1.45</t>
   </si>
   <si>
-    <t>Balingit,Barbara</t>
+    <t>Balingit, Barbara</t>
   </si>
   <si>
     <t>HR &amp;amp; Admin</t>
   </si>
   <si>
-    <t>Balino,Kamille Diane</t>
+    <t>Balino, Kamille Diane</t>
   </si>
   <si>
     <t>Product</t>
@@ -296,82 +299,64 @@
     <t>0.0.30</t>
   </si>
   <si>
-    <t>Barrion,Jane Katherine</t>
-  </si>
-  <si>
-    <t>1.4.0</t>
-  </si>
-  <si>
-    <t>Bayogos,Charmaine</t>
+    <t>Barrion, Jane Katherine</t>
+  </si>
+  <si>
+    <t>Bayogos, Charmaine</t>
   </si>
   <si>
     <t>Enterprise - Ayagold</t>
   </si>
   <si>
-    <t>Bernardo,Gianilla Mae</t>
+    <t>Bernardo, Gianilla Mae</t>
   </si>
   <si>
     <t>0.0.15</t>
   </si>
   <si>
-    <t>Borlagdan,Aldrin</t>
+    <t>Borlagdan, Aldrin</t>
   </si>
   <si>
     <t>ATVI</t>
   </si>
   <si>
-    <t>0.4.0</t>
-  </si>
-  <si>
-    <t>Buena,Ian Christopher</t>
+    <t>Buena, Ian Christopher</t>
   </si>
   <si>
     <t>0.1.0</t>
   </si>
   <si>
-    <t>2.1.15</t>
-  </si>
-  <si>
-    <t>Buenafe,Rajiv</t>
-  </si>
-  <si>
-    <t>Cataluna,Christian Gilbert</t>
+    <t>Buenafe, Rajiv</t>
+  </si>
+  <si>
+    <t>Cataluna, Christian Gilbert</t>
   </si>
   <si>
     <t>Sales</t>
   </si>
   <si>
-    <t>CaÃ±ete,Carol Ann</t>
+    <t>CaÃ±ete, Carol Ann</t>
   </si>
   <si>
     <t>0.0.45</t>
   </si>
   <si>
-    <t>Cerbo,Jaycer</t>
-  </si>
-  <si>
-    <t>Ching,Mark Angelo</t>
+    <t>Cerbo, Jaycer</t>
+  </si>
+  <si>
+    <t>Ching, Mark Angelo</t>
   </si>
   <si>
     <t>Imaghine</t>
   </si>
   <si>
-    <t>0.2.0</t>
-  </si>
-  <si>
-    <t>2.2.0</t>
-  </si>
-  <si>
-    <t>Cortez,Jomar</t>
-  </si>
-  <si>
-    <t>1.0.45</t>
-  </si>
-  <si>
-    <t>Cruz,Cesar</t>
-  </si>
-  <si>
-    <t>0.3.30</t>
+    <t>0.1.30</t>
+  </si>
+  <si>
+    <t>Cortez, Jomar</t>
+  </si>
+  <si>
+    <t>Cruz, Cesar</t>
   </si>
   <si>
     <t>7.0.0</t>
@@ -380,7 +365,7 @@
     <t>1.0.0</t>
   </si>
   <si>
-    <t>Delfin,Jonathan</t>
+    <t>Delfin, Jonathan</t>
   </si>
   <si>
     <t>International Business - PNG</t>
@@ -389,43 +374,40 @@
     <t>0.7.0</t>
   </si>
   <si>
-    <t>Dino,Arvin</t>
-  </si>
-  <si>
-    <t>1.2.30</t>
-  </si>
-  <si>
-    <t>Dy,Hubert</t>
+    <t>Dino, Arvin</t>
+  </si>
+  <si>
+    <t>0.2.15</t>
+  </si>
+  <si>
+    <t>Dy, Hubert</t>
   </si>
   <si>
     <t>Executive</t>
   </si>
   <si>
-    <t>Egamino,Ellen</t>
-  </si>
-  <si>
-    <t>Enrique,Christian Dan</t>
+    <t>Egamino, Ellen</t>
+  </si>
+  <si>
+    <t>Enrique, Christian Dan</t>
   </si>
   <si>
     <t>Barter Local - Project</t>
   </si>
   <si>
-    <t>0.1.30</t>
-  </si>
-  <si>
-    <t>Espiritu,Carl Philip</t>
+    <t>Espiritu, Carl Philip</t>
   </si>
   <si>
     <t>0.3.45</t>
   </si>
   <si>
-    <t>Fadrilan,Liezl</t>
+    <t>Fadrilan, Liezl</t>
   </si>
   <si>
     <t>Synext (Nexus)</t>
   </si>
   <si>
-    <t>Flores,Arianne Grace</t>
+    <t>Flores, Arianne Grace</t>
   </si>
   <si>
     <t>6.0.0</t>
@@ -434,64 +416,55 @@
     <t>4.4.0</t>
   </si>
   <si>
-    <t>Francisco,Roed Ronualdo </t>
-  </si>
-  <si>
-    <t>Javier,Victor </t>
-  </si>
-  <si>
-    <t>Joson,Alfonso Miguel</t>
+    <t>Francisco, Roed Ronualdo </t>
+  </si>
+  <si>
+    <t>Javier, Victor </t>
+  </si>
+  <si>
+    <t>Joson, Alfonso Miguel</t>
   </si>
   <si>
     <t>0.2.45</t>
   </si>
   <si>
-    <t>Keng,Julie</t>
-  </si>
-  <si>
-    <t>Laude,Ted Marty</t>
-  </si>
-  <si>
-    <t>0.2.15</t>
-  </si>
-  <si>
-    <t>Ledesma,Jesse</t>
-  </si>
-  <si>
-    <t>Mangundayao,Mac Donald</t>
+    <t>Keng, Julie</t>
+  </si>
+  <si>
+    <t>Laude, Ted Marty</t>
+  </si>
+  <si>
+    <t>Ledesma, Jesse</t>
+  </si>
+  <si>
+    <t>Mangundayao, Mac Donald</t>
   </si>
   <si>
     <t>Barter CX</t>
   </si>
   <si>
-    <t>2.0.0</t>
-  </si>
-  <si>
     <t>0.6.0</t>
   </si>
   <si>
-    <t>Matias,Ma. Jeremia Jetheth </t>
+    <t>Matias, Ma. Jeremia Jetheth </t>
   </si>
   <si>
     <t>0.4.15</t>
   </si>
   <si>
-    <t>Mendoza,Diana</t>
-  </si>
-  <si>
-    <t>1.1.30</t>
-  </si>
-  <si>
-    <t>Nagnal,Fracy</t>
-  </si>
-  <si>
-    <t>Newsom,Jifferson</t>
-  </si>
-  <si>
-    <t>Pajo,Maricel</t>
-  </si>
-  <si>
-    <t>Pancho,Jona</t>
+    <t>Mendoza, Diana</t>
+  </si>
+  <si>
+    <t>Nagnal, Fracy</t>
+  </si>
+  <si>
+    <t>Newsom, Jifferson</t>
+  </si>
+  <si>
+    <t>Pajo, Maricel</t>
+  </si>
+  <si>
+    <t>Pancho, Jona</t>
   </si>
   <si>
     <t>Finance</t>
@@ -500,76 +473,67 @@
     <t>0.5.45</t>
   </si>
   <si>
-    <t>Pechuanging,Ma. Antoinette</t>
-  </si>
-  <si>
-    <t>Pendre,Contessa</t>
-  </si>
-  <si>
-    <t>Ranes,Jonathan</t>
+    <t>Pechuanging, Ma. Antoinette</t>
+  </si>
+  <si>
+    <t>Pendre, Contessa</t>
+  </si>
+  <si>
+    <t>Ranes, Jonathan</t>
   </si>
   <si>
     <t>0.2.30</t>
   </si>
   <si>
-    <t>Reyes,Mark Gil</t>
-  </si>
-  <si>
-    <t>0.3.0</t>
+    <t>Reyes, Mark Gil</t>
   </si>
   <si>
     <t>5.4.0</t>
   </si>
   <si>
-    <t>Reyes,Salvador</t>
+    <t>Reyes, Salvador</t>
   </si>
   <si>
     <t>1.2.0</t>
   </si>
   <si>
-    <t>Sanoria,Samuel</t>
-  </si>
-  <si>
-    <t>2.5.15</t>
-  </si>
-  <si>
-    <t>Santos,Patricia</t>
-  </si>
-  <si>
-    <t>See,Jenilyn</t>
-  </si>
-  <si>
-    <t>Solbita,Felmar</t>
+    <t>Sanoria, Samuel</t>
+  </si>
+  <si>
+    <t>Santos, Patricia</t>
+  </si>
+  <si>
+    <t>See, Jenilyn</t>
+  </si>
+  <si>
+    <t>Solbita, Felmar</t>
   </si>
   <si>
     <t>Enterprise - Primer</t>
   </si>
   <si>
-    <t>Soriano,Josif Hans</t>
-  </si>
-  <si>
-    <t>Suarez,Katrina </t>
-  </si>
-  <si>
-    <t>Tanqueco,Mikee Dorina</t>
-  </si>
-  <si>
-    <t>1.6.30</t>
-  </si>
-  <si>
-    <t>Tesoro,Rose Natalie</t>
-  </si>
-  <si>
-    <t>Unson,Mary Anne</t>
+    <t>Soriano, Josif Hans</t>
+  </si>
+  <si>
+    <t>Suarez, Katrina </t>
+  </si>
+  <si>
+    <t>Tanqueco, Mikee Dorina</t>
+  </si>
+  <si>
+    <t>Tesoro, Rose Natalie</t>
+  </si>
+  <si>
+    <t>Unson, Mary Anne</t>
   </si>
   <si>
     <t>Marketing &amp;amp; Hardware</t>
   </si>
   <si>
-    <t>Viloria,Eizell</t>
-  </si>
-  <si>
-    <t>Viloria,Benito Jr.</t>
+    <t>Viloria, Eizell</t>
+  </si>
+  <si>
+    <t>Viloria, Benito Jr.</t>
   </si>
 </sst>
 </file>
@@ -1557,16 +1521,16 @@
         <v>80</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>77</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K5" s="5" t="str">
         <f>INT(LEFT(E5,2))</f>
@@ -1680,13 +1644,13 @@
         <v>76</v>
       </c>
       <c r="AV5" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AW5" s="5" t="s">
         <v>76</v>
       </c>
       <c r="AX5" s="5" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AY5" s="5" t="s">
         <v>76</v>
@@ -1793,10 +1757,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>0</v>
@@ -1817,7 +1781,7 @@
         <v>76</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="K6" s="5" t="str">
         <f>INT(LEFT(E6,2))</f>
@@ -2044,19 +2008,19 @@
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D7" s="5" t="n">
         <v>2</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>76</v>
@@ -2295,10 +2259,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D8" s="5" t="n">
         <v>0</v>
@@ -2546,16 +2510,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D9" s="5" t="n">
         <v>2</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>76</v>
@@ -2797,22 +2761,22 @@
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D10" s="5" t="n">
         <v>2</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>76</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>77</v>
@@ -3063,7 +3027,7 @@
         <v>76</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>77</v>
@@ -3302,7 +3266,7 @@
         <v>99</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D12" s="5" t="n">
         <v>1</v>
@@ -3562,7 +3526,7 @@
         <v>76</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>76</v>
@@ -3801,7 +3765,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>102</v>
@@ -3810,10 +3774,10 @@
         <v>2</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>76</v>
@@ -4052,7 +4016,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>79</v>
@@ -4303,10 +4267,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D16" s="5" t="n">
         <v>0</v>
@@ -4554,16 +4518,16 @@
         <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D17" s="5" t="n">
         <v>2</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>76</v>
@@ -4805,10 +4769,10 @@
         <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D18" s="5" t="n">
         <v>0</v>
@@ -5056,19 +5020,19 @@
         <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D19" s="5" t="n">
         <v>2</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>76</v>
@@ -5307,7 +5271,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>73</v>
@@ -5316,10 +5280,10 @@
         <v>1</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>118</v>
+        <v>76</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>76</v>
@@ -5558,28 +5522,28 @@
         <v>18</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D21" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>120</v>
+        <v>76</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>77</v>
@@ -5809,10 +5773,10 @@
         <v>19</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D22" s="5" t="n">
         <v>1</v>
@@ -5944,7 +5908,7 @@
         <f>FLOOR(AS22/8,1)&amp;"."&amp;FLOOR(MOD(AS22,8),1)&amp;"."&amp;(MOD(AS22,8)-FLOOR(MOD(AS22,8),1))*60</f>
       </c>
       <c r="AU22" s="5" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="AV22" s="5" t="s">
         <v>76</v>
@@ -5953,7 +5917,7 @@
         <v>76</v>
       </c>
       <c r="AX22" s="5" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="AY22" s="5" t="s">
         <v>76</v>
@@ -6060,7 +6024,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>102</v>
@@ -6072,7 +6036,7 @@
         <v>76</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>76</v>
@@ -6311,10 +6275,10 @@
         <v>21</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D24" s="5" t="n">
         <v>0</v>
@@ -6323,7 +6287,7 @@
         <v>76</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>76</v>
@@ -6562,7 +6526,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>73</v>
@@ -6571,7 +6535,7 @@
         <v>2</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>76</v>
@@ -6813,10 +6777,10 @@
         <v>23</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D26" s="5" t="n">
         <v>0</v>
@@ -6825,7 +6789,7 @@
         <v>76</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>133</v>
+        <v>76</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>76</v>
@@ -7064,25 +7028,25 @@
         <v>24</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D27" s="5" t="n">
         <v>7</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>76</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>76</v>
@@ -7315,10 +7279,10 @@
         <v>25</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D28" s="5" t="n">
         <v>0</v>
@@ -7566,31 +7530,31 @@
         <v>26</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D29" s="5" t="n">
         <v>3</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>76</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>76</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="K29" s="5" t="str">
         <f>INT(LEFT(E29,2))</f>
@@ -7817,16 +7781,16 @@
         <v>27</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D30" s="5" t="n">
         <v>2</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>76</v>
@@ -8068,10 +8032,10 @@
         <v>28</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D31" s="5" t="n">
         <v>0</v>
@@ -8080,7 +8044,7 @@
         <v>76</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>76</v>
@@ -8319,7 +8283,7 @@
         <v>29</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>79</v>
@@ -8328,10 +8292,10 @@
         <v>7</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>76</v>
@@ -8454,7 +8418,7 @@
         <f>FLOOR(AS32/8,1)&amp;"."&amp;FLOOR(MOD(AS32,8),1)&amp;"."&amp;(MOD(AS32,8)-FLOOR(MOD(AS32,8),1))*60</f>
       </c>
       <c r="AU32" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AV32" s="5" t="s">
         <v>76</v>
@@ -8570,10 +8534,10 @@
         <v>30</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D33" s="5" t="n">
         <v>0</v>
@@ -8821,7 +8785,7 @@
         <v>31</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>79</v>
@@ -8833,7 +8797,7 @@
         <v>100</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>147</v>
+        <v>76</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>76</v>
@@ -8842,7 +8806,7 @@
         <v>77</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="J34" s="5" t="s">
         <v>77</v>
@@ -9072,7 +9036,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>73</v>
@@ -9081,7 +9045,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>76</v>
@@ -9323,19 +9287,19 @@
         <v>33</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D36" s="5" t="n">
         <v>5</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>151</v>
+        <v>122</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>76</v>
@@ -9458,7 +9422,7 @@
         <f>FLOOR(AS36/8,1)&amp;"."&amp;FLOOR(MOD(AS36,8),1)&amp;"."&amp;(MOD(AS36,8)-FLOOR(MOD(AS36,8),1))*60</f>
       </c>
       <c r="AU36" s="5" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="AV36" s="5" t="s">
         <v>76</v>
@@ -9574,7 +9538,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>102</v>
@@ -9583,7 +9547,7 @@
         <v>7</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>76</v>
@@ -9825,19 +9789,19 @@
         <v>35</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D38" s="5" t="n">
         <v>6</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>156</v>
+        <v>76</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>76</v>
@@ -10076,7 +10040,7 @@
         <v>36</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>79</v>
@@ -10088,7 +10052,7 @@
         <v>76</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>76</v>
@@ -10327,10 +10291,10 @@
         <v>37</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D40" s="5" t="n">
         <v>0</v>
@@ -10578,7 +10542,7 @@
         <v>38</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>102</v>
@@ -10829,16 +10793,16 @@
         <v>39</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="D42" s="5" t="n">
         <v>8</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>76</v>
@@ -11080,10 +11044,10 @@
         <v>40</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="D43" s="5" t="n">
         <v>0</v>
@@ -11331,7 +11295,7 @@
         <v>41</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>102</v>
@@ -11343,7 +11307,7 @@
         <v>76</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>76</v>
@@ -11582,7 +11546,7 @@
         <v>42</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>102</v>
@@ -11591,10 +11555,10 @@
         <v>5</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>76</v>
@@ -11833,25 +11797,25 @@
         <v>43</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D46" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>168</v>
+        <v>76</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>76</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="I46" s="5" t="s">
         <v>76</v>
@@ -12084,7 +12048,7 @@
         <v>44</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>98</v>
@@ -12093,10 +12057,10 @@
         <v>7</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>76</v>
@@ -12219,7 +12183,7 @@
         <f>FLOOR(AS47/8,1)&amp;"."&amp;FLOOR(MOD(AS47,8),1)&amp;"."&amp;(MOD(AS47,8)-FLOOR(MOD(AS47,8),1))*60</f>
       </c>
       <c r="AU47" s="5" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="AV47" s="5" t="s">
         <v>76</v>
@@ -12335,10 +12299,10 @@
         <v>45</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D48" s="5" t="n">
         <v>0</v>
@@ -12347,7 +12311,7 @@
         <v>76</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>173</v>
+        <v>76</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>76</v>
@@ -12586,7 +12550,7 @@
         <v>46</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>73</v>
@@ -12595,10 +12559,10 @@
         <v>6</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>76</v>
@@ -12837,7 +12801,7 @@
         <v>47</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>73</v>
@@ -13088,19 +13052,19 @@
         <v>48</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="D51" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>76</v>
@@ -13339,19 +13303,19 @@
         <v>49</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D52" s="5" t="n">
         <v>4</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>168</v>
+        <v>76</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>76</v>
@@ -13590,7 +13554,7 @@
         <v>50</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>98</v>
@@ -13599,13 +13563,13 @@
         <v>4</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>147</v>
+        <v>76</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>77</v>
@@ -13614,7 +13578,7 @@
         <v>76</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="K53" s="5" t="str">
         <f>INT(LEFT(E53,2))</f>
@@ -13841,10 +13805,10 @@
         <v>51</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D54" s="5" t="n">
         <v>0</v>
@@ -13853,7 +13817,7 @@
         <v>76</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>181</v>
+        <v>76</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>76</v>
@@ -14092,10 +14056,10 @@
         <v>52</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D55" s="5" t="n">
         <v>0</v>
@@ -14343,10 +14307,10 @@
         <v>53</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="D56" s="5" t="n">
         <v>0</v>
@@ -14594,10 +14558,10 @@
         <v>54</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D57" s="5" t="n">
         <v>0</v>
@@ -14606,7 +14570,7 @@
         <v>76</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>76</v>
@@ -14845,10 +14809,10 @@
         <v>55</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D58" s="5" t="n">
         <v>0</v>
@@ -14857,7 +14821,7 @@
         <v>76</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
fixed excel file error
</commit_message>
<xml_diff>
--- a/exceltocsv/public/reports/DTRSUMMARY.xlsx
+++ b/exceltocsv/public/reports/DTRSUMMARY.xlsx
@@ -9,9 +9,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="179" xml:space="preserve">
-  <si>
-    <t>iRipple, Inc. | DTR Summary Sheet for the period March 21, 2015 to April 03, 2015</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="185" xml:space="preserve">
+  <si>
+    <t>iRipple, Inc. | DTR Summary Sheet for the period April 25, 2015 to May 08, 2015</t>
   </si>
   <si>
     <t>Employee Information</t>
@@ -257,289 +257,307 @@
     <t>0.0.0</t>
   </si>
   <si>
+    <t>0.1.15</t>
+  </si>
+  <si>
     <t>7.4.0</t>
   </si>
   <si>
+    <t>6.4.0</t>
+  </si>
+  <si>
+    <t>0.5.0</t>
+  </si>
+  <si>
+    <t>4.4.0</t>
+  </si>
+  <si>
     <t>Ardamoy, Ma. Rica Catherine</t>
   </si>
   <si>
     <t>Enterprise - Petron</t>
   </si>
   <si>
+    <t>Bacani, Eddie Marie</t>
+  </si>
+  <si>
+    <t>International Business - Thailand</t>
+  </si>
+  <si>
+    <t>0.1.45</t>
+  </si>
+  <si>
+    <t>Balingit, Barbara</t>
+  </si>
+  <si>
+    <t>HR &amp;amp; Admin</t>
+  </si>
+  <si>
+    <t>Balino, Kamille Diane</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>0.0.30</t>
+  </si>
+  <si>
+    <t>Barrion, Jane Katherine</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>0.4.0</t>
+  </si>
+  <si>
+    <t>Bayogos, Charmaine</t>
+  </si>
+  <si>
+    <t>Enterprise - Ayagold</t>
+  </si>
+  <si>
+    <t>Bernardo, Gianilla Mae</t>
+  </si>
+  <si>
     <t>0.0.15</t>
   </si>
   <si>
-    <t>0.4.0</t>
-  </si>
-  <si>
-    <t>Bacani, Eddie Marie</t>
-  </si>
-  <si>
-    <t>International Business - Thailand</t>
-  </si>
-  <si>
-    <t>Balingit, Barbara</t>
-  </si>
-  <si>
-    <t>HR &amp;amp; Admin</t>
-  </si>
-  <si>
-    <t>1.0.0</t>
-  </si>
-  <si>
-    <t>Balino, Kamille Diane</t>
-  </si>
-  <si>
-    <t>Product</t>
+    <t>Borlagdan, Aldrin</t>
+  </si>
+  <si>
+    <t>ATVI</t>
+  </si>
+  <si>
+    <t>Buena, Ian Christopher</t>
+  </si>
+  <si>
+    <t>0.1.0</t>
+  </si>
+  <si>
+    <t>5.0.0</t>
+  </si>
+  <si>
+    <t>Buenafe, Rajiv</t>
+  </si>
+  <si>
+    <t>9.0.0</t>
+  </si>
+  <si>
+    <t>Cataluna, Christian Gilbert</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>CaÃ±ete, Carol Ann</t>
   </si>
   <si>
     <t>0.0.45</t>
   </si>
   <si>
-    <t>Barrion, Jane Katherine</t>
-  </si>
-  <si>
-    <t>Bayogos, Charmaine</t>
-  </si>
-  <si>
-    <t>Enterprise - Ayagold</t>
-  </si>
-  <si>
-    <t>Borlagdan, Aldrin</t>
-  </si>
-  <si>
-    <t>ATVI</t>
-  </si>
-  <si>
-    <t>0.1.15</t>
-  </si>
-  <si>
-    <t>Buena, Ian Christopher</t>
-  </si>
-  <si>
-    <t>0.3.0</t>
+    <t>2.0.0</t>
+  </si>
+  <si>
+    <t>Cerbo, Jaycer</t>
+  </si>
+  <si>
+    <t>Ching, Mark Angelo</t>
+  </si>
+  <si>
+    <t>Imaghine</t>
+  </si>
+  <si>
+    <t>0.2.0</t>
+  </si>
+  <si>
+    <t>0.1.30</t>
+  </si>
+  <si>
+    <t>Cortez, Jomar</t>
+  </si>
+  <si>
+    <t>Barter Local - Support</t>
+  </si>
+  <si>
+    <t>2.4.0</t>
+  </si>
+  <si>
+    <t>Cruz, Cesar</t>
   </si>
   <si>
     <t>1.4.0</t>
   </si>
   <si>
-    <t>Buenafe, Rajiv</t>
+    <t>Delfin, Jonathan</t>
+  </si>
+  <si>
+    <t>International Business - PNG</t>
+  </si>
+  <si>
+    <t>0.7.0</t>
+  </si>
+  <si>
+    <t>Dino, Arvin</t>
+  </si>
+  <si>
+    <t>0.2.15</t>
+  </si>
+  <si>
+    <t>6.0.0</t>
+  </si>
+  <si>
+    <t>Dy, Hubert</t>
+  </si>
+  <si>
+    <t>Executive</t>
+  </si>
+  <si>
+    <t>Egamino, Ellen</t>
+  </si>
+  <si>
+    <t>Enrique, Christian Dan</t>
+  </si>
+  <si>
+    <t>Barter Local - Project</t>
+  </si>
+  <si>
+    <t>Espiritu, Carl Philip</t>
+  </si>
+  <si>
+    <t>0.3.45</t>
+  </si>
+  <si>
+    <t>Fadrilan, Liezl</t>
+  </si>
+  <si>
+    <t>Synext (Nexus)</t>
+  </si>
+  <si>
+    <t>Flores, Arianne Grace</t>
+  </si>
+  <si>
+    <t>Francisco, Roed Ronualdo </t>
+  </si>
+  <si>
+    <t>Javier, Victor </t>
+  </si>
+  <si>
+    <t>3.0.0</t>
+  </si>
+  <si>
+    <t>Joson, Alfonso Miguel</t>
+  </si>
+  <si>
+    <t>0.2.45</t>
+  </si>
+  <si>
+    <t>Keng, Julie</t>
+  </si>
+  <si>
+    <t>8.4.0</t>
+  </si>
+  <si>
+    <t>Laude, Ted Marty</t>
+  </si>
+  <si>
+    <t>Mangundayao, Mac Donald</t>
+  </si>
+  <si>
+    <t>Barter CX</t>
+  </si>
+  <si>
+    <t>0.6.0</t>
+  </si>
+  <si>
+    <t>Matias, Ma. Jeremia Jetheth </t>
+  </si>
+  <si>
+    <t>0.4.15</t>
+  </si>
+  <si>
+    <t>Mendoza, Diana</t>
+  </si>
+  <si>
+    <t>Nagnal, Fracy</t>
+  </si>
+  <si>
+    <t>Newsom, Jifferson</t>
+  </si>
+  <si>
+    <t>3.4.0</t>
+  </si>
+  <si>
+    <t>Pajo, Maricel</t>
+  </si>
+  <si>
+    <t>Pancho, Jona</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>0.5.45</t>
+  </si>
+  <si>
+    <t>Pechuanging, Ma. Antoinette</t>
+  </si>
+  <si>
+    <t>Pendre, Contessa</t>
+  </si>
+  <si>
+    <t>Ranes, Jonathan</t>
+  </si>
+  <si>
+    <t>0.2.30</t>
   </si>
   <si>
     <t>4.0.0</t>
   </si>
   <si>
-    <t>3.0.0</t>
-  </si>
-  <si>
-    <t>Cataluna, Christian Gilbert</t>
-  </si>
-  <si>
-    <t>Sales</t>
+    <t>Reyes, Mark Gil</t>
+  </si>
+  <si>
+    <t>Reyes, Salvador</t>
+  </si>
+  <si>
+    <t>1.2.0</t>
+  </si>
+  <si>
+    <t>Santos, Patricia</t>
+  </si>
+  <si>
+    <t>See, Jenilyn</t>
+  </si>
+  <si>
+    <t>Solbita, Felmar</t>
+  </si>
+  <si>
+    <t>Enterprise - Primer</t>
+  </si>
+  <si>
+    <t>Soriano, Josif Hans</t>
+  </si>
+  <si>
+    <t>1.1.0</t>
+  </si>
+  <si>
+    <t>Suarez, Katrina </t>
+  </si>
+  <si>
+    <t>5.4.0</t>
+  </si>
+  <si>
+    <t>Tesoro, Rose Natalie</t>
+  </si>
+  <si>
+    <t>Unson, Mary Anne</t>
+  </si>
+  <si>
+    <t>Marketing &amp;amp; Hardware</t>
   </si>
   <si>
     <t>8.0.0</t>
-  </si>
-  <si>
-    <t>CaÃ±ete, Carol Ann</t>
-  </si>
-  <si>
-    <t>0.1.0</t>
-  </si>
-  <si>
-    <t>2.4.0</t>
-  </si>
-  <si>
-    <t>Cerbo, Jaycer</t>
-  </si>
-  <si>
-    <t>Ching, Mark Angelo</t>
-  </si>
-  <si>
-    <t>Imaghine</t>
-  </si>
-  <si>
-    <t>0.5.0</t>
-  </si>
-  <si>
-    <t>3.4.0</t>
-  </si>
-  <si>
-    <t>Cortez, Jomar</t>
-  </si>
-  <si>
-    <t>Barter Local - Support</t>
-  </si>
-  <si>
-    <t>Cruz, Cesar</t>
-  </si>
-  <si>
-    <t>Delfin, Jonathan</t>
-  </si>
-  <si>
-    <t>International Business - PNG</t>
-  </si>
-  <si>
-    <t>0.2.0</t>
-  </si>
-  <si>
-    <t>Dino, Arvin</t>
-  </si>
-  <si>
-    <t>4.4.0</t>
-  </si>
-  <si>
-    <t>Dy, Hubert</t>
-  </si>
-  <si>
-    <t>Executive</t>
-  </si>
-  <si>
-    <t>Egamino, Ellen</t>
-  </si>
-  <si>
-    <t>0.1.45</t>
-  </si>
-  <si>
-    <t>0.7.0</t>
-  </si>
-  <si>
-    <t>Enrique, Christian Dan</t>
-  </si>
-  <si>
-    <t>Barter Local - Project</t>
-  </si>
-  <si>
-    <t>5.0.0</t>
-  </si>
-  <si>
-    <t>Espiritu, Carl Philip</t>
-  </si>
-  <si>
-    <t>1.3.0</t>
-  </si>
-  <si>
-    <t>Fadrilan, Liezl</t>
-  </si>
-  <si>
-    <t>Synext (Nexus)</t>
-  </si>
-  <si>
-    <t>Flores, Arianne Grace</t>
-  </si>
-  <si>
-    <t>1.7.0</t>
-  </si>
-  <si>
-    <t>Francisco, Roed Ronualdo </t>
-  </si>
-  <si>
-    <t>Javier, Victor </t>
-  </si>
-  <si>
-    <t>5.4.0</t>
-  </si>
-  <si>
-    <t>Joson, Alfonso Miguel</t>
-  </si>
-  <si>
-    <t>Keng, Julie</t>
-  </si>
-  <si>
-    <t>Laude, Ted Marty</t>
-  </si>
-  <si>
-    <t>Mangundayao, Mac Donald</t>
-  </si>
-  <si>
-    <t>Barter CX</t>
-  </si>
-  <si>
-    <t>0.0.30</t>
-  </si>
-  <si>
-    <t>Matias, Ma. Jeremia Jetheth </t>
-  </si>
-  <si>
-    <t>0.4.15</t>
-  </si>
-  <si>
-    <t>Mendoza, Diana</t>
-  </si>
-  <si>
-    <t>0.5.15</t>
-  </si>
-  <si>
-    <t>2.0.0</t>
-  </si>
-  <si>
-    <t>Nagnal, Fracy</t>
-  </si>
-  <si>
-    <t>Newsom, Jifferson</t>
-  </si>
-  <si>
-    <t>Pajo, Maricel</t>
-  </si>
-  <si>
-    <t>Pancho, Jona</t>
-  </si>
-  <si>
-    <t>Finance</t>
-  </si>
-  <si>
-    <t>Pechuanging, Ma. Antoinette</t>
-  </si>
-  <si>
-    <t>Pendre, Contessa</t>
-  </si>
-  <si>
-    <t>Ranes, Jonathan</t>
-  </si>
-  <si>
-    <t>0.1.30</t>
-  </si>
-  <si>
-    <t>Reyes, Mark Gil</t>
-  </si>
-  <si>
-    <t>Reyes, Salvador</t>
-  </si>
-  <si>
-    <t>2.3.0</t>
-  </si>
-  <si>
-    <t>Santos, Patricia</t>
-  </si>
-  <si>
-    <t>See, Jenilyn</t>
-  </si>
-  <si>
-    <t>Solbita, Felmar</t>
-  </si>
-  <si>
-    <t>Enterprise - Primer</t>
-  </si>
-  <si>
-    <t>1.1.0</t>
-  </si>
-  <si>
-    <t>Soriano, Josif Hans</t>
-  </si>
-  <si>
-    <t>Suarez, Katrina </t>
-  </si>
-  <si>
-    <t>1.6.0</t>
-  </si>
-  <si>
-    <t>Tesoro, Rose Natalie</t>
-  </si>
-  <si>
-    <t>Unson, Mary Anne</t>
-  </si>
-  <si>
-    <t>Marketing &amp;amp; Hardware</t>
   </si>
   <si>
     <t>Viloria, Benito Jr.</t>
@@ -662,7 +680,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:CK54"/>
+  <dimension ref="A1:CK55"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0">
       <pane topLeftCell="D4" state="frozenSplit" activePane="bottomRight" ySplit="3" xSplit="3"/>
@@ -1321,19 +1339,19 @@
         <v>81</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K4" s="5" t="str">
         <f>INT(LEFT(E4,2))</f>
@@ -1447,7 +1465,7 @@
         <v>81</v>
       </c>
       <c r="AV4" s="5" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="AW4" s="5" t="s">
         <v>81</v>
@@ -1552,10 +1570,10 @@
         <v>0</v>
       </c>
       <c r="CE4" s="5" t="str">
-        <f>FLOOR(CC4/8,1,1)&amp;"."&amp;FLOOR(MOD(CC4,8),1,1)&amp;"."&amp;(MOD(CC4,8)-FLOOR(MOD(CC4,8),1,1))*60</f>
+        <f>FLOOR(CC4/8,1)&amp;"."&amp;FLOOR(MOD(CC4,8),1)&amp;"."&amp;(MOD(CC4,8)-FLOOR(MOD(CC4,8),1))*60</f>
       </c>
       <c r="CF4" s="5" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="CG4" s="5" t="str">
         <f>INT(LEFT(CF4,2))</f>
@@ -1578,31 +1596,31 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="I5" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="D5" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="K5" s="5" t="str">
         <f>INT(LEFT(E5,2))</f>
@@ -1821,10 +1839,10 @@
         <v>0</v>
       </c>
       <c r="CE5" s="5" t="str">
-        <f>FLOOR(CC5/8,1,1)&amp;"."&amp;FLOOR(MOD(CC5,8),1,1)&amp;"."&amp;(MOD(CC5,8)-FLOOR(MOD(CC5,8),1,1))*60</f>
+        <f>FLOOR(CC5/8,1)&amp;"."&amp;FLOOR(MOD(CC5,8),1)&amp;"."&amp;(MOD(CC5,8)-FLOOR(MOD(CC5,8),1))*60</f>
       </c>
       <c r="CF5" s="5" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="CG5" s="5" t="str">
         <f>INT(LEFT(CF5,2))</f>
@@ -1847,31 +1865,31 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K6" s="5" t="str">
         <f>INT(LEFT(E6,2))</f>
@@ -2090,7 +2108,7 @@
         <v>0</v>
       </c>
       <c r="CE6" s="5" t="str">
-        <f>FLOOR(CC6/8,1,1)&amp;"."&amp;FLOOR(MOD(CC6,8),1,1)&amp;"."&amp;(MOD(CC6,8)-FLOOR(MOD(CC6,8),1,1))*60</f>
+        <f>FLOOR(CC6/8,1)&amp;"."&amp;FLOOR(MOD(CC6,8),1)&amp;"."&amp;(MOD(CC6,8)-FLOOR(MOD(CC6,8),1))*60</f>
       </c>
       <c r="CF6" s="5" t="s">
         <v>81</v>
@@ -2116,10 +2134,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D7" s="5" t="n">
         <v>0</v>
@@ -2134,13 +2152,13 @@
         <v>81</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K7" s="5" t="str">
         <f>INT(LEFT(E7,2))</f>
@@ -2359,10 +2377,10 @@
         <v>0</v>
       </c>
       <c r="CE7" s="5" t="str">
-        <f>FLOOR(CC7/8,1,1)&amp;"."&amp;FLOOR(MOD(CC7,8),1,1)&amp;"."&amp;(MOD(CC7,8)-FLOOR(MOD(CC7,8),1,1))*60</f>
+        <f>FLOOR(CC7/8,1)&amp;"."&amp;FLOOR(MOD(CC7,8),1)&amp;"."&amp;(MOD(CC7,8)-FLOOR(MOD(CC7,8),1))*60</f>
       </c>
       <c r="CF7" s="5" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="CG7" s="5" t="str">
         <f>INT(LEFT(CF7,2))</f>
@@ -2385,16 +2403,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D8" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>81</v>
@@ -2403,13 +2421,13 @@
         <v>81</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K8" s="5" t="str">
         <f>INT(LEFT(E8,2))</f>
@@ -2628,7 +2646,7 @@
         <v>0</v>
       </c>
       <c r="CE8" s="5" t="str">
-        <f>FLOOR(CC8/8,1,1)&amp;"."&amp;FLOOR(MOD(CC8,8),1,1)&amp;"."&amp;(MOD(CC8,8)-FLOOR(MOD(CC8,8),1,1))*60</f>
+        <f>FLOOR(CC8/8,1)&amp;"."&amp;FLOOR(MOD(CC8,8),1)&amp;"."&amp;(MOD(CC8,8)-FLOOR(MOD(CC8,8),1))*60</f>
       </c>
       <c r="CF8" s="5" t="s">
         <v>81</v>
@@ -2654,31 +2672,31 @@
         <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D9" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>81</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K9" s="5" t="str">
         <f>INT(LEFT(E9,2))</f>
@@ -2897,10 +2915,10 @@
         <v>0</v>
       </c>
       <c r="CE9" s="5" t="str">
-        <f>FLOOR(CC9/8,1,1)&amp;"."&amp;FLOOR(MOD(CC9,8),1,1)&amp;"."&amp;(MOD(CC9,8)-FLOOR(MOD(CC9,8),1,1))*60</f>
+        <f>FLOOR(CC9/8,1)&amp;"."&amp;FLOOR(MOD(CC9,8),1)&amp;"."&amp;(MOD(CC9,8)-FLOOR(MOD(CC9,8),1))*60</f>
       </c>
       <c r="CF9" s="5" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="CG9" s="5" t="str">
         <f>INT(LEFT(CF9,2))</f>
@@ -2923,10 +2941,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D10" s="5" t="n">
         <v>0</v>
@@ -2938,16 +2956,16 @@
         <v>81</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K10" s="5" t="str">
         <f>INT(LEFT(E10,2))</f>
@@ -3058,7 +3076,7 @@
         <f>FLOOR(AS10/8,1)&amp;"."&amp;FLOOR(MOD(AS10,8),1)&amp;"."&amp;(MOD(AS10,8)-FLOOR(MOD(AS10,8),1))*60</f>
       </c>
       <c r="AU10" s="5" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="AV10" s="5" t="s">
         <v>81</v>
@@ -3166,10 +3184,10 @@
         <v>0</v>
       </c>
       <c r="CE10" s="5" t="str">
-        <f>FLOOR(CC10/8,1,1)&amp;"."&amp;FLOOR(MOD(CC10,8),1,1)&amp;"."&amp;(MOD(CC10,8)-FLOOR(MOD(CC10,8),1,1))*60</f>
+        <f>FLOOR(CC10/8,1)&amp;"."&amp;FLOOR(MOD(CC10,8),1)&amp;"."&amp;(MOD(CC10,8)-FLOOR(MOD(CC10,8),1))*60</f>
       </c>
       <c r="CF10" s="5" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="CG10" s="5" t="str">
         <f>INT(LEFT(CF10,2))</f>
@@ -3192,31 +3210,31 @@
         <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="D11" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K11" s="5" t="str">
         <f>INT(LEFT(E11,2))</f>
@@ -3435,10 +3453,10 @@
         <v>0</v>
       </c>
       <c r="CE11" s="5" t="str">
-        <f>FLOOR(CC11/8,1,1)&amp;"."&amp;FLOOR(MOD(CC11,8),1,1)&amp;"."&amp;(MOD(CC11,8)-FLOOR(MOD(CC11,8),1,1))*60</f>
+        <f>FLOOR(CC11/8,1)&amp;"."&amp;FLOOR(MOD(CC11,8),1)&amp;"."&amp;(MOD(CC11,8)-FLOOR(MOD(CC11,8),1))*60</f>
       </c>
       <c r="CF11" s="5" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="CG11" s="5" t="str">
         <f>INT(LEFT(CF11,2))</f>
@@ -3461,31 +3479,31 @@
         <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D12" s="5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K12" s="5" t="str">
         <f>INT(LEFT(E12,2))</f>
@@ -3704,10 +3722,10 @@
         <v>0</v>
       </c>
       <c r="CE12" s="5" t="str">
-        <f>FLOOR(CC12/8,1,1)&amp;"."&amp;FLOOR(MOD(CC12,8),1,1)&amp;"."&amp;(MOD(CC12,8)-FLOOR(MOD(CC12,8),1,1))*60</f>
+        <f>FLOOR(CC12/8,1)&amp;"."&amp;FLOOR(MOD(CC12,8),1)&amp;"."&amp;(MOD(CC12,8)-FLOOR(MOD(CC12,8),1))*60</f>
       </c>
       <c r="CF12" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="CG12" s="5" t="str">
         <f>INT(LEFT(CF12,2))</f>
@@ -3730,16 +3748,16 @@
         <v>10</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>81</v>
@@ -3748,13 +3766,13 @@
         <v>81</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K13" s="5" t="str">
         <f>INT(LEFT(E13,2))</f>
@@ -3973,10 +3991,10 @@
         <v>0</v>
       </c>
       <c r="CE13" s="5" t="str">
-        <f>FLOOR(CC13/8,1,1)&amp;"."&amp;FLOOR(MOD(CC13,8),1,1)&amp;"."&amp;(MOD(CC13,8)-FLOOR(MOD(CC13,8),1,1))*60</f>
+        <f>FLOOR(CC13/8,1)&amp;"."&amp;FLOOR(MOD(CC13,8),1)&amp;"."&amp;(MOD(CC13,8)-FLOOR(MOD(CC13,8),1))*60</f>
       </c>
       <c r="CF13" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="CG13" s="5" t="str">
         <f>INT(LEFT(CF13,2))</f>
@@ -3999,10 +4017,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="D14" s="5" t="n">
         <v>0</v>
@@ -4017,13 +4035,13 @@
         <v>81</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K14" s="5" t="str">
         <f>INT(LEFT(E14,2))</f>
@@ -4242,10 +4260,10 @@
         <v>0</v>
       </c>
       <c r="CE14" s="5" t="str">
-        <f>FLOOR(CC14/8,1,1)&amp;"."&amp;FLOOR(MOD(CC14,8),1,1)&amp;"."&amp;(MOD(CC14,8)-FLOOR(MOD(CC14,8),1,1))*60</f>
+        <f>FLOOR(CC14/8,1)&amp;"."&amp;FLOOR(MOD(CC14,8),1)&amp;"."&amp;(MOD(CC14,8)-FLOOR(MOD(CC14,8),1))*60</f>
       </c>
       <c r="CF14" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="CG14" s="5" t="str">
         <f>INT(LEFT(CF14,2))</f>
@@ -4268,16 +4286,16 @@
         <v>12</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="D15" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>81</v>
@@ -4286,13 +4304,13 @@
         <v>81</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K15" s="5" t="str">
         <f>INT(LEFT(E15,2))</f>
@@ -4511,10 +4529,10 @@
         <v>0</v>
       </c>
       <c r="CE15" s="5" t="str">
-        <f>FLOOR(CC15/8,1,1)&amp;"."&amp;FLOOR(MOD(CC15,8),1,1)&amp;"."&amp;(MOD(CC15,8)-FLOOR(MOD(CC15,8),1,1))*60</f>
+        <f>FLOOR(CC15/8,1)&amp;"."&amp;FLOOR(MOD(CC15,8),1)&amp;"."&amp;(MOD(CC15,8)-FLOOR(MOD(CC15,8),1))*60</f>
       </c>
       <c r="CF15" s="5" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="CG15" s="5" t="str">
         <f>INT(LEFT(CF15,2))</f>
@@ -4543,25 +4561,25 @@
         <v>93</v>
       </c>
       <c r="D16" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>81</v>
+        <v>115</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K16" s="5" t="str">
         <f>INT(LEFT(E16,2))</f>
@@ -4780,7 +4798,7 @@
         <v>0</v>
       </c>
       <c r="CE16" s="5" t="str">
-        <f>FLOOR(CC16/8,1,1)&amp;"."&amp;FLOOR(MOD(CC16,8),1,1)&amp;"."&amp;(MOD(CC16,8)-FLOOR(MOD(CC16,8),1,1))*60</f>
+        <f>FLOOR(CC16/8,1)&amp;"."&amp;FLOOR(MOD(CC16,8),1)&amp;"."&amp;(MOD(CC16,8)-FLOOR(MOD(CC16,8),1))*60</f>
       </c>
       <c r="CF16" s="5" t="s">
         <v>81</v>
@@ -4806,10 +4824,10 @@
         <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="D17" s="5" t="n">
         <v>0</v>
@@ -4818,19 +4836,19 @@
         <v>81</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K17" s="5" t="str">
         <f>INT(LEFT(E17,2))</f>
@@ -5049,10 +5067,10 @@
         <v>0</v>
       </c>
       <c r="CE17" s="5" t="str">
-        <f>FLOOR(CC17/8,1,1)&amp;"."&amp;FLOOR(MOD(CC17,8),1,1)&amp;"."&amp;(MOD(CC17,8)-FLOOR(MOD(CC17,8),1,1))*60</f>
+        <f>FLOOR(CC17/8,1)&amp;"."&amp;FLOOR(MOD(CC17,8),1)&amp;"."&amp;(MOD(CC17,8)-FLOOR(MOD(CC17,8),1))*60</f>
       </c>
       <c r="CF17" s="5" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
       <c r="CG17" s="5" t="str">
         <f>INT(LEFT(CF17,2))</f>
@@ -5075,31 +5093,31 @@
         <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="D18" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D18" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>85</v>
-      </c>
       <c r="F18" s="5" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K18" s="5" t="str">
         <f>INT(LEFT(E18,2))</f>
@@ -5210,7 +5228,7 @@
         <f>FLOOR(AS18/8,1)&amp;"."&amp;FLOOR(MOD(AS18,8),1)&amp;"."&amp;(MOD(AS18,8)-FLOOR(MOD(AS18,8),1))*60</f>
       </c>
       <c r="AU18" s="5" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="AV18" s="5" t="s">
         <v>81</v>
@@ -5318,10 +5336,10 @@
         <v>0</v>
       </c>
       <c r="CE18" s="5" t="str">
-        <f>FLOOR(CC18/8,1,1)&amp;"."&amp;FLOOR(MOD(CC18,8),1,1)&amp;"."&amp;(MOD(CC18,8)-FLOOR(MOD(CC18,8),1,1))*60</f>
+        <f>FLOOR(CC18/8,1)&amp;"."&amp;FLOOR(MOD(CC18,8),1)&amp;"."&amp;(MOD(CC18,8)-FLOOR(MOD(CC18,8),1))*60</f>
       </c>
       <c r="CF18" s="5" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="CG18" s="5" t="str">
         <f>INT(LEFT(CF18,2))</f>
@@ -5344,16 +5362,16 @@
         <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>93</v>
+        <v>122</v>
       </c>
       <c r="D19" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>81</v>
@@ -5362,13 +5380,13 @@
         <v>81</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K19" s="5" t="str">
         <f>INT(LEFT(E19,2))</f>
@@ -5587,10 +5605,10 @@
         <v>0</v>
       </c>
       <c r="CE19" s="5" t="str">
-        <f>FLOOR(CC19/8,1,1)&amp;"."&amp;FLOOR(MOD(CC19,8),1,1)&amp;"."&amp;(MOD(CC19,8)-FLOOR(MOD(CC19,8),1,1))*60</f>
+        <f>FLOOR(CC19/8,1)&amp;"."&amp;FLOOR(MOD(CC19,8),1)&amp;"."&amp;(MOD(CC19,8)-FLOOR(MOD(CC19,8),1))*60</f>
       </c>
       <c r="CF19" s="5" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="CG19" s="5" t="str">
         <f>INT(LEFT(CF19,2))</f>
@@ -5613,16 +5631,16 @@
         <v>17</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="D20" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>81</v>
@@ -5631,13 +5649,13 @@
         <v>81</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K20" s="5" t="str">
         <f>INT(LEFT(E20,2))</f>
@@ -5748,10 +5766,10 @@
         <f>FLOOR(AS20/8,1)&amp;"."&amp;FLOOR(MOD(AS20,8),1)&amp;"."&amp;(MOD(AS20,8)-FLOOR(MOD(AS20,8),1))*60</f>
       </c>
       <c r="AU20" s="5" t="s">
-        <v>123</v>
+        <v>81</v>
       </c>
       <c r="AV20" s="5" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="AW20" s="5" t="s">
         <v>81</v>
@@ -5856,10 +5874,10 @@
         <v>0</v>
       </c>
       <c r="CE20" s="5" t="str">
-        <f>FLOOR(CC20/8,1,1)&amp;"."&amp;FLOOR(MOD(CC20,8),1,1)&amp;"."&amp;(MOD(CC20,8)-FLOOR(MOD(CC20,8),1,1))*60</f>
+        <f>FLOOR(CC20/8,1)&amp;"."&amp;FLOOR(MOD(CC20,8),1)&amp;"."&amp;(MOD(CC20,8)-FLOOR(MOD(CC20,8),1))*60</f>
       </c>
       <c r="CF20" s="5" t="s">
-        <v>81</v>
+        <v>125</v>
       </c>
       <c r="CG20" s="5" t="str">
         <f>INT(LEFT(CF20,2))</f>
@@ -5882,31 +5900,31 @@
         <v>18</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>99</v>
+        <v>127</v>
       </c>
       <c r="D21" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K21" s="5" t="str">
         <f>INT(LEFT(E21,2))</f>
@@ -6017,7 +6035,7 @@
         <f>FLOOR(AS21/8,1)&amp;"."&amp;FLOOR(MOD(AS21,8),1)&amp;"."&amp;(MOD(AS21,8)-FLOOR(MOD(AS21,8),1))*60</f>
       </c>
       <c r="AU21" s="5" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="AV21" s="5" t="s">
         <v>81</v>
@@ -6026,7 +6044,7 @@
         <v>81</v>
       </c>
       <c r="AX21" s="5" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
       <c r="AY21" s="5" t="s">
         <v>81</v>
@@ -6125,10 +6143,10 @@
         <v>0</v>
       </c>
       <c r="CE21" s="5" t="str">
-        <f>FLOOR(CC21/8,1,1)&amp;"."&amp;FLOOR(MOD(CC21,8),1,1)&amp;"."&amp;(MOD(CC21,8)-FLOOR(MOD(CC21,8),1,1))*60</f>
+        <f>FLOOR(CC21/8,1)&amp;"."&amp;FLOOR(MOD(CC21,8),1)&amp;"."&amp;(MOD(CC21,8)-FLOOR(MOD(CC21,8),1))*60</f>
       </c>
       <c r="CF21" s="5" t="s">
-        <v>125</v>
+        <v>81</v>
       </c>
       <c r="CG21" s="5" t="str">
         <f>INT(LEFT(CF21,2))</f>
@@ -6151,10 +6169,10 @@
         <v>19</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="D22" s="5" t="n">
         <v>0</v>
@@ -6163,19 +6181,19 @@
         <v>81</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K22" s="5" t="str">
         <f>INT(LEFT(E22,2))</f>
@@ -6394,10 +6412,10 @@
         <v>0</v>
       </c>
       <c r="CE22" s="5" t="str">
-        <f>FLOOR(CC22/8,1,1)&amp;"."&amp;FLOOR(MOD(CC22,8),1,1)&amp;"."&amp;(MOD(CC22,8)-FLOOR(MOD(CC22,8),1,1))*60</f>
+        <f>FLOOR(CC22/8,1)&amp;"."&amp;FLOOR(MOD(CC22,8),1)&amp;"."&amp;(MOD(CC22,8)-FLOOR(MOD(CC22,8),1))*60</f>
       </c>
       <c r="CF22" s="5" t="s">
-        <v>103</v>
+        <v>131</v>
       </c>
       <c r="CG22" s="5" t="str">
         <f>INT(LEFT(CF22,2))</f>
@@ -6420,16 +6438,16 @@
         <v>20</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="D23" s="5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>129</v>
+        <v>81</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>81</v>
@@ -6438,13 +6456,13 @@
         <v>81</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K23" s="5" t="str">
         <f>INT(LEFT(E23,2))</f>
@@ -6555,7 +6573,7 @@
         <f>FLOOR(AS23/8,1)&amp;"."&amp;FLOOR(MOD(AS23,8),1)&amp;"."&amp;(MOD(AS23,8)-FLOOR(MOD(AS23,8),1))*60</f>
       </c>
       <c r="AU23" s="5" t="s">
-        <v>130</v>
+        <v>81</v>
       </c>
       <c r="AV23" s="5" t="s">
         <v>81</v>
@@ -6663,10 +6681,10 @@
         <v>0</v>
       </c>
       <c r="CE23" s="5" t="str">
-        <f>FLOOR(CC23/8,1,1)&amp;"."&amp;FLOOR(MOD(CC23,8),1,1)&amp;"."&amp;(MOD(CC23,8)-FLOOR(MOD(CC23,8),1,1))*60</f>
+        <f>FLOOR(CC23/8,1)&amp;"."&amp;FLOOR(MOD(CC23,8),1)&amp;"."&amp;(MOD(CC23,8)-FLOOR(MOD(CC23,8),1))*60</f>
       </c>
       <c r="CF23" s="5" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="CG23" s="5" t="str">
         <f>INT(LEFT(CF23,2))</f>
@@ -6689,16 +6707,16 @@
         <v>21</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="D24" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>81</v>
@@ -6707,13 +6725,13 @@
         <v>81</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I24" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K24" s="5" t="str">
         <f>INT(LEFT(E24,2))</f>
@@ -6932,10 +6950,10 @@
         <v>0</v>
       </c>
       <c r="CE24" s="5" t="str">
-        <f>FLOOR(CC24/8,1,1)&amp;"."&amp;FLOOR(MOD(CC24,8),1,1)&amp;"."&amp;(MOD(CC24,8)-FLOOR(MOD(CC24,8),1,1))*60</f>
+        <f>FLOOR(CC24/8,1)&amp;"."&amp;FLOOR(MOD(CC24,8),1)&amp;"."&amp;(MOD(CC24,8)-FLOOR(MOD(CC24,8),1))*60</f>
       </c>
       <c r="CF24" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="CG24" s="5" t="str">
         <f>INT(LEFT(CF24,2))</f>
@@ -6958,16 +6976,16 @@
         <v>22</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="D25" s="5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>81</v>
@@ -6976,13 +6994,13 @@
         <v>81</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K25" s="5" t="str">
         <f>INT(LEFT(E25,2))</f>
@@ -7096,7 +7114,7 @@
         <v>81</v>
       </c>
       <c r="AV25" s="5" t="s">
-        <v>135</v>
+        <v>81</v>
       </c>
       <c r="AW25" s="5" t="s">
         <v>81</v>
@@ -7201,10 +7219,10 @@
         <v>0</v>
       </c>
       <c r="CE25" s="5" t="str">
-        <f>FLOOR(CC25/8,1,1)&amp;"."&amp;FLOOR(MOD(CC25,8),1,1)&amp;"."&amp;(MOD(CC25,8)-FLOOR(MOD(CC25,8),1,1))*60</f>
+        <f>FLOOR(CC25/8,1)&amp;"."&amp;FLOOR(MOD(CC25,8),1)&amp;"."&amp;(MOD(CC25,8)-FLOOR(MOD(CC25,8),1))*60</f>
       </c>
       <c r="CF25" s="5" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="CG25" s="5" t="str">
         <f>INT(LEFT(CF25,2))</f>
@@ -7227,31 +7245,31 @@
         <v>23</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="D26" s="5" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>81</v>
+        <v>138</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>81</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K26" s="5" t="str">
         <f>INT(LEFT(E26,2))</f>
@@ -7470,10 +7488,10 @@
         <v>0</v>
       </c>
       <c r="CE26" s="5" t="str">
-        <f>FLOOR(CC26/8,1,1)&amp;"."&amp;FLOOR(MOD(CC26,8),1,1)&amp;"."&amp;(MOD(CC26,8)-FLOOR(MOD(CC26,8),1,1))*60</f>
+        <f>FLOOR(CC26/8,1)&amp;"."&amp;FLOOR(MOD(CC26,8),1)&amp;"."&amp;(MOD(CC26,8)-FLOOR(MOD(CC26,8),1))*60</f>
       </c>
       <c r="CF26" s="5" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="CG26" s="5" t="str">
         <f>INT(LEFT(CF26,2))</f>
@@ -7496,10 +7514,10 @@
         <v>24</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>84</v>
+        <v>140</v>
       </c>
       <c r="D27" s="5" t="n">
         <v>0</v>
@@ -7514,13 +7532,13 @@
         <v>81</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K27" s="5" t="str">
         <f>INT(LEFT(E27,2))</f>
@@ -7631,7 +7649,7 @@
         <f>FLOOR(AS27/8,1)&amp;"."&amp;FLOOR(MOD(AS27,8),1)&amp;"."&amp;(MOD(AS27,8)-FLOOR(MOD(AS27,8),1))*60</f>
       </c>
       <c r="AU27" s="5" t="s">
-        <v>139</v>
+        <v>81</v>
       </c>
       <c r="AV27" s="5" t="s">
         <v>81</v>
@@ -7739,10 +7757,10 @@
         <v>0</v>
       </c>
       <c r="CE27" s="5" t="str">
-        <f>FLOOR(CC27/8,1,1)&amp;"."&amp;FLOOR(MOD(CC27,8),1,1)&amp;"."&amp;(MOD(CC27,8)-FLOOR(MOD(CC27,8),1,1))*60</f>
+        <f>FLOOR(CC27/8,1)&amp;"."&amp;FLOOR(MOD(CC27,8),1)&amp;"."&amp;(MOD(CC27,8)-FLOOR(MOD(CC27,8),1))*60</f>
       </c>
       <c r="CF27" s="5" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="CG27" s="5" t="str">
         <f>INT(LEFT(CF27,2))</f>
@@ -7765,31 +7783,31 @@
         <v>25</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D28" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>81</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I28" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="K28" s="5" t="str">
         <f>INT(LEFT(E28,2))</f>
@@ -8008,10 +8026,10 @@
         <v>0</v>
       </c>
       <c r="CE28" s="5" t="str">
-        <f>FLOOR(CC28/8,1,1)&amp;"."&amp;FLOOR(MOD(CC28,8),1,1)&amp;"."&amp;(MOD(CC28,8)-FLOOR(MOD(CC28,8),1,1))*60</f>
+        <f>FLOOR(CC28/8,1)&amp;"."&amp;FLOOR(MOD(CC28,8),1)&amp;"."&amp;(MOD(CC28,8)-FLOOR(MOD(CC28,8),1))*60</f>
       </c>
       <c r="CF28" s="5" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="CG28" s="5" t="str">
         <f>INT(LEFT(CF28,2))</f>
@@ -8034,16 +8052,16 @@
         <v>26</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="D29" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>81</v>
@@ -8052,13 +8070,13 @@
         <v>81</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K29" s="5" t="str">
         <f>INT(LEFT(E29,2))</f>
@@ -8277,10 +8295,10 @@
         <v>0</v>
       </c>
       <c r="CE29" s="5" t="str">
-        <f>FLOOR(CC29/8,1,1)&amp;"."&amp;FLOOR(MOD(CC29,8),1,1)&amp;"."&amp;(MOD(CC29,8)-FLOOR(MOD(CC29,8),1,1))*60</f>
+        <f>FLOOR(CC29/8,1)&amp;"."&amp;FLOOR(MOD(CC29,8),1)&amp;"."&amp;(MOD(CC29,8)-FLOOR(MOD(CC29,8),1))*60</f>
       </c>
       <c r="CF29" s="5" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="CG29" s="5" t="str">
         <f>INT(LEFT(CF29,2))</f>
@@ -8306,7 +8324,7 @@
         <v>143</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>80</v>
+        <v>133</v>
       </c>
       <c r="D30" s="5" t="n">
         <v>0</v>
@@ -8321,13 +8339,13 @@
         <v>81</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I30" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K30" s="5" t="str">
         <f>INT(LEFT(E30,2))</f>
@@ -8450,7 +8468,7 @@
         <v>81</v>
       </c>
       <c r="AY30" s="5" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="AZ30" s="5" t="str">
         <f>INT(LEFT(AU30,1))</f>
@@ -8546,10 +8564,10 @@
         <v>0</v>
       </c>
       <c r="CE30" s="5" t="str">
-        <f>FLOOR(CC30/8,1,1)&amp;"."&amp;FLOOR(MOD(CC30,8),1,1)&amp;"."&amp;(MOD(CC30,8)-FLOOR(MOD(CC30,8),1,1))*60</f>
+        <f>FLOOR(CC30/8,1)&amp;"."&amp;FLOOR(MOD(CC30,8),1)&amp;"."&amp;(MOD(CC30,8)-FLOOR(MOD(CC30,8),1))*60</f>
       </c>
       <c r="CF30" s="5" t="s">
-        <v>81</v>
+        <v>144</v>
       </c>
       <c r="CG30" s="5" t="str">
         <f>INT(LEFT(CF30,2))</f>
@@ -8572,16 +8590,16 @@
         <v>28</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>127</v>
+        <v>80</v>
       </c>
       <c r="D31" s="5" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>81</v>
+        <v>146</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>81</v>
@@ -8590,13 +8608,13 @@
         <v>81</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K31" s="5" t="str">
         <f>INT(LEFT(E31,2))</f>
@@ -8707,7 +8725,7 @@
         <f>FLOOR(AS31/8,1)&amp;"."&amp;FLOOR(MOD(AS31,8),1)&amp;"."&amp;(MOD(AS31,8)-FLOOR(MOD(AS31,8),1))*60</f>
       </c>
       <c r="AU31" s="5" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="AV31" s="5" t="s">
         <v>81</v>
@@ -8815,10 +8833,10 @@
         <v>0</v>
       </c>
       <c r="CE31" s="5" t="str">
-        <f>FLOOR(CC31/8,1,1)&amp;"."&amp;FLOOR(MOD(CC31,8),1,1)&amp;"."&amp;(MOD(CC31,8)-FLOOR(MOD(CC31,8),1,1))*60</f>
+        <f>FLOOR(CC31/8,1)&amp;"."&amp;FLOOR(MOD(CC31,8),1)&amp;"."&amp;(MOD(CC31,8)-FLOOR(MOD(CC31,8),1))*60</f>
       </c>
       <c r="CF31" s="5" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="CG31" s="5" t="str">
         <f>INT(LEFT(CF31,2))</f>
@@ -8841,10 +8859,10 @@
         <v>29</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>80</v>
+        <v>133</v>
       </c>
       <c r="D32" s="5" t="n">
         <v>0</v>
@@ -8859,13 +8877,13 @@
         <v>81</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I32" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K32" s="5" t="str">
         <f>INT(LEFT(E32,2))</f>
@@ -9084,10 +9102,10 @@
         <v>0</v>
       </c>
       <c r="CE32" s="5" t="str">
-        <f>FLOOR(CC32/8,1,1)&amp;"."&amp;FLOOR(MOD(CC32,8),1,1)&amp;"."&amp;(MOD(CC32,8)-FLOOR(MOD(CC32,8),1,1))*60</f>
+        <f>FLOOR(CC32/8,1)&amp;"."&amp;FLOOR(MOD(CC32,8),1)&amp;"."&amp;(MOD(CC32,8)-FLOOR(MOD(CC32,8),1))*60</f>
       </c>
       <c r="CF32" s="5" t="s">
-        <v>81</v>
+        <v>148</v>
       </c>
       <c r="CG32" s="5" t="str">
         <f>INT(LEFT(CF32,2))</f>
@@ -9110,16 +9128,16 @@
         <v>30</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>147</v>
+        <v>80</v>
       </c>
       <c r="D33" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>148</v>
+        <v>103</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>81</v>
@@ -9128,13 +9146,13 @@
         <v>81</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K33" s="5" t="str">
         <f>INT(LEFT(E33,2))</f>
@@ -9245,7 +9263,7 @@
         <f>FLOOR(AS33/8,1)&amp;"."&amp;FLOOR(MOD(AS33,8),1)&amp;"."&amp;(MOD(AS33,8)-FLOOR(MOD(AS33,8),1))*60</f>
       </c>
       <c r="AU33" s="5" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="AV33" s="5" t="s">
         <v>81</v>
@@ -9353,10 +9371,10 @@
         <v>0</v>
       </c>
       <c r="CE33" s="5" t="str">
-        <f>FLOOR(CC33/8,1,1)&amp;"."&amp;FLOOR(MOD(CC33,8),1,1)&amp;"."&amp;(MOD(CC33,8)-FLOOR(MOD(CC33,8),1,1))*60</f>
+        <f>FLOOR(CC33/8,1)&amp;"."&amp;FLOOR(MOD(CC33,8),1)&amp;"."&amp;(MOD(CC33,8)-FLOOR(MOD(CC33,8),1))*60</f>
       </c>
       <c r="CF33" s="5" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="CG33" s="5" t="str">
         <f>INT(LEFT(CF33,2))</f>
@@ -9379,31 +9397,31 @@
         <v>31</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="D34" s="5" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K34" s="5" t="str">
         <f>INT(LEFT(E34,2))</f>
@@ -9514,7 +9532,7 @@
         <f>FLOOR(AS34/8,1)&amp;"."&amp;FLOOR(MOD(AS34,8),1)&amp;"."&amp;(MOD(AS34,8)-FLOOR(MOD(AS34,8),1))*60</f>
       </c>
       <c r="AU34" s="5" t="s">
-        <v>81</v>
+        <v>152</v>
       </c>
       <c r="AV34" s="5" t="s">
         <v>81</v>
@@ -9622,10 +9640,10 @@
         <v>0</v>
       </c>
       <c r="CE34" s="5" t="str">
-        <f>FLOOR(CC34/8,1,1)&amp;"."&amp;FLOOR(MOD(CC34,8),1,1)&amp;"."&amp;(MOD(CC34,8)-FLOOR(MOD(CC34,8),1,1))*60</f>
+        <f>FLOOR(CC34/8,1)&amp;"."&amp;FLOOR(MOD(CC34,8),1)&amp;"."&amp;(MOD(CC34,8)-FLOOR(MOD(CC34,8),1))*60</f>
       </c>
       <c r="CF34" s="5" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="CG34" s="5" t="str">
         <f>INT(LEFT(CF34,2))</f>
@@ -9648,16 +9666,16 @@
         <v>32</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="D35" s="5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>81</v>
@@ -9666,13 +9684,13 @@
         <v>81</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K35" s="5" t="str">
         <f>INT(LEFT(E35,2))</f>
@@ -9891,10 +9909,10 @@
         <v>0</v>
       </c>
       <c r="CE35" s="5" t="str">
-        <f>FLOOR(CC35/8,1,1)&amp;"."&amp;FLOOR(MOD(CC35,8),1,1)&amp;"."&amp;(MOD(CC35,8)-FLOOR(MOD(CC35,8),1,1))*60</f>
+        <f>FLOOR(CC35/8,1)&amp;"."&amp;FLOOR(MOD(CC35,8),1)&amp;"."&amp;(MOD(CC35,8)-FLOOR(MOD(CC35,8),1))*60</f>
       </c>
       <c r="CF35" s="5" t="s">
-        <v>153</v>
+        <v>115</v>
       </c>
       <c r="CG35" s="5" t="str">
         <f>INT(LEFT(CF35,2))</f>
@@ -9917,16 +9935,16 @@
         <v>33</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="D36" s="5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>81</v>
@@ -9935,13 +9953,13 @@
         <v>81</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I36" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K36" s="5" t="str">
         <f>INT(LEFT(E36,2))</f>
@@ -10160,10 +10178,10 @@
         <v>0</v>
       </c>
       <c r="CE36" s="5" t="str">
-        <f>FLOOR(CC36/8,1,1)&amp;"."&amp;FLOOR(MOD(CC36,8),1,1)&amp;"."&amp;(MOD(CC36,8)-FLOOR(MOD(CC36,8),1,1))*60</f>
+        <f>FLOOR(CC36/8,1)&amp;"."&amp;FLOOR(MOD(CC36,8),1)&amp;"."&amp;(MOD(CC36,8)-FLOOR(MOD(CC36,8),1))*60</f>
       </c>
       <c r="CF36" s="5" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="CG36" s="5" t="str">
         <f>INT(LEFT(CF36,2))</f>
@@ -10186,10 +10204,10 @@
         <v>34</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D37" s="5" t="n">
         <v>0</v>
@@ -10204,13 +10222,13 @@
         <v>81</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I37" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K37" s="5" t="str">
         <f>INT(LEFT(E37,2))</f>
@@ -10321,7 +10339,7 @@
         <f>FLOOR(AS37/8,1)&amp;"."&amp;FLOOR(MOD(AS37,8),1)&amp;"."&amp;(MOD(AS37,8)-FLOOR(MOD(AS37,8),1))*60</f>
       </c>
       <c r="AU37" s="5" t="s">
-        <v>153</v>
+        <v>81</v>
       </c>
       <c r="AV37" s="5" t="s">
         <v>81</v>
@@ -10429,10 +10447,10 @@
         <v>0</v>
       </c>
       <c r="CE37" s="5" t="str">
-        <f>FLOOR(CC37/8,1,1)&amp;"."&amp;FLOOR(MOD(CC37,8),1,1)&amp;"."&amp;(MOD(CC37,8)-FLOOR(MOD(CC37,8),1,1))*60</f>
+        <f>FLOOR(CC37/8,1)&amp;"."&amp;FLOOR(MOD(CC37,8),1)&amp;"."&amp;(MOD(CC37,8)-FLOOR(MOD(CC37,8),1))*60</f>
       </c>
       <c r="CF37" s="5" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="CG37" s="5" t="str">
         <f>INT(LEFT(CF37,2))</f>
@@ -10455,10 +10473,10 @@
         <v>35</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D38" s="5" t="n">
         <v>0</v>
@@ -10473,13 +10491,13 @@
         <v>81</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I38" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K38" s="5" t="str">
         <f>INT(LEFT(E38,2))</f>
@@ -10698,10 +10716,10 @@
         <v>0</v>
       </c>
       <c r="CE38" s="5" t="str">
-        <f>FLOOR(CC38/8,1,1)&amp;"."&amp;FLOOR(MOD(CC38,8),1,1)&amp;"."&amp;(MOD(CC38,8)-FLOOR(MOD(CC38,8),1,1))*60</f>
+        <f>FLOOR(CC38/8,1)&amp;"."&amp;FLOOR(MOD(CC38,8),1)&amp;"."&amp;(MOD(CC38,8)-FLOOR(MOD(CC38,8),1))*60</f>
       </c>
       <c r="CF38" s="5" t="s">
-        <v>91</v>
+        <v>158</v>
       </c>
       <c r="CG38" s="5" t="str">
         <f>INT(LEFT(CF38,2))</f>
@@ -10724,16 +10742,16 @@
         <v>36</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>158</v>
+        <v>105</v>
       </c>
       <c r="D39" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>81</v>
@@ -10742,13 +10760,13 @@
         <v>81</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K39" s="5" t="str">
         <f>INT(LEFT(E39,2))</f>
@@ -10967,10 +10985,10 @@
         <v>0</v>
       </c>
       <c r="CE39" s="5" t="str">
-        <f>FLOOR(CC39/8,1,1)&amp;"."&amp;FLOOR(MOD(CC39,8),1,1)&amp;"."&amp;(MOD(CC39,8)-FLOOR(MOD(CC39,8),1,1))*60</f>
+        <f>FLOOR(CC39/8,1)&amp;"."&amp;FLOOR(MOD(CC39,8),1)&amp;"."&amp;(MOD(CC39,8)-FLOOR(MOD(CC39,8),1))*60</f>
       </c>
       <c r="CF39" s="5" t="s">
-        <v>91</v>
+        <v>144</v>
       </c>
       <c r="CG39" s="5" t="str">
         <f>INT(LEFT(CF39,2))</f>
@@ -10993,16 +11011,16 @@
         <v>37</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D40" s="5" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>81</v>
+        <v>162</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>81</v>
@@ -11011,13 +11029,13 @@
         <v>81</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I40" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K40" s="5" t="str">
         <f>INT(LEFT(E40,2))</f>
@@ -11236,10 +11254,10 @@
         <v>0</v>
       </c>
       <c r="CE40" s="5" t="str">
-        <f>FLOOR(CC40/8,1,1)&amp;"."&amp;FLOOR(MOD(CC40,8),1,1)&amp;"."&amp;(MOD(CC40,8)-FLOOR(MOD(CC40,8),1,1))*60</f>
+        <f>FLOOR(CC40/8,1)&amp;"."&amp;FLOOR(MOD(CC40,8),1)&amp;"."&amp;(MOD(CC40,8)-FLOOR(MOD(CC40,8),1))*60</f>
       </c>
       <c r="CF40" s="5" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="CG40" s="5" t="str">
         <f>INT(LEFT(CF40,2))</f>
@@ -11262,10 +11280,10 @@
         <v>38</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>99</v>
+        <v>161</v>
       </c>
       <c r="D41" s="5" t="n">
         <v>0</v>
@@ -11280,13 +11298,13 @@
         <v>81</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I41" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K41" s="5" t="str">
         <f>INT(LEFT(E41,2))</f>
@@ -11505,10 +11523,10 @@
         <v>0</v>
       </c>
       <c r="CE41" s="5" t="str">
-        <f>FLOOR(CC41/8,1,1)&amp;"."&amp;FLOOR(MOD(CC41,8),1,1)&amp;"."&amp;(MOD(CC41,8)-FLOOR(MOD(CC41,8),1,1))*60</f>
+        <f>FLOOR(CC41/8,1)&amp;"."&amp;FLOOR(MOD(CC41,8),1)&amp;"."&amp;(MOD(CC41,8)-FLOOR(MOD(CC41,8),1))*60</f>
       </c>
       <c r="CF41" s="5" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
       <c r="CG41" s="5" t="str">
         <f>INT(LEFT(CF41,2))</f>
@@ -11531,16 +11549,16 @@
         <v>39</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D42" s="5" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>162</v>
+        <v>81</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>81</v>
@@ -11549,13 +11567,13 @@
         <v>81</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I42" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K42" s="5" t="str">
         <f>INT(LEFT(E42,2))</f>
@@ -11774,10 +11792,10 @@
         <v>0</v>
       </c>
       <c r="CE42" s="5" t="str">
-        <f>FLOOR(CC42/8,1,1)&amp;"."&amp;FLOOR(MOD(CC42,8),1,1)&amp;"."&amp;(MOD(CC42,8)-FLOOR(MOD(CC42,8),1,1))*60</f>
+        <f>FLOOR(CC42/8,1)&amp;"."&amp;FLOOR(MOD(CC42,8),1)&amp;"."&amp;(MOD(CC42,8)-FLOOR(MOD(CC42,8),1))*60</f>
       </c>
       <c r="CF42" s="5" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="CG42" s="5" t="str">
         <f>INT(LEFT(CF42,2))</f>
@@ -11800,31 +11818,31 @@
         <v>40</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="D43" s="5" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K43" s="5" t="str">
         <f>INT(LEFT(E43,2))</f>
@@ -12043,10 +12061,10 @@
         <v>0</v>
       </c>
       <c r="CE43" s="5" t="str">
-        <f>FLOOR(CC43/8,1,1)&amp;"."&amp;FLOOR(MOD(CC43,8),1,1)&amp;"."&amp;(MOD(CC43,8)-FLOOR(MOD(CC43,8),1,1))*60</f>
+        <f>FLOOR(CC43/8,1)&amp;"."&amp;FLOOR(MOD(CC43,8),1)&amp;"."&amp;(MOD(CC43,8)-FLOOR(MOD(CC43,8),1))*60</f>
       </c>
       <c r="CF43" s="5" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="CG43" s="5" t="str">
         <f>INT(LEFT(CF43,2))</f>
@@ -12069,16 +12087,16 @@
         <v>41</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D44" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>81</v>
@@ -12087,13 +12105,13 @@
         <v>81</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I44" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K44" s="5" t="str">
         <f>INT(LEFT(E44,2))</f>
@@ -12204,7 +12222,7 @@
         <f>FLOOR(AS44/8,1)&amp;"."&amp;FLOOR(MOD(AS44,8),1)&amp;"."&amp;(MOD(AS44,8)-FLOOR(MOD(AS44,8),1))*60</f>
       </c>
       <c r="AU44" s="5" t="s">
-        <v>165</v>
+        <v>81</v>
       </c>
       <c r="AV44" s="5" t="s">
         <v>81</v>
@@ -12312,10 +12330,10 @@
         <v>0</v>
       </c>
       <c r="CE44" s="5" t="str">
-        <f>FLOOR(CC44/8,1,1)&amp;"."&amp;FLOOR(MOD(CC44,8),1,1)&amp;"."&amp;(MOD(CC44,8)-FLOOR(MOD(CC44,8),1,1))*60</f>
+        <f>FLOOR(CC44/8,1)&amp;"."&amp;FLOOR(MOD(CC44,8),1)&amp;"."&amp;(MOD(CC44,8)-FLOOR(MOD(CC44,8),1))*60</f>
       </c>
       <c r="CF44" s="5" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="CG44" s="5" t="str">
         <f>INT(LEFT(CF44,2))</f>
@@ -12338,31 +12356,31 @@
         <v>42</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="D45" s="5" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>81</v>
+        <v>138</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I45" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K45" s="5" t="str">
         <f>INT(LEFT(E45,2))</f>
@@ -12473,10 +12491,10 @@
         <f>FLOOR(AS45/8,1)&amp;"."&amp;FLOOR(MOD(AS45,8),1)&amp;"."&amp;(MOD(AS45,8)-FLOOR(MOD(AS45,8),1))*60</f>
       </c>
       <c r="AU45" s="5" t="s">
-        <v>81</v>
+        <v>170</v>
       </c>
       <c r="AV45" s="5" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="AW45" s="5" t="s">
         <v>81</v>
@@ -12581,10 +12599,10 @@
         <v>0</v>
       </c>
       <c r="CE45" s="5" t="str">
-        <f>FLOOR(CC45/8,1,1)&amp;"."&amp;FLOOR(MOD(CC45,8),1,1)&amp;"."&amp;(MOD(CC45,8)-FLOOR(MOD(CC45,8),1,1))*60</f>
+        <f>FLOOR(CC45/8,1)&amp;"."&amp;FLOOR(MOD(CC45,8),1)&amp;"."&amp;(MOD(CC45,8)-FLOOR(MOD(CC45,8),1))*60</f>
       </c>
       <c r="CF45" s="5" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="CG45" s="5" t="str">
         <f>INT(LEFT(CF45,2))</f>
@@ -12607,31 +12625,31 @@
         <v>43</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D46" s="5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>81</v>
+        <v>146</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I46" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K46" s="5" t="str">
         <f>INT(LEFT(E46,2))</f>
@@ -12850,10 +12868,10 @@
         <v>0</v>
       </c>
       <c r="CE46" s="5" t="str">
-        <f>FLOOR(CC46/8,1,1)&amp;"."&amp;FLOOR(MOD(CC46,8),1,1)&amp;"."&amp;(MOD(CC46,8)-FLOOR(MOD(CC46,8),1,1))*60</f>
+        <f>FLOOR(CC46/8,1)&amp;"."&amp;FLOOR(MOD(CC46,8),1)&amp;"."&amp;(MOD(CC46,8)-FLOOR(MOD(CC46,8),1))*60</f>
       </c>
       <c r="CF46" s="5" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="CG46" s="5" t="str">
         <f>INT(LEFT(CF46,2))</f>
@@ -12876,10 +12894,10 @@
         <v>44</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>169</v>
+        <v>122</v>
       </c>
       <c r="D47" s="5" t="n">
         <v>0</v>
@@ -12888,19 +12906,19 @@
         <v>81</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>148</v>
+        <v>81</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I47" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K47" s="5" t="str">
         <f>INT(LEFT(E47,2))</f>
@@ -13011,7 +13029,7 @@
         <f>FLOOR(AS47/8,1)&amp;"."&amp;FLOOR(MOD(AS47,8),1)&amp;"."&amp;(MOD(AS47,8)-FLOOR(MOD(AS47,8),1))*60</f>
       </c>
       <c r="AU47" s="5" t="s">
-        <v>170</v>
+        <v>81</v>
       </c>
       <c r="AV47" s="5" t="s">
         <v>81</v>
@@ -13119,10 +13137,10 @@
         <v>0</v>
       </c>
       <c r="CE47" s="5" t="str">
-        <f>FLOOR(CC47/8,1,1)&amp;"."&amp;FLOOR(MOD(CC47,8),1,1)&amp;"."&amp;(MOD(CC47,8)-FLOOR(MOD(CC47,8),1,1))*60</f>
+        <f>FLOOR(CC47/8,1)&amp;"."&amp;FLOOR(MOD(CC47,8),1)&amp;"."&amp;(MOD(CC47,8)-FLOOR(MOD(CC47,8),1))*60</f>
       </c>
       <c r="CF47" s="5" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="CG47" s="5" t="str">
         <f>INT(LEFT(CF47,2))</f>
@@ -13145,31 +13163,31 @@
         <v>45</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="D48" s="5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I48" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K48" s="5" t="str">
         <f>INT(LEFT(E48,2))</f>
@@ -13280,7 +13298,7 @@
         <f>FLOOR(AS48/8,1)&amp;"."&amp;FLOOR(MOD(AS48,8),1)&amp;"."&amp;(MOD(AS48,8)-FLOOR(MOD(AS48,8),1))*60</f>
       </c>
       <c r="AU48" s="5" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="AV48" s="5" t="s">
         <v>81</v>
@@ -13388,10 +13406,10 @@
         <v>0</v>
       </c>
       <c r="CE48" s="5" t="str">
-        <f>FLOOR(CC48/8,1,1)&amp;"."&amp;FLOOR(MOD(CC48,8),1,1)&amp;"."&amp;(MOD(CC48,8)-FLOOR(MOD(CC48,8),1,1))*60</f>
+        <f>FLOOR(CC48/8,1)&amp;"."&amp;FLOOR(MOD(CC48,8),1)&amp;"."&amp;(MOD(CC48,8)-FLOOR(MOD(CC48,8),1))*60</f>
       </c>
       <c r="CF48" s="5" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="CG48" s="5" t="str">
         <f>INT(LEFT(CF48,2))</f>
@@ -13414,16 +13432,16 @@
         <v>46</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>97</v>
+        <v>151</v>
       </c>
       <c r="D49" s="5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>81</v>
+        <v>146</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>81</v>
@@ -13432,13 +13450,13 @@
         <v>81</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I49" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K49" s="5" t="str">
         <f>INT(LEFT(E49,2))</f>
@@ -13549,10 +13567,10 @@
         <f>FLOOR(AS49/8,1)&amp;"."&amp;FLOOR(MOD(AS49,8),1)&amp;"."&amp;(MOD(AS49,8)-FLOOR(MOD(AS49,8),1))*60</f>
       </c>
       <c r="AU49" s="5" t="s">
-        <v>173</v>
+        <v>115</v>
       </c>
       <c r="AV49" s="5" t="s">
-        <v>81</v>
+        <v>176</v>
       </c>
       <c r="AW49" s="5" t="s">
         <v>81</v>
@@ -13657,10 +13675,10 @@
         <v>0</v>
       </c>
       <c r="CE49" s="5" t="str">
-        <f>FLOOR(CC49/8,1,1)&amp;"."&amp;FLOOR(MOD(CC49,8),1,1)&amp;"."&amp;(MOD(CC49,8)-FLOOR(MOD(CC49,8),1,1))*60</f>
+        <f>FLOOR(CC49/8,1)&amp;"."&amp;FLOOR(MOD(CC49,8),1)&amp;"."&amp;(MOD(CC49,8)-FLOOR(MOD(CC49,8),1))*60</f>
       </c>
       <c r="CF49" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="CG49" s="5" t="str">
         <f>INT(LEFT(CF49,2))</f>
@@ -13683,31 +13701,31 @@
         <v>47</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="D50" s="5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>81</v>
+        <v>166</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>148</v>
+        <v>81</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I50" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>82</v>
+        <v>178</v>
       </c>
       <c r="K50" s="5" t="str">
         <f>INT(LEFT(E50,2))</f>
@@ -13818,7 +13836,7 @@
         <f>FLOOR(AS50/8,1)&amp;"."&amp;FLOOR(MOD(AS50,8),1)&amp;"."&amp;(MOD(AS50,8)-FLOOR(MOD(AS50,8),1))*60</f>
       </c>
       <c r="AU50" s="5" t="s">
-        <v>130</v>
+        <v>81</v>
       </c>
       <c r="AV50" s="5" t="s">
         <v>81</v>
@@ -13926,10 +13944,10 @@
         <v>0</v>
       </c>
       <c r="CE50" s="5" t="str">
-        <f>FLOOR(CC50/8,1,1)&amp;"."&amp;FLOOR(MOD(CC50,8),1,1)&amp;"."&amp;(MOD(CC50,8)-FLOOR(MOD(CC50,8),1,1))*60</f>
+        <f>FLOOR(CC50/8,1)&amp;"."&amp;FLOOR(MOD(CC50,8),1)&amp;"."&amp;(MOD(CC50,8)-FLOOR(MOD(CC50,8),1))*60</f>
       </c>
       <c r="CF50" s="5" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="CG50" s="5" t="str">
         <f>INT(LEFT(CF50,2))</f>
@@ -13952,10 +13970,10 @@
         <v>48</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>176</v>
+        <v>88</v>
       </c>
       <c r="D51" s="5" t="n">
         <v>0</v>
@@ -13970,13 +13988,13 @@
         <v>81</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I51" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K51" s="5" t="str">
         <f>INT(LEFT(E51,2))</f>
@@ -14195,10 +14213,10 @@
         <v>0</v>
       </c>
       <c r="CE51" s="5" t="str">
-        <f>FLOOR(CC51/8,1,1)&amp;"."&amp;FLOOR(MOD(CC51,8),1,1)&amp;"."&amp;(MOD(CC51,8)-FLOOR(MOD(CC51,8),1,1))*60</f>
+        <f>FLOOR(CC51/8,1)&amp;"."&amp;FLOOR(MOD(CC51,8),1)&amp;"."&amp;(MOD(CC51,8)-FLOOR(MOD(CC51,8),1))*60</f>
       </c>
       <c r="CF51" s="5" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="CG51" s="5" t="str">
         <f>INT(LEFT(CF51,2))</f>
@@ -14221,10 +14239,10 @@
         <v>49</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>93</v>
+        <v>181</v>
       </c>
       <c r="D52" s="5" t="n">
         <v>0</v>
@@ -14239,13 +14257,13 @@
         <v>81</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I52" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K52" s="5" t="str">
         <f>INT(LEFT(E52,2))</f>
@@ -14464,10 +14482,10 @@
         <v>0</v>
       </c>
       <c r="CE52" s="5" t="str">
-        <f>FLOOR(CC52/8,1,1)&amp;"."&amp;FLOOR(MOD(CC52,8),1,1)&amp;"."&amp;(MOD(CC52,8)-FLOOR(MOD(CC52,8),1,1))*60</f>
+        <f>FLOOR(CC52/8,1)&amp;"."&amp;FLOOR(MOD(CC52,8),1)&amp;"."&amp;(MOD(CC52,8)-FLOOR(MOD(CC52,8),1))*60</f>
       </c>
       <c r="CF52" s="5" t="s">
-        <v>103</v>
+        <v>182</v>
       </c>
       <c r="CG52" s="5" t="str">
         <f>INT(LEFT(CF52,2))</f>
@@ -14490,10 +14508,10 @@
         <v>50</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="D53" s="5" t="n">
         <v>0</v>
@@ -14508,13 +14526,13 @@
         <v>81</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I53" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K53" s="5" t="str">
         <f>INT(LEFT(E53,2))</f>
@@ -14733,10 +14751,10 @@
         <v>0</v>
       </c>
       <c r="CE53" s="5" t="str">
-        <f>FLOOR(CC53/8,1,1)&amp;"."&amp;FLOOR(MOD(CC53,8),1,1)&amp;"."&amp;(MOD(CC53,8)-FLOOR(MOD(CC53,8),1,1))*60</f>
+        <f>FLOOR(CC53/8,1)&amp;"."&amp;FLOOR(MOD(CC53,8),1)&amp;"."&amp;(MOD(CC53,8)-FLOOR(MOD(CC53,8),1))*60</f>
       </c>
       <c r="CF53" s="5" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="CG53" s="5" t="str">
         <f>INT(LEFT(CF53,2))</f>
@@ -14755,271 +14773,540 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="I54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="J54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="K54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="L54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="M54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="N54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="O54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="P54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="R54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="S54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="T54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="U54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="V54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="W54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="X54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AG54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AN54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AO54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AP54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AQ54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AR54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AS54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AT54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AU54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AV54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AW54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AX54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AY54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AZ54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BA54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BB54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BC54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BD54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BE54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BF54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BG54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BH54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BI54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BJ54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BK54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BL54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BM54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BN54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BO54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BP54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BQ54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BR54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BS54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BT54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BU54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BV54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BW54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BX54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BY54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BZ54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="CA54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="CB54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="CC54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="CD54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="CE54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="CF54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="CG54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="CH54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="CI54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="CJ54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="CK54" s="6" t="s">
+      <c r="A54" s="5" t="n">
+        <v>51</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D54" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="K54" s="5" t="str">
+        <f>INT(LEFT(E54,2))</f>
+      </c>
+      <c r="L54" s="5" t="str">
+        <f>INT(LEFT(F54,2))</f>
+      </c>
+      <c r="M54" s="5" t="str">
+        <f>INT(LEFT(I54,2))</f>
+      </c>
+      <c r="N54" s="5" t="str">
+        <f>INT(LEFT(G54,2))</f>
+      </c>
+      <c r="O54" s="5" t="str">
+        <f>INT(LEFT(J54,2))</f>
+      </c>
+      <c r="P54" s="5" t="str">
+        <f>INT(LEFT(H54,2))</f>
+      </c>
+      <c r="Q54" s="5" t="str">
+        <f>K54+L54+CG54+IF(M54&gt;O54,M54-O54,0)+IF(N54&gt;P54,N54-P54,0)</f>
+      </c>
+      <c r="R54" s="5" t="str">
+        <f>IF(LEFT(RIGHT(E54,LEN(E54)-2),1)=".",RIGHT(E54,LEN(E54)-3),RIGHT(E54,LEN(E54)-2))</f>
+      </c>
+      <c r="S54" s="5" t="str">
+        <f>IF(LEFT(RIGHT(F54,LEN(F54)-2),1)=".",RIGHT(F54,LEN(F54)-3),RIGHT(F54,LEN(F54)-2))</f>
+      </c>
+      <c r="T54" s="5" t="str">
+        <f>IF(LEFT(RIGHT(I54,LEN(I54)-2),1)=".",RIGHT(I54,LEN(I54)-3),RIGHT(I54,LEN(I54)-2))</f>
+      </c>
+      <c r="U54" s="5" t="str">
+        <f>IF(LEFT(RIGHT(G54,LEN(G54)-2),1)=".",RIGHT(G54,LEN(G54)-3),RIGHT(G54,LEN(G54)-2))</f>
+      </c>
+      <c r="V54" s="5" t="str">
+        <f>IF(LEFT(RIGHT(J54,LEN(J54)-2),1)=".",RIGHT(J54,LEN(J54)-3),RIGHT(J54,LEN(J54)-2))</f>
+      </c>
+      <c r="W54" s="5" t="str">
+        <f>IF(LEFT(RIGHT(H54,LEN(H54)-2),1)=".",RIGHT(H54,LEN(H54)-3),RIGHT(H54,LEN(H54)-2))</f>
+      </c>
+      <c r="X54" s="5" t="str">
+        <f>INT(LEFT(R54,1))</f>
+      </c>
+      <c r="Y54" s="5" t="str">
+        <f>INT(LEFT(S54,1))</f>
+      </c>
+      <c r="Z54" s="5" t="str">
+        <f>INT(LEFT(T54,1))</f>
+      </c>
+      <c r="AA54" s="5" t="str">
+        <f>INT(LEFT(U54,1))</f>
+      </c>
+      <c r="AB54" s="5" t="str">
+        <f>INT(LEFT(V54,1))</f>
+      </c>
+      <c r="AC54" s="5" t="str">
+        <f>INT(LEFT(W54,1))</f>
+      </c>
+      <c r="AD54" s="5" t="str">
+        <f>R54+S54+CH54+IF(T54&gt;V54,T54-V54,0)+IF(U54&gt;W54,U54-W54,0)</f>
+      </c>
+      <c r="AE54" s="5" t="str">
+        <f>RIGHT(R54,LEN(R54)-2)+0</f>
+      </c>
+      <c r="AF54" s="5" t="str">
+        <f>RIGHT(S54,LEN(S54)-2)+0</f>
+      </c>
+      <c r="AG54" s="5" t="str">
+        <f>RIGHT(T54,LEN(T54)-2)+0</f>
+      </c>
+      <c r="AH54" s="5" t="str">
+        <f>RIGHT(U54,LEN(U54)-2)+0</f>
+      </c>
+      <c r="AI54" s="5" t="str">
+        <f>RIGHT(V54,LEN(V54)-2)+0</f>
+      </c>
+      <c r="AJ54" s="5" t="str">
+        <f>RIGHT(W54,LEN(W54)-2)+0</f>
+      </c>
+      <c r="AK54" s="5" t="str">
+        <f>AE54+AF54+CJ54+IF(AG54&gt;AI54,AG54-AI54,0)+IF(AH54&gt;AJ54,AH54-AJ54,0)</f>
+      </c>
+      <c r="AL54" s="5" t="str">
+        <f>K54*8*60+X54*60+AE54</f>
+      </c>
+      <c r="AM54" s="5" t="str">
+        <f>L54*8*60+Y54*60+AF54</f>
+      </c>
+      <c r="AN54" s="5" t="str">
+        <f>M54*8*60+Z54*60+AG54</f>
+      </c>
+      <c r="AO54" s="5" t="str">
+        <f>N54*8*60+AA54*60+AH54</f>
+      </c>
+      <c r="AP54" s="5" t="str">
+        <f>O54*8*60+AB54*60+AI54</f>
+      </c>
+      <c r="AQ54" s="5" t="str">
+        <f>P54*8*60+AC54*60+AJ54</f>
+      </c>
+      <c r="AR54" s="5" t="str">
+        <f>AL54+AM54+CK54+IF(AN54&gt;AP54,AN54-AP54,0)+IF(AO54&gt;AQ54,AO54-AQ54,0)</f>
+      </c>
+      <c r="AS54" s="5" t="str">
+        <f>AR54/60</f>
+      </c>
+      <c r="AT54" s="5" t="str">
+        <f>FLOOR(AS54/8,1)&amp;"."&amp;FLOOR(MOD(AS54,8),1)&amp;"."&amp;(MOD(AS54,8)-FLOOR(MOD(AS54,8),1))*60</f>
+      </c>
+      <c r="AU54" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AV54" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AW54" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AX54" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AY54" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AZ54" s="5" t="str">
+        <f>INT(LEFT(AU54,1))</f>
+      </c>
+      <c r="BA54" s="5" t="str">
+        <f>INT(LEFT(AV54,1))</f>
+      </c>
+      <c r="BB54" s="5" t="str">
+        <f>INT(LEFT(AW54,1))</f>
+      </c>
+      <c r="BC54" s="5" t="str">
+        <f>INT(LEFT(AX54,1))</f>
+      </c>
+      <c r="BD54" s="5" t="str">
+        <f>INT(LEFT(AY54,1))</f>
+      </c>
+      <c r="BE54" s="5" t="str">
+        <f>SUM(AZ54,BA54,BB54,BC54,BD54)</f>
+      </c>
+      <c r="BF54" s="5" t="str">
+        <f>RIGHT(AU54,LEN(AU54)-2)</f>
+      </c>
+      <c r="BG54" s="5" t="str">
+        <f>RIGHT(AV54,LEN(AV54)-2)</f>
+      </c>
+      <c r="BH54" s="5" t="str">
+        <f>RIGHT(AW54,LEN(AW54)-2)</f>
+      </c>
+      <c r="BI54" s="5" t="str">
+        <f>RIGHT(AX54,LEN(AX54)-2)</f>
+      </c>
+      <c r="BJ54" s="5" t="str">
+        <f>RIGHT(AY54,LEN(AY54)-2)</f>
+      </c>
+      <c r="BK54" s="5" t="str">
+        <f>INT(LEFT(BF54,1))</f>
+      </c>
+      <c r="BL54" s="5" t="str">
+        <f>INT(LEFT(BG54,1))</f>
+      </c>
+      <c r="BM54" s="5" t="str">
+        <f>INT(LEFT(BH54,1))</f>
+      </c>
+      <c r="BN54" s="5" t="str">
+        <f>INT(LEFT(BI54,1))</f>
+      </c>
+      <c r="BO54" s="5" t="str">
+        <f>INT(LEFT(BJ54,1))</f>
+      </c>
+      <c r="BP54" s="5" t="str">
+        <f>SUM(BK54:BO54)</f>
+      </c>
+      <c r="BQ54" s="5" t="str">
+        <f>RIGHT(BF54,LEN(BF54)-2)+0</f>
+      </c>
+      <c r="BR54" s="5" t="str">
+        <f>RIGHT(BG54,LEN(BG54)-2)+0</f>
+      </c>
+      <c r="BS54" s="5" t="str">
+        <f>RIGHT(BH54,LEN(BH54)-2)+0</f>
+      </c>
+      <c r="BT54" s="5" t="str">
+        <f>RIGHT(BI54,LEN(BI54)-2)+0</f>
+      </c>
+      <c r="BU54" s="5" t="str">
+        <f>RIGHT(BJ54,LEN(BJ54)-2)+0</f>
+      </c>
+      <c r="BV54" s="5" t="str">
+        <f>SUM(BQ54:BU54)</f>
+      </c>
+      <c r="BW54" s="5" t="str">
+        <f>AZ54*8*60+BK54*60+BQ54</f>
+      </c>
+      <c r="BX54" s="5" t="str">
+        <f>BA54*8*60+BL54*60+BR54</f>
+      </c>
+      <c r="BY54" s="5" t="str">
+        <f>BB54*8*60+BM54*60+BS54</f>
+      </c>
+      <c r="BZ54" s="5" t="str">
+        <f>BC54*8*60+BN54*60+BT54</f>
+      </c>
+      <c r="CA54" s="5" t="str">
+        <f>BD54*8*60+BO54*60+BU54</f>
+      </c>
+      <c r="CB54" s="5" t="str">
+        <f>SUM(BW54:CA54)</f>
+      </c>
+      <c r="CC54" s="5" t="str">
+        <f>CB54/60</f>
+      </c>
+      <c r="CD54" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CE54" s="5" t="str">
+        <f>FLOOR(CC54/8,1)&amp;"."&amp;FLOOR(MOD(CC54,8),1)&amp;"."&amp;(MOD(CC54,8)-FLOOR(MOD(CC54,8),1))*60</f>
+      </c>
+      <c r="CF54" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="CG54" s="5" t="str">
+        <f>INT(LEFT(CF54,2))</f>
+      </c>
+      <c r="CH54" s="5" t="str">
+        <f>IF(LEFT(RIGHT(CF54,LEN(CF54)-2),1)=".",RIGHT(CF54,LEN(CF54)-3),RIGHT(CF54,LEN(CF54)-2))</f>
+      </c>
+      <c r="CI54" s="5" t="str">
+        <f>INT(LEFT(CH54,1))</f>
+      </c>
+      <c r="CJ54" s="5" t="str">
+        <f>RIGHT(CH54,LEN(CH54)-2)+0</f>
+      </c>
+      <c r="CK54" s="5" t="str">
+        <f>CG54*8*60+CI54*60+CJ54</f>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="O55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="R55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="S55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="T55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="U55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="V55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="W55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="X55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AN55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AR55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AY55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BD55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BE55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BF55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BI55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BJ55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BK55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BL55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BM55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BN55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BO55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BP55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BQ55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BR55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BS55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BT55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BU55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BV55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BW55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BX55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BY55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BZ55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CA55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CB55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CC55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CD55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CE55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CF55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CG55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CH55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CI55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CJ55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CK55" s="6" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed employee dtr folder name. Also added thin in gemfile
</commit_message>
<xml_diff>
--- a/exceltocsv/public/reports/DTRSUMMARY.xlsx
+++ b/exceltocsv/public/reports/DTRSUMMARY.xlsx
@@ -9,9 +9,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="185" xml:space="preserve">
-  <si>
-    <t>iRipple, Inc. | DTR Summary Sheet for the period April 25, 2015 to May 08, 2015</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="179" xml:space="preserve">
+  <si>
+    <t>iRipple, Inc. | DTR Summary Sheet for the period March 21, 2015 to April 03, 2015</t>
   </si>
   <si>
     <t>Employee Information</t>
@@ -257,271 +257,256 @@
     <t>0.0.0</t>
   </si>
   <si>
+    <t>7.4.0</t>
+  </si>
+  <si>
+    <t>Ardamoy, Ma. Rica Catherine</t>
+  </si>
+  <si>
+    <t>Enterprise - Petron</t>
+  </si>
+  <si>
+    <t>0.0.15</t>
+  </si>
+  <si>
+    <t>0.4.0</t>
+  </si>
+  <si>
+    <t>Bacani, Eddie Marie</t>
+  </si>
+  <si>
+    <t>International Business - Thailand</t>
+  </si>
+  <si>
+    <t>Balingit, Barbara</t>
+  </si>
+  <si>
+    <t>HR &amp;amp; Admin</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>Balino, Kamille Diane</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>0.0.45</t>
+  </si>
+  <si>
+    <t>Barrion, Jane Katherine</t>
+  </si>
+  <si>
+    <t>Bayogos, Charmaine</t>
+  </si>
+  <si>
+    <t>Enterprise - Ayagold</t>
+  </si>
+  <si>
+    <t>Borlagdan, Aldrin</t>
+  </si>
+  <si>
+    <t>ATVI</t>
+  </si>
+  <si>
     <t>0.1.15</t>
   </si>
   <si>
-    <t>7.4.0</t>
-  </si>
-  <si>
-    <t>6.4.0</t>
+    <t>Buena, Ian Christopher</t>
+  </si>
+  <si>
+    <t>0.3.0</t>
+  </si>
+  <si>
+    <t>1.4.0</t>
+  </si>
+  <si>
+    <t>Buenafe, Rajiv</t>
+  </si>
+  <si>
+    <t>4.0.0</t>
+  </si>
+  <si>
+    <t>3.0.0</t>
+  </si>
+  <si>
+    <t>Cataluna, Christian Gilbert</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>8.0.0</t>
+  </si>
+  <si>
+    <t>CaÃ±ete, Carol Ann</t>
+  </si>
+  <si>
+    <t>0.1.0</t>
+  </si>
+  <si>
+    <t>2.4.0</t>
+  </si>
+  <si>
+    <t>Cerbo, Jaycer</t>
+  </si>
+  <si>
+    <t>Ching, Mark Angelo</t>
+  </si>
+  <si>
+    <t>Imaghine</t>
   </si>
   <si>
     <t>0.5.0</t>
   </si>
   <si>
+    <t>3.4.0</t>
+  </si>
+  <si>
+    <t>Cortez, Jomar</t>
+  </si>
+  <si>
+    <t>Barter Local - Support</t>
+  </si>
+  <si>
+    <t>Cruz, Cesar</t>
+  </si>
+  <si>
+    <t>Delfin, Jonathan</t>
+  </si>
+  <si>
+    <t>International Business - PNG</t>
+  </si>
+  <si>
+    <t>0.2.0</t>
+  </si>
+  <si>
+    <t>Dino, Arvin</t>
+  </si>
+  <si>
     <t>4.4.0</t>
   </si>
   <si>
-    <t>Ardamoy, Ma. Rica Catherine</t>
-  </si>
-  <si>
-    <t>Enterprise - Petron</t>
-  </si>
-  <si>
-    <t>Bacani, Eddie Marie</t>
-  </si>
-  <si>
-    <t>International Business - Thailand</t>
+    <t>Dy, Hubert</t>
+  </si>
+  <si>
+    <t>Executive</t>
+  </si>
+  <si>
+    <t>Egamino, Ellen</t>
   </si>
   <si>
     <t>0.1.45</t>
   </si>
   <si>
-    <t>Balingit, Barbara</t>
-  </si>
-  <si>
-    <t>HR &amp;amp; Admin</t>
-  </si>
-  <si>
-    <t>Balino, Kamille Diane</t>
-  </si>
-  <si>
-    <t>Product</t>
+    <t>0.7.0</t>
+  </si>
+  <si>
+    <t>Enrique, Christian Dan</t>
+  </si>
+  <si>
+    <t>Barter Local - Project</t>
+  </si>
+  <si>
+    <t>5.0.0</t>
+  </si>
+  <si>
+    <t>Espiritu, Carl Philip</t>
+  </si>
+  <si>
+    <t>1.3.0</t>
+  </si>
+  <si>
+    <t>Fadrilan, Liezl</t>
+  </si>
+  <si>
+    <t>Synext (Nexus)</t>
+  </si>
+  <si>
+    <t>Flores, Arianne Grace</t>
+  </si>
+  <si>
+    <t>1.7.0</t>
+  </si>
+  <si>
+    <t>Francisco, Roed Ronualdo </t>
+  </si>
+  <si>
+    <t>Javier, Victor </t>
+  </si>
+  <si>
+    <t>5.4.0</t>
+  </si>
+  <si>
+    <t>Joson, Alfonso Miguel</t>
+  </si>
+  <si>
+    <t>Keng, Julie</t>
+  </si>
+  <si>
+    <t>Laude, Ted Marty</t>
+  </si>
+  <si>
+    <t>Mangundayao, Mac Donald</t>
+  </si>
+  <si>
+    <t>Barter CX</t>
   </si>
   <si>
     <t>0.0.30</t>
   </si>
   <si>
-    <t>Barrion, Jane Katherine</t>
-  </si>
-  <si>
-    <t>1.0.0</t>
-  </si>
-  <si>
-    <t>0.4.0</t>
-  </si>
-  <si>
-    <t>Bayogos, Charmaine</t>
-  </si>
-  <si>
-    <t>Enterprise - Ayagold</t>
-  </si>
-  <si>
-    <t>Bernardo, Gianilla Mae</t>
-  </si>
-  <si>
-    <t>0.0.15</t>
-  </si>
-  <si>
-    <t>Borlagdan, Aldrin</t>
-  </si>
-  <si>
-    <t>ATVI</t>
-  </si>
-  <si>
-    <t>Buena, Ian Christopher</t>
-  </si>
-  <si>
-    <t>0.1.0</t>
-  </si>
-  <si>
-    <t>5.0.0</t>
-  </si>
-  <si>
-    <t>Buenafe, Rajiv</t>
-  </si>
-  <si>
-    <t>9.0.0</t>
-  </si>
-  <si>
-    <t>Cataluna, Christian Gilbert</t>
-  </si>
-  <si>
-    <t>Sales</t>
-  </si>
-  <si>
-    <t>CaÃ±ete, Carol Ann</t>
-  </si>
-  <si>
-    <t>0.0.45</t>
+    <t>Matias, Ma. Jeremia Jetheth </t>
+  </si>
+  <si>
+    <t>0.4.15</t>
+  </si>
+  <si>
+    <t>Mendoza, Diana</t>
+  </si>
+  <si>
+    <t>0.5.15</t>
   </si>
   <si>
     <t>2.0.0</t>
   </si>
   <si>
-    <t>Cerbo, Jaycer</t>
-  </si>
-  <si>
-    <t>Ching, Mark Angelo</t>
-  </si>
-  <si>
-    <t>Imaghine</t>
-  </si>
-  <si>
-    <t>0.2.0</t>
+    <t>Nagnal, Fracy</t>
+  </si>
+  <si>
+    <t>Newsom, Jifferson</t>
+  </si>
+  <si>
+    <t>Pajo, Maricel</t>
+  </si>
+  <si>
+    <t>Pancho, Jona</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>Pechuanging, Ma. Antoinette</t>
+  </si>
+  <si>
+    <t>Pendre, Contessa</t>
+  </si>
+  <si>
+    <t>Ranes, Jonathan</t>
   </si>
   <si>
     <t>0.1.30</t>
   </si>
   <si>
-    <t>Cortez, Jomar</t>
-  </si>
-  <si>
-    <t>Barter Local - Support</t>
-  </si>
-  <si>
-    <t>2.4.0</t>
-  </si>
-  <si>
-    <t>Cruz, Cesar</t>
-  </si>
-  <si>
-    <t>1.4.0</t>
-  </si>
-  <si>
-    <t>Delfin, Jonathan</t>
-  </si>
-  <si>
-    <t>International Business - PNG</t>
-  </si>
-  <si>
-    <t>0.7.0</t>
-  </si>
-  <si>
-    <t>Dino, Arvin</t>
-  </si>
-  <si>
-    <t>0.2.15</t>
-  </si>
-  <si>
-    <t>6.0.0</t>
-  </si>
-  <si>
-    <t>Dy, Hubert</t>
-  </si>
-  <si>
-    <t>Executive</t>
-  </si>
-  <si>
-    <t>Egamino, Ellen</t>
-  </si>
-  <si>
-    <t>Enrique, Christian Dan</t>
-  </si>
-  <si>
-    <t>Barter Local - Project</t>
-  </si>
-  <si>
-    <t>Espiritu, Carl Philip</t>
-  </si>
-  <si>
-    <t>0.3.45</t>
-  </si>
-  <si>
-    <t>Fadrilan, Liezl</t>
-  </si>
-  <si>
-    <t>Synext (Nexus)</t>
-  </si>
-  <si>
-    <t>Flores, Arianne Grace</t>
-  </si>
-  <si>
-    <t>Francisco, Roed Ronualdo </t>
-  </si>
-  <si>
-    <t>Javier, Victor </t>
-  </si>
-  <si>
-    <t>3.0.0</t>
-  </si>
-  <si>
-    <t>Joson, Alfonso Miguel</t>
-  </si>
-  <si>
-    <t>0.2.45</t>
-  </si>
-  <si>
-    <t>Keng, Julie</t>
-  </si>
-  <si>
-    <t>8.4.0</t>
-  </si>
-  <si>
-    <t>Laude, Ted Marty</t>
-  </si>
-  <si>
-    <t>Mangundayao, Mac Donald</t>
-  </si>
-  <si>
-    <t>Barter CX</t>
-  </si>
-  <si>
-    <t>0.6.0</t>
-  </si>
-  <si>
-    <t>Matias, Ma. Jeremia Jetheth </t>
-  </si>
-  <si>
-    <t>0.4.15</t>
-  </si>
-  <si>
-    <t>Mendoza, Diana</t>
-  </si>
-  <si>
-    <t>Nagnal, Fracy</t>
-  </si>
-  <si>
-    <t>Newsom, Jifferson</t>
-  </si>
-  <si>
-    <t>3.4.0</t>
-  </si>
-  <si>
-    <t>Pajo, Maricel</t>
-  </si>
-  <si>
-    <t>Pancho, Jona</t>
-  </si>
-  <si>
-    <t>Finance</t>
-  </si>
-  <si>
-    <t>0.5.45</t>
-  </si>
-  <si>
-    <t>Pechuanging, Ma. Antoinette</t>
-  </si>
-  <si>
-    <t>Pendre, Contessa</t>
-  </si>
-  <si>
-    <t>Ranes, Jonathan</t>
-  </si>
-  <si>
-    <t>0.2.30</t>
-  </si>
-  <si>
-    <t>4.0.0</t>
-  </si>
-  <si>
     <t>Reyes, Mark Gil</t>
   </si>
   <si>
     <t>Reyes, Salvador</t>
   </si>
   <si>
-    <t>1.2.0</t>
+    <t>2.3.0</t>
   </si>
   <si>
     <t>Santos, Patricia</t>
@@ -536,16 +521,16 @@
     <t>Enterprise - Primer</t>
   </si>
   <si>
+    <t>1.1.0</t>
+  </si>
+  <si>
     <t>Soriano, Josif Hans</t>
   </si>
   <si>
-    <t>1.1.0</t>
-  </si>
-  <si>
     <t>Suarez, Katrina </t>
   </si>
   <si>
-    <t>5.4.0</t>
+    <t>1.6.0</t>
   </si>
   <si>
     <t>Tesoro, Rose Natalie</t>
@@ -555,9 +540,6 @@
   </si>
   <si>
     <t>Marketing &amp;amp; Hardware</t>
-  </si>
-  <si>
-    <t>8.0.0</t>
   </si>
   <si>
     <t>Viloria, Benito Jr.</t>
@@ -585,7 +567,6 @@
       <sz val="15"/>
       <family val="1"/>
       <b val="true"/>
-      <u val="true"/>
     </font>
     <font>
       <name val="Arial"/>
@@ -680,7 +661,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:CK55"/>
+  <dimension ref="A1:CK54"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0">
       <pane topLeftCell="D4" state="frozenSplit" activePane="bottomRight" ySplit="3" xSplit="3"/>
@@ -1339,19 +1320,19 @@
         <v>81</v>
       </c>
       <c r="F4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="I4" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K4" s="5" t="str">
         <f>INT(LEFT(E4,2))</f>
@@ -1465,7 +1446,7 @@
         <v>81</v>
       </c>
       <c r="AV4" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="AW4" s="5" t="s">
         <v>81</v>
@@ -1573,7 +1554,7 @@
         <f>FLOOR(CC4/8,1)&amp;"."&amp;FLOOR(MOD(CC4,8),1)&amp;"."&amp;(MOD(CC4,8)-FLOOR(MOD(CC4,8),1))*60</f>
       </c>
       <c r="CF4" s="5" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="CG4" s="5" t="str">
         <f>INT(LEFT(CF4,2))</f>
@@ -1596,16 +1577,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>81</v>
@@ -1614,13 +1595,13 @@
         <v>81</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K5" s="5" t="str">
         <f>INT(LEFT(E5,2))</f>
@@ -1842,7 +1823,7 @@
         <f>FLOOR(CC5/8,1)&amp;"."&amp;FLOOR(MOD(CC5,8),1)&amp;"."&amp;(MOD(CC5,8)-FLOOR(MOD(CC5,8),1))*60</f>
       </c>
       <c r="CF5" s="5" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="CG5" s="5" t="str">
         <f>INT(LEFT(CF5,2))</f>
@@ -1865,31 +1846,31 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="I6" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K6" s="5" t="str">
         <f>INT(LEFT(E6,2))</f>
@@ -2134,10 +2115,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D7" s="5" t="n">
         <v>0</v>
@@ -2152,13 +2133,13 @@
         <v>81</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K7" s="5" t="str">
         <f>INT(LEFT(E7,2))</f>
@@ -2380,7 +2361,7 @@
         <f>FLOOR(CC7/8,1)&amp;"."&amp;FLOOR(MOD(CC7,8),1)&amp;"."&amp;(MOD(CC7,8)-FLOOR(MOD(CC7,8),1))*60</f>
       </c>
       <c r="CF7" s="5" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="CG7" s="5" t="str">
         <f>INT(LEFT(CF7,2))</f>
@@ -2403,17 +2384,17 @@
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D8" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>96</v>
-      </c>
       <c r="F8" s="5" t="s">
         <v>81</v>
       </c>
@@ -2421,13 +2402,13 @@
         <v>81</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K8" s="5" t="str">
         <f>INT(LEFT(E8,2))</f>
@@ -2672,31 +2653,31 @@
         <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D9" s="5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>81</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K9" s="5" t="str">
         <f>INT(LEFT(E9,2))</f>
@@ -2918,7 +2899,7 @@
         <f>FLOOR(CC9/8,1)&amp;"."&amp;FLOOR(MOD(CC9,8),1)&amp;"."&amp;(MOD(CC9,8)-FLOOR(MOD(CC9,8),1))*60</f>
       </c>
       <c r="CF9" s="5" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="CG9" s="5" t="str">
         <f>INT(LEFT(CF9,2))</f>
@@ -2941,10 +2922,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D10" s="5" t="n">
         <v>0</v>
@@ -2956,16 +2937,16 @@
         <v>81</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K10" s="5" t="str">
         <f>INT(LEFT(E10,2))</f>
@@ -3076,7 +3057,7 @@
         <f>FLOOR(AS10/8,1)&amp;"."&amp;FLOOR(MOD(AS10,8),1)&amp;"."&amp;(MOD(AS10,8)-FLOOR(MOD(AS10,8),1))*60</f>
       </c>
       <c r="AU10" s="5" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="AV10" s="5" t="s">
         <v>81</v>
@@ -3187,7 +3168,7 @@
         <f>FLOOR(CC10/8,1)&amp;"."&amp;FLOOR(MOD(CC10,8),1)&amp;"."&amp;(MOD(CC10,8)-FLOOR(MOD(CC10,8),1))*60</f>
       </c>
       <c r="CF10" s="5" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="CG10" s="5" t="str">
         <f>INT(LEFT(CF10,2))</f>
@@ -3210,31 +3191,31 @@
         <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="D11" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K11" s="5" t="str">
         <f>INT(LEFT(E11,2))</f>
@@ -3456,7 +3437,7 @@
         <f>FLOOR(CC11/8,1)&amp;"."&amp;FLOOR(MOD(CC11,8),1)&amp;"."&amp;(MOD(CC11,8)-FLOOR(MOD(CC11,8),1))*60</f>
       </c>
       <c r="CF11" s="5" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="CG11" s="5" t="str">
         <f>INT(LEFT(CF11,2))</f>
@@ -3479,31 +3460,31 @@
         <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D12" s="5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K12" s="5" t="str">
         <f>INT(LEFT(E12,2))</f>
@@ -3725,7 +3706,7 @@
         <f>FLOOR(CC12/8,1)&amp;"."&amp;FLOOR(MOD(CC12,8),1)&amp;"."&amp;(MOD(CC12,8)-FLOOR(MOD(CC12,8),1))*60</f>
       </c>
       <c r="CF12" s="5" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="CG12" s="5" t="str">
         <f>INT(LEFT(CF12,2))</f>
@@ -3748,31 +3729,31 @@
         <v>10</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I13" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D13" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>81</v>
-      </c>
       <c r="J13" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K13" s="5" t="str">
         <f>INT(LEFT(E13,2))</f>
@@ -3994,7 +3975,7 @@
         <f>FLOOR(CC13/8,1)&amp;"."&amp;FLOOR(MOD(CC13,8),1)&amp;"."&amp;(MOD(CC13,8)-FLOOR(MOD(CC13,8),1))*60</f>
       </c>
       <c r="CF13" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="CG13" s="5" t="str">
         <f>INT(LEFT(CF13,2))</f>
@@ -4017,10 +3998,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="D14" s="5" t="n">
         <v>0</v>
@@ -4035,13 +4016,13 @@
         <v>81</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K14" s="5" t="str">
         <f>INT(LEFT(E14,2))</f>
@@ -4263,7 +4244,7 @@
         <f>FLOOR(CC14/8,1)&amp;"."&amp;FLOOR(MOD(CC14,8),1)&amp;"."&amp;(MOD(CC14,8)-FLOOR(MOD(CC14,8),1))*60</f>
       </c>
       <c r="CF14" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="CG14" s="5" t="str">
         <f>INT(LEFT(CF14,2))</f>
@@ -4286,17 +4267,17 @@
         <v>12</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D15" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>81</v>
-      </c>
       <c r="F15" s="5" t="s">
         <v>81</v>
       </c>
@@ -4304,13 +4285,13 @@
         <v>81</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K15" s="5" t="str">
         <f>INT(LEFT(E15,2))</f>
@@ -4532,7 +4513,7 @@
         <f>FLOOR(CC15/8,1)&amp;"."&amp;FLOOR(MOD(CC15,8),1)&amp;"."&amp;(MOD(CC15,8)-FLOOR(MOD(CC15,8),1))*60</f>
       </c>
       <c r="CF15" s="5" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="CG15" s="5" t="str">
         <f>INT(LEFT(CF15,2))</f>
@@ -4561,25 +4542,25 @@
         <v>93</v>
       </c>
       <c r="D16" s="5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K16" s="5" t="str">
         <f>INT(LEFT(E16,2))</f>
@@ -4824,10 +4805,10 @@
         <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="D17" s="5" t="n">
         <v>0</v>
@@ -4836,19 +4817,19 @@
         <v>81</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>81</v>
+        <v>116</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K17" s="5" t="str">
         <f>INT(LEFT(E17,2))</f>
@@ -5070,7 +5051,7 @@
         <f>FLOOR(CC17/8,1)&amp;"."&amp;FLOOR(MOD(CC17,8),1)&amp;"."&amp;(MOD(CC17,8)-FLOOR(MOD(CC17,8),1))*60</f>
       </c>
       <c r="CF17" s="5" t="s">
-        <v>81</v>
+        <v>117</v>
       </c>
       <c r="CG17" s="5" t="str">
         <f>INT(LEFT(CF17,2))</f>
@@ -5093,31 +5074,31 @@
         <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D18" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>120</v>
+        <v>81</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K18" s="5" t="str">
         <f>INT(LEFT(E18,2))</f>
@@ -5228,7 +5209,7 @@
         <f>FLOOR(AS18/8,1)&amp;"."&amp;FLOOR(MOD(AS18,8),1)&amp;"."&amp;(MOD(AS18,8)-FLOOR(MOD(AS18,8),1))*60</f>
       </c>
       <c r="AU18" s="5" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="AV18" s="5" t="s">
         <v>81</v>
@@ -5339,7 +5320,7 @@
         <f>FLOOR(CC18/8,1)&amp;"."&amp;FLOOR(MOD(CC18,8),1)&amp;"."&amp;(MOD(CC18,8)-FLOOR(MOD(CC18,8),1))*60</f>
       </c>
       <c r="CF18" s="5" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="CG18" s="5" t="str">
         <f>INT(LEFT(CF18,2))</f>
@@ -5362,16 +5343,16 @@
         <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>122</v>
+        <v>93</v>
       </c>
       <c r="D19" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>81</v>
@@ -5380,13 +5361,13 @@
         <v>81</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K19" s="5" t="str">
         <f>INT(LEFT(E19,2))</f>
@@ -5608,7 +5589,7 @@
         <f>FLOOR(CC19/8,1)&amp;"."&amp;FLOOR(MOD(CC19,8),1)&amp;"."&amp;(MOD(CC19,8)-FLOOR(MOD(CC19,8),1))*60</f>
       </c>
       <c r="CF19" s="5" t="s">
-        <v>123</v>
+        <v>86</v>
       </c>
       <c r="CG19" s="5" t="str">
         <f>INT(LEFT(CF19,2))</f>
@@ -5631,16 +5612,16 @@
         <v>17</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="D20" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>81</v>
@@ -5649,13 +5630,13 @@
         <v>81</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K20" s="5" t="str">
         <f>INT(LEFT(E20,2))</f>
@@ -5766,10 +5747,10 @@
         <f>FLOOR(AS20/8,1)&amp;"."&amp;FLOOR(MOD(AS20,8),1)&amp;"."&amp;(MOD(AS20,8)-FLOOR(MOD(AS20,8),1))*60</f>
       </c>
       <c r="AU20" s="5" t="s">
-        <v>81</v>
+        <v>123</v>
       </c>
       <c r="AV20" s="5" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="AW20" s="5" t="s">
         <v>81</v>
@@ -5877,7 +5858,7 @@
         <f>FLOOR(CC20/8,1)&amp;"."&amp;FLOOR(MOD(CC20,8),1)&amp;"."&amp;(MOD(CC20,8)-FLOOR(MOD(CC20,8),1))*60</f>
       </c>
       <c r="CF20" s="5" t="s">
-        <v>125</v>
+        <v>86</v>
       </c>
       <c r="CG20" s="5" t="str">
         <f>INT(LEFT(CF20,2))</f>
@@ -5900,31 +5881,31 @@
         <v>18</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
       <c r="D21" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K21" s="5" t="str">
         <f>INT(LEFT(E21,2))</f>
@@ -6035,7 +6016,7 @@
         <f>FLOOR(AS21/8,1)&amp;"."&amp;FLOOR(MOD(AS21,8),1)&amp;"."&amp;(MOD(AS21,8)-FLOOR(MOD(AS21,8),1))*60</f>
       </c>
       <c r="AU21" s="5" t="s">
-        <v>119</v>
+        <v>81</v>
       </c>
       <c r="AV21" s="5" t="s">
         <v>81</v>
@@ -6044,7 +6025,7 @@
         <v>81</v>
       </c>
       <c r="AX21" s="5" t="s">
-        <v>128</v>
+        <v>81</v>
       </c>
       <c r="AY21" s="5" t="s">
         <v>81</v>
@@ -6146,7 +6127,7 @@
         <f>FLOOR(CC21/8,1)&amp;"."&amp;FLOOR(MOD(CC21,8),1)&amp;"."&amp;(MOD(CC21,8)-FLOOR(MOD(CC21,8),1))*60</f>
       </c>
       <c r="CF21" s="5" t="s">
-        <v>81</v>
+        <v>125</v>
       </c>
       <c r="CG21" s="5" t="str">
         <f>INT(LEFT(CF21,2))</f>
@@ -6169,10 +6150,10 @@
         <v>19</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="D22" s="5" t="n">
         <v>0</v>
@@ -6181,19 +6162,19 @@
         <v>81</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>130</v>
+        <v>81</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K22" s="5" t="str">
         <f>INT(LEFT(E22,2))</f>
@@ -6415,7 +6396,7 @@
         <f>FLOOR(CC22/8,1)&amp;"."&amp;FLOOR(MOD(CC22,8),1)&amp;"."&amp;(MOD(CC22,8)-FLOOR(MOD(CC22,8),1))*60</f>
       </c>
       <c r="CF22" s="5" t="s">
-        <v>131</v>
+        <v>103</v>
       </c>
       <c r="CG22" s="5" t="str">
         <f>INT(LEFT(CF22,2))</f>
@@ -6438,16 +6419,16 @@
         <v>20</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="D23" s="5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>81</v>
@@ -6456,13 +6437,13 @@
         <v>81</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K23" s="5" t="str">
         <f>INT(LEFT(E23,2))</f>
@@ -6573,7 +6554,7 @@
         <f>FLOOR(AS23/8,1)&amp;"."&amp;FLOOR(MOD(AS23,8),1)&amp;"."&amp;(MOD(AS23,8)-FLOOR(MOD(AS23,8),1))*60</f>
       </c>
       <c r="AU23" s="5" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="AV23" s="5" t="s">
         <v>81</v>
@@ -6684,7 +6665,7 @@
         <f>FLOOR(CC23/8,1)&amp;"."&amp;FLOOR(MOD(CC23,8),1)&amp;"."&amp;(MOD(CC23,8)-FLOOR(MOD(CC23,8),1))*60</f>
       </c>
       <c r="CF23" s="5" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="CG23" s="5" t="str">
         <f>INT(LEFT(CF23,2))</f>
@@ -6707,31 +6688,31 @@
         <v>21</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="D24" s="5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E24" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H24" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="I24" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K24" s="5" t="str">
         <f>INT(LEFT(E24,2))</f>
@@ -6953,7 +6934,7 @@
         <f>FLOOR(CC24/8,1)&amp;"."&amp;FLOOR(MOD(CC24,8),1)&amp;"."&amp;(MOD(CC24,8)-FLOOR(MOD(CC24,8),1))*60</f>
       </c>
       <c r="CF24" s="5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="CG24" s="5" t="str">
         <f>INT(LEFT(CF24,2))</f>
@@ -6976,16 +6957,16 @@
         <v>22</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="D25" s="5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>81</v>
@@ -6994,13 +6975,13 @@
         <v>81</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K25" s="5" t="str">
         <f>INT(LEFT(E25,2))</f>
@@ -7114,7 +7095,7 @@
         <v>81</v>
       </c>
       <c r="AV25" s="5" t="s">
-        <v>81</v>
+        <v>135</v>
       </c>
       <c r="AW25" s="5" t="s">
         <v>81</v>
@@ -7222,7 +7203,7 @@
         <f>FLOOR(CC25/8,1)&amp;"."&amp;FLOOR(MOD(CC25,8),1)&amp;"."&amp;(MOD(CC25,8)-FLOOR(MOD(CC25,8),1))*60</f>
       </c>
       <c r="CF25" s="5" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="CG25" s="5" t="str">
         <f>INT(LEFT(CF25,2))</f>
@@ -7245,31 +7226,31 @@
         <v>23</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>127</v>
-      </c>
       <c r="D26" s="5" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>138</v>
+        <v>81</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>81</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K26" s="5" t="str">
         <f>INT(LEFT(E26,2))</f>
@@ -7491,7 +7472,7 @@
         <f>FLOOR(CC26/8,1)&amp;"."&amp;FLOOR(MOD(CC26,8),1)&amp;"."&amp;(MOD(CC26,8)-FLOOR(MOD(CC26,8),1))*60</f>
       </c>
       <c r="CF26" s="5" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="CG26" s="5" t="str">
         <f>INT(LEFT(CF26,2))</f>
@@ -7514,10 +7495,10 @@
         <v>24</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>140</v>
+        <v>84</v>
       </c>
       <c r="D27" s="5" t="n">
         <v>0</v>
@@ -7532,13 +7513,13 @@
         <v>81</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K27" s="5" t="str">
         <f>INT(LEFT(E27,2))</f>
@@ -7649,7 +7630,7 @@
         <f>FLOOR(AS27/8,1)&amp;"."&amp;FLOOR(MOD(AS27,8),1)&amp;"."&amp;(MOD(AS27,8)-FLOOR(MOD(AS27,8),1))*60</f>
       </c>
       <c r="AU27" s="5" t="s">
-        <v>81</v>
+        <v>139</v>
       </c>
       <c r="AV27" s="5" t="s">
         <v>81</v>
@@ -7760,7 +7741,7 @@
         <f>FLOOR(CC27/8,1)&amp;"."&amp;FLOOR(MOD(CC27,8),1)&amp;"."&amp;(MOD(CC27,8)-FLOOR(MOD(CC27,8),1))*60</f>
       </c>
       <c r="CF27" s="5" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="CG27" s="5" t="str">
         <f>INT(LEFT(CF27,2))</f>
@@ -7783,31 +7764,31 @@
         <v>25</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D28" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E28" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H28" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F28" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="I28" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="K28" s="5" t="str">
         <f>INT(LEFT(E28,2))</f>
@@ -8029,7 +8010,7 @@
         <f>FLOOR(CC28/8,1)&amp;"."&amp;FLOOR(MOD(CC28,8),1)&amp;"."&amp;(MOD(CC28,8)-FLOOR(MOD(CC28,8),1))*60</f>
       </c>
       <c r="CF28" s="5" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="CG28" s="5" t="str">
         <f>INT(LEFT(CF28,2))</f>
@@ -8052,31 +8033,31 @@
         <v>26</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
       <c r="D29" s="5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E29" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H29" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F29" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="I29" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K29" s="5" t="str">
         <f>INT(LEFT(E29,2))</f>
@@ -8298,7 +8279,7 @@
         <f>FLOOR(CC29/8,1)&amp;"."&amp;FLOOR(MOD(CC29,8),1)&amp;"."&amp;(MOD(CC29,8)-FLOOR(MOD(CC29,8),1))*60</f>
       </c>
       <c r="CF29" s="5" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="CG29" s="5" t="str">
         <f>INT(LEFT(CF29,2))</f>
@@ -8324,7 +8305,7 @@
         <v>143</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>133</v>
+        <v>80</v>
       </c>
       <c r="D30" s="5" t="n">
         <v>0</v>
@@ -8339,13 +8320,13 @@
         <v>81</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I30" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K30" s="5" t="str">
         <f>INT(LEFT(E30,2))</f>
@@ -8468,7 +8449,7 @@
         <v>81</v>
       </c>
       <c r="AY30" s="5" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="AZ30" s="5" t="str">
         <f>INT(LEFT(AU30,1))</f>
@@ -8567,7 +8548,7 @@
         <f>FLOOR(CC30/8,1)&amp;"."&amp;FLOOR(MOD(CC30,8),1)&amp;"."&amp;(MOD(CC30,8)-FLOOR(MOD(CC30,8),1))*60</f>
       </c>
       <c r="CF30" s="5" t="s">
-        <v>144</v>
+        <v>81</v>
       </c>
       <c r="CG30" s="5" t="str">
         <f>INT(LEFT(CF30,2))</f>
@@ -8590,16 +8571,16 @@
         <v>28</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>80</v>
+        <v>127</v>
       </c>
       <c r="D31" s="5" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>146</v>
+        <v>81</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>81</v>
@@ -8608,13 +8589,13 @@
         <v>81</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K31" s="5" t="str">
         <f>INT(LEFT(E31,2))</f>
@@ -8725,7 +8706,7 @@
         <f>FLOOR(AS31/8,1)&amp;"."&amp;FLOOR(MOD(AS31,8),1)&amp;"."&amp;(MOD(AS31,8)-FLOOR(MOD(AS31,8),1))*60</f>
       </c>
       <c r="AU31" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="AV31" s="5" t="s">
         <v>81</v>
@@ -8836,7 +8817,7 @@
         <f>FLOOR(CC31/8,1)&amp;"."&amp;FLOOR(MOD(CC31,8),1)&amp;"."&amp;(MOD(CC31,8)-FLOOR(MOD(CC31,8),1))*60</f>
       </c>
       <c r="CF31" s="5" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="CG31" s="5" t="str">
         <f>INT(LEFT(CF31,2))</f>
@@ -8859,10 +8840,10 @@
         <v>29</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>133</v>
+        <v>80</v>
       </c>
       <c r="D32" s="5" t="n">
         <v>0</v>
@@ -8877,13 +8858,13 @@
         <v>81</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I32" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K32" s="5" t="str">
         <f>INT(LEFT(E32,2))</f>
@@ -9105,7 +9086,7 @@
         <f>FLOOR(CC32/8,1)&amp;"."&amp;FLOOR(MOD(CC32,8),1)&amp;"."&amp;(MOD(CC32,8)-FLOOR(MOD(CC32,8),1))*60</f>
       </c>
       <c r="CF32" s="5" t="s">
-        <v>148</v>
+        <v>81</v>
       </c>
       <c r="CG32" s="5" t="str">
         <f>INT(LEFT(CF32,2))</f>
@@ -9128,16 +9109,16 @@
         <v>30</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>80</v>
+        <v>147</v>
       </c>
       <c r="D33" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>103</v>
+        <v>148</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>81</v>
@@ -9146,13 +9127,13 @@
         <v>81</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K33" s="5" t="str">
         <f>INT(LEFT(E33,2))</f>
@@ -9263,7 +9244,7 @@
         <f>FLOOR(AS33/8,1)&amp;"."&amp;FLOOR(MOD(AS33,8),1)&amp;"."&amp;(MOD(AS33,8)-FLOOR(MOD(AS33,8),1))*60</f>
       </c>
       <c r="AU33" s="5" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="AV33" s="5" t="s">
         <v>81</v>
@@ -9374,7 +9355,7 @@
         <f>FLOOR(CC33/8,1)&amp;"."&amp;FLOOR(MOD(CC33,8),1)&amp;"."&amp;(MOD(CC33,8)-FLOOR(MOD(CC33,8),1))*60</f>
       </c>
       <c r="CF33" s="5" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="CG33" s="5" t="str">
         <f>INT(LEFT(CF33,2))</f>
@@ -9397,31 +9378,31 @@
         <v>31</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="D34" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>146</v>
-      </c>
       <c r="F34" s="5" t="s">
-        <v>130</v>
+        <v>81</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K34" s="5" t="str">
         <f>INT(LEFT(E34,2))</f>
@@ -9532,7 +9513,7 @@
         <f>FLOOR(AS34/8,1)&amp;"."&amp;FLOOR(MOD(AS34,8),1)&amp;"."&amp;(MOD(AS34,8)-FLOOR(MOD(AS34,8),1))*60</f>
       </c>
       <c r="AU34" s="5" t="s">
-        <v>152</v>
+        <v>81</v>
       </c>
       <c r="AV34" s="5" t="s">
         <v>81</v>
@@ -9643,7 +9624,7 @@
         <f>FLOOR(CC34/8,1)&amp;"."&amp;FLOOR(MOD(CC34,8),1)&amp;"."&amp;(MOD(CC34,8)-FLOOR(MOD(CC34,8),1))*60</f>
       </c>
       <c r="CF34" s="5" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="CG34" s="5" t="str">
         <f>INT(LEFT(CF34,2))</f>
@@ -9666,16 +9647,16 @@
         <v>32</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="D35" s="5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>81</v>
@@ -9684,13 +9665,13 @@
         <v>81</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K35" s="5" t="str">
         <f>INT(LEFT(E35,2))</f>
@@ -9912,7 +9893,7 @@
         <f>FLOOR(CC35/8,1)&amp;"."&amp;FLOOR(MOD(CC35,8),1)&amp;"."&amp;(MOD(CC35,8)-FLOOR(MOD(CC35,8),1))*60</f>
       </c>
       <c r="CF35" s="5" t="s">
-        <v>115</v>
+        <v>153</v>
       </c>
       <c r="CG35" s="5" t="str">
         <f>INT(LEFT(CF35,2))</f>
@@ -9935,16 +9916,16 @@
         <v>33</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D36" s="5" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>81</v>
@@ -9953,13 +9934,13 @@
         <v>81</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I36" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K36" s="5" t="str">
         <f>INT(LEFT(E36,2))</f>
@@ -10181,7 +10162,7 @@
         <f>FLOOR(CC36/8,1)&amp;"."&amp;FLOOR(MOD(CC36,8),1)&amp;"."&amp;(MOD(CC36,8)-FLOOR(MOD(CC36,8),1))*60</f>
       </c>
       <c r="CF36" s="5" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="CG36" s="5" t="str">
         <f>INT(LEFT(CF36,2))</f>
@@ -10204,10 +10185,10 @@
         <v>34</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="D37" s="5" t="n">
         <v>0</v>
@@ -10222,13 +10203,13 @@
         <v>81</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I37" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K37" s="5" t="str">
         <f>INT(LEFT(E37,2))</f>
@@ -10339,7 +10320,7 @@
         <f>FLOOR(AS37/8,1)&amp;"."&amp;FLOOR(MOD(AS37,8),1)&amp;"."&amp;(MOD(AS37,8)-FLOOR(MOD(AS37,8),1))*60</f>
       </c>
       <c r="AU37" s="5" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="AV37" s="5" t="s">
         <v>81</v>
@@ -10450,7 +10431,7 @@
         <f>FLOOR(CC37/8,1)&amp;"."&amp;FLOOR(MOD(CC37,8),1)&amp;"."&amp;(MOD(CC37,8)-FLOOR(MOD(CC37,8),1))*60</f>
       </c>
       <c r="CF37" s="5" t="s">
-        <v>125</v>
+        <v>86</v>
       </c>
       <c r="CG37" s="5" t="str">
         <f>INT(LEFT(CF37,2))</f>
@@ -10473,10 +10454,10 @@
         <v>35</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D38" s="5" t="n">
         <v>0</v>
@@ -10491,13 +10472,13 @@
         <v>81</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I38" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K38" s="5" t="str">
         <f>INT(LEFT(E38,2))</f>
@@ -10719,7 +10700,7 @@
         <f>FLOOR(CC38/8,1)&amp;"."&amp;FLOOR(MOD(CC38,8),1)&amp;"."&amp;(MOD(CC38,8)-FLOOR(MOD(CC38,8),1))*60</f>
       </c>
       <c r="CF38" s="5" t="s">
-        <v>158</v>
+        <v>91</v>
       </c>
       <c r="CG38" s="5" t="str">
         <f>INT(LEFT(CF38,2))</f>
@@ -10742,16 +10723,16 @@
         <v>36</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>105</v>
+        <v>158</v>
       </c>
       <c r="D39" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>81</v>
@@ -10760,13 +10741,13 @@
         <v>81</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K39" s="5" t="str">
         <f>INT(LEFT(E39,2))</f>
@@ -10988,7 +10969,7 @@
         <f>FLOOR(CC39/8,1)&amp;"."&amp;FLOOR(MOD(CC39,8),1)&amp;"."&amp;(MOD(CC39,8)-FLOOR(MOD(CC39,8),1))*60</f>
       </c>
       <c r="CF39" s="5" t="s">
-        <v>144</v>
+        <v>91</v>
       </c>
       <c r="CG39" s="5" t="str">
         <f>INT(LEFT(CF39,2))</f>
@@ -11011,16 +10992,16 @@
         <v>37</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D40" s="5" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>162</v>
+        <v>81</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>81</v>
@@ -11029,13 +11010,13 @@
         <v>81</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I40" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K40" s="5" t="str">
         <f>INT(LEFT(E40,2))</f>
@@ -11257,7 +11238,7 @@
         <f>FLOOR(CC40/8,1)&amp;"."&amp;FLOOR(MOD(CC40,8),1)&amp;"."&amp;(MOD(CC40,8)-FLOOR(MOD(CC40,8),1))*60</f>
       </c>
       <c r="CF40" s="5" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="CG40" s="5" t="str">
         <f>INT(LEFT(CF40,2))</f>
@@ -11280,10 +11261,10 @@
         <v>38</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>161</v>
+        <v>99</v>
       </c>
       <c r="D41" s="5" t="n">
         <v>0</v>
@@ -11298,13 +11279,13 @@
         <v>81</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I41" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K41" s="5" t="str">
         <f>INT(LEFT(E41,2))</f>
@@ -11526,7 +11507,7 @@
         <f>FLOOR(CC41/8,1)&amp;"."&amp;FLOOR(MOD(CC41,8),1)&amp;"."&amp;(MOD(CC41,8)-FLOOR(MOD(CC41,8),1))*60</f>
       </c>
       <c r="CF41" s="5" t="s">
-        <v>81</v>
+        <v>117</v>
       </c>
       <c r="CG41" s="5" t="str">
         <f>INT(LEFT(CF41,2))</f>
@@ -11549,16 +11530,16 @@
         <v>39</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D42" s="5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>81</v>
+        <v>162</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>81</v>
@@ -11567,13 +11548,13 @@
         <v>81</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I42" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K42" s="5" t="str">
         <f>INT(LEFT(E42,2))</f>
@@ -11795,7 +11776,7 @@
         <f>FLOOR(CC42/8,1)&amp;"."&amp;FLOOR(MOD(CC42,8),1)&amp;"."&amp;(MOD(CC42,8)-FLOOR(MOD(CC42,8),1))*60</f>
       </c>
       <c r="CF42" s="5" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
       <c r="CG42" s="5" t="str">
         <f>INT(LEFT(CF42,2))</f>
@@ -11818,31 +11799,31 @@
         <v>40</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="D43" s="5" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="F43" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H43" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="G43" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="H43" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="I43" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K43" s="5" t="str">
         <f>INT(LEFT(E43,2))</f>
@@ -12064,7 +12045,7 @@
         <f>FLOOR(CC43/8,1)&amp;"."&amp;FLOOR(MOD(CC43,8),1)&amp;"."&amp;(MOD(CC43,8)-FLOOR(MOD(CC43,8),1))*60</f>
       </c>
       <c r="CF43" s="5" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="CG43" s="5" t="str">
         <f>INT(LEFT(CF43,2))</f>
@@ -12087,16 +12068,16 @@
         <v>41</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D44" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>114</v>
+        <v>148</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>81</v>
@@ -12105,13 +12086,13 @@
         <v>81</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I44" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K44" s="5" t="str">
         <f>INT(LEFT(E44,2))</f>
@@ -12222,7 +12203,7 @@
         <f>FLOOR(AS44/8,1)&amp;"."&amp;FLOOR(MOD(AS44,8),1)&amp;"."&amp;(MOD(AS44,8)-FLOOR(MOD(AS44,8),1))*60</f>
       </c>
       <c r="AU44" s="5" t="s">
-        <v>81</v>
+        <v>165</v>
       </c>
       <c r="AV44" s="5" t="s">
         <v>81</v>
@@ -12333,7 +12314,7 @@
         <f>FLOOR(CC44/8,1)&amp;"."&amp;FLOOR(MOD(CC44,8),1)&amp;"."&amp;(MOD(CC44,8)-FLOOR(MOD(CC44,8),1))*60</f>
       </c>
       <c r="CF44" s="5" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="CG44" s="5" t="str">
         <f>INT(LEFT(CF44,2))</f>
@@ -12356,31 +12337,31 @@
         <v>42</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="D45" s="5" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>138</v>
+        <v>81</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>120</v>
+        <v>81</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I45" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K45" s="5" t="str">
         <f>INT(LEFT(E45,2))</f>
@@ -12491,10 +12472,10 @@
         <f>FLOOR(AS45/8,1)&amp;"."&amp;FLOOR(MOD(AS45,8),1)&amp;"."&amp;(MOD(AS45,8)-FLOOR(MOD(AS45,8),1))*60</f>
       </c>
       <c r="AU45" s="5" t="s">
-        <v>170</v>
+        <v>81</v>
       </c>
       <c r="AV45" s="5" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="AW45" s="5" t="s">
         <v>81</v>
@@ -12602,7 +12583,7 @@
         <f>FLOOR(CC45/8,1)&amp;"."&amp;FLOOR(MOD(CC45,8),1)&amp;"."&amp;(MOD(CC45,8)-FLOOR(MOD(CC45,8),1))*60</f>
       </c>
       <c r="CF45" s="5" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="CG45" s="5" t="str">
         <f>INT(LEFT(CF45,2))</f>
@@ -12625,31 +12606,31 @@
         <v>43</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D46" s="5" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>146</v>
+        <v>81</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>120</v>
+        <v>81</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I46" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K46" s="5" t="str">
         <f>INT(LEFT(E46,2))</f>
@@ -12871,7 +12852,7 @@
         <f>FLOOR(CC46/8,1)&amp;"."&amp;FLOOR(MOD(CC46,8),1)&amp;"."&amp;(MOD(CC46,8)-FLOOR(MOD(CC46,8),1))*60</f>
       </c>
       <c r="CF46" s="5" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="CG46" s="5" t="str">
         <f>INT(LEFT(CF46,2))</f>
@@ -12894,10 +12875,10 @@
         <v>44</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>122</v>
+        <v>169</v>
       </c>
       <c r="D47" s="5" t="n">
         <v>0</v>
@@ -12906,19 +12887,19 @@
         <v>81</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>81</v>
+        <v>148</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I47" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K47" s="5" t="str">
         <f>INT(LEFT(E47,2))</f>
@@ -13029,7 +13010,7 @@
         <f>FLOOR(AS47/8,1)&amp;"."&amp;FLOOR(MOD(AS47,8),1)&amp;"."&amp;(MOD(AS47,8)-FLOOR(MOD(AS47,8),1))*60</f>
       </c>
       <c r="AU47" s="5" t="s">
-        <v>81</v>
+        <v>170</v>
       </c>
       <c r="AV47" s="5" t="s">
         <v>81</v>
@@ -13140,7 +13121,7 @@
         <f>FLOOR(CC47/8,1)&amp;"."&amp;FLOOR(MOD(CC47,8),1)&amp;"."&amp;(MOD(CC47,8)-FLOOR(MOD(CC47,8),1))*60</f>
       </c>
       <c r="CF47" s="5" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="CG47" s="5" t="str">
         <f>INT(LEFT(CF47,2))</f>
@@ -13163,31 +13144,31 @@
         <v>45</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>174</v>
+        <v>147</v>
       </c>
       <c r="D48" s="5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I48" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K48" s="5" t="str">
         <f>INT(LEFT(E48,2))</f>
@@ -13298,7 +13279,7 @@
         <f>FLOOR(AS48/8,1)&amp;"."&amp;FLOOR(MOD(AS48,8),1)&amp;"."&amp;(MOD(AS48,8)-FLOOR(MOD(AS48,8),1))*60</f>
       </c>
       <c r="AU48" s="5" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="AV48" s="5" t="s">
         <v>81</v>
@@ -13409,7 +13390,7 @@
         <f>FLOOR(CC48/8,1)&amp;"."&amp;FLOOR(MOD(CC48,8),1)&amp;"."&amp;(MOD(CC48,8)-FLOOR(MOD(CC48,8),1))*60</f>
       </c>
       <c r="CF48" s="5" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="CG48" s="5" t="str">
         <f>INT(LEFT(CF48,2))</f>
@@ -13432,16 +13413,16 @@
         <v>46</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>151</v>
+        <v>97</v>
       </c>
       <c r="D49" s="5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>146</v>
+        <v>81</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>81</v>
@@ -13450,13 +13431,13 @@
         <v>81</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I49" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K49" s="5" t="str">
         <f>INT(LEFT(E49,2))</f>
@@ -13567,10 +13548,10 @@
         <f>FLOOR(AS49/8,1)&amp;"."&amp;FLOOR(MOD(AS49,8),1)&amp;"."&amp;(MOD(AS49,8)-FLOOR(MOD(AS49,8),1))*60</f>
       </c>
       <c r="AU49" s="5" t="s">
-        <v>115</v>
+        <v>173</v>
       </c>
       <c r="AV49" s="5" t="s">
-        <v>176</v>
+        <v>81</v>
       </c>
       <c r="AW49" s="5" t="s">
         <v>81</v>
@@ -13678,7 +13659,7 @@
         <f>FLOOR(CC49/8,1)&amp;"."&amp;FLOOR(MOD(CC49,8),1)&amp;"."&amp;(MOD(CC49,8)-FLOOR(MOD(CC49,8),1))*60</f>
       </c>
       <c r="CF49" s="5" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="CG49" s="5" t="str">
         <f>INT(LEFT(CF49,2))</f>
@@ -13701,31 +13682,31 @@
         <v>47</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="D50" s="5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>166</v>
+        <v>81</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>81</v>
+        <v>148</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I50" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>178</v>
+        <v>82</v>
       </c>
       <c r="K50" s="5" t="str">
         <f>INT(LEFT(E50,2))</f>
@@ -13836,7 +13817,7 @@
         <f>FLOOR(AS50/8,1)&amp;"."&amp;FLOOR(MOD(AS50,8),1)&amp;"."&amp;(MOD(AS50,8)-FLOOR(MOD(AS50,8),1))*60</f>
       </c>
       <c r="AU50" s="5" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="AV50" s="5" t="s">
         <v>81</v>
@@ -13947,7 +13928,7 @@
         <f>FLOOR(CC50/8,1)&amp;"."&amp;FLOOR(MOD(CC50,8),1)&amp;"."&amp;(MOD(CC50,8)-FLOOR(MOD(CC50,8),1))*60</f>
       </c>
       <c r="CF50" s="5" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="CG50" s="5" t="str">
         <f>INT(LEFT(CF50,2))</f>
@@ -13970,10 +13951,10 @@
         <v>48</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>88</v>
+        <v>176</v>
       </c>
       <c r="D51" s="5" t="n">
         <v>0</v>
@@ -13988,13 +13969,13 @@
         <v>81</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I51" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K51" s="5" t="str">
         <f>INT(LEFT(E51,2))</f>
@@ -14216,7 +14197,7 @@
         <f>FLOOR(CC51/8,1)&amp;"."&amp;FLOOR(MOD(CC51,8),1)&amp;"."&amp;(MOD(CC51,8)-FLOOR(MOD(CC51,8),1))*60</f>
       </c>
       <c r="CF51" s="5" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="CG51" s="5" t="str">
         <f>INT(LEFT(CF51,2))</f>
@@ -14239,10 +14220,10 @@
         <v>49</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>181</v>
+        <v>93</v>
       </c>
       <c r="D52" s="5" t="n">
         <v>0</v>
@@ -14257,13 +14238,13 @@
         <v>81</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I52" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K52" s="5" t="str">
         <f>INT(LEFT(E52,2))</f>
@@ -14485,7 +14466,7 @@
         <f>FLOOR(CC52/8,1)&amp;"."&amp;FLOOR(MOD(CC52,8),1)&amp;"."&amp;(MOD(CC52,8)-FLOOR(MOD(CC52,8),1))*60</f>
       </c>
       <c r="CF52" s="5" t="s">
-        <v>182</v>
+        <v>103</v>
       </c>
       <c r="CG52" s="5" t="str">
         <f>INT(LEFT(CF52,2))</f>
@@ -14508,10 +14489,10 @@
         <v>50</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="D53" s="5" t="n">
         <v>0</v>
@@ -14526,13 +14507,13 @@
         <v>81</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I53" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K53" s="5" t="str">
         <f>INT(LEFT(E53,2))</f>
@@ -14754,7 +14735,7 @@
         <f>FLOOR(CC53/8,1)&amp;"."&amp;FLOOR(MOD(CC53,8),1)&amp;"."&amp;(MOD(CC53,8)-FLOOR(MOD(CC53,8),1))*60</f>
       </c>
       <c r="CF53" s="5" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
       <c r="CG53" s="5" t="str">
         <f>INT(LEFT(CF53,2))</f>
@@ -14773,540 +14754,271 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D54" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="G54" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="H54" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="J54" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="K54" s="5" t="str">
-        <f>INT(LEFT(E54,2))</f>
-      </c>
-      <c r="L54" s="5" t="str">
-        <f>INT(LEFT(F54,2))</f>
-      </c>
-      <c r="M54" s="5" t="str">
-        <f>INT(LEFT(I54,2))</f>
-      </c>
-      <c r="N54" s="5" t="str">
-        <f>INT(LEFT(G54,2))</f>
-      </c>
-      <c r="O54" s="5" t="str">
-        <f>INT(LEFT(J54,2))</f>
-      </c>
-      <c r="P54" s="5" t="str">
-        <f>INT(LEFT(H54,2))</f>
-      </c>
-      <c r="Q54" s="5" t="str">
-        <f>K54+L54+CG54+IF(M54&gt;O54,M54-O54,0)+IF(N54&gt;P54,N54-P54,0)</f>
-      </c>
-      <c r="R54" s="5" t="str">
-        <f>IF(LEFT(RIGHT(E54,LEN(E54)-2),1)=".",RIGHT(E54,LEN(E54)-3),RIGHT(E54,LEN(E54)-2))</f>
-      </c>
-      <c r="S54" s="5" t="str">
-        <f>IF(LEFT(RIGHT(F54,LEN(F54)-2),1)=".",RIGHT(F54,LEN(F54)-3),RIGHT(F54,LEN(F54)-2))</f>
-      </c>
-      <c r="T54" s="5" t="str">
-        <f>IF(LEFT(RIGHT(I54,LEN(I54)-2),1)=".",RIGHT(I54,LEN(I54)-3),RIGHT(I54,LEN(I54)-2))</f>
-      </c>
-      <c r="U54" s="5" t="str">
-        <f>IF(LEFT(RIGHT(G54,LEN(G54)-2),1)=".",RIGHT(G54,LEN(G54)-3),RIGHT(G54,LEN(G54)-2))</f>
-      </c>
-      <c r="V54" s="5" t="str">
-        <f>IF(LEFT(RIGHT(J54,LEN(J54)-2),1)=".",RIGHT(J54,LEN(J54)-3),RIGHT(J54,LEN(J54)-2))</f>
-      </c>
-      <c r="W54" s="5" t="str">
-        <f>IF(LEFT(RIGHT(H54,LEN(H54)-2),1)=".",RIGHT(H54,LEN(H54)-3),RIGHT(H54,LEN(H54)-2))</f>
-      </c>
-      <c r="X54" s="5" t="str">
-        <f>INT(LEFT(R54,1))</f>
-      </c>
-      <c r="Y54" s="5" t="str">
-        <f>INT(LEFT(S54,1))</f>
-      </c>
-      <c r="Z54" s="5" t="str">
-        <f>INT(LEFT(T54,1))</f>
-      </c>
-      <c r="AA54" s="5" t="str">
-        <f>INT(LEFT(U54,1))</f>
-      </c>
-      <c r="AB54" s="5" t="str">
-        <f>INT(LEFT(V54,1))</f>
-      </c>
-      <c r="AC54" s="5" t="str">
-        <f>INT(LEFT(W54,1))</f>
-      </c>
-      <c r="AD54" s="5" t="str">
-        <f>R54+S54+CH54+IF(T54&gt;V54,T54-V54,0)+IF(U54&gt;W54,U54-W54,0)</f>
-      </c>
-      <c r="AE54" s="5" t="str">
-        <f>RIGHT(R54,LEN(R54)-2)+0</f>
-      </c>
-      <c r="AF54" s="5" t="str">
-        <f>RIGHT(S54,LEN(S54)-2)+0</f>
-      </c>
-      <c r="AG54" s="5" t="str">
-        <f>RIGHT(T54,LEN(T54)-2)+0</f>
-      </c>
-      <c r="AH54" s="5" t="str">
-        <f>RIGHT(U54,LEN(U54)-2)+0</f>
-      </c>
-      <c r="AI54" s="5" t="str">
-        <f>RIGHT(V54,LEN(V54)-2)+0</f>
-      </c>
-      <c r="AJ54" s="5" t="str">
-        <f>RIGHT(W54,LEN(W54)-2)+0</f>
-      </c>
-      <c r="AK54" s="5" t="str">
-        <f>AE54+AF54+CJ54+IF(AG54&gt;AI54,AG54-AI54,0)+IF(AH54&gt;AJ54,AH54-AJ54,0)</f>
-      </c>
-      <c r="AL54" s="5" t="str">
-        <f>K54*8*60+X54*60+AE54</f>
-      </c>
-      <c r="AM54" s="5" t="str">
-        <f>L54*8*60+Y54*60+AF54</f>
-      </c>
-      <c r="AN54" s="5" t="str">
-        <f>M54*8*60+Z54*60+AG54</f>
-      </c>
-      <c r="AO54" s="5" t="str">
-        <f>N54*8*60+AA54*60+AH54</f>
-      </c>
-      <c r="AP54" s="5" t="str">
-        <f>O54*8*60+AB54*60+AI54</f>
-      </c>
-      <c r="AQ54" s="5" t="str">
-        <f>P54*8*60+AC54*60+AJ54</f>
-      </c>
-      <c r="AR54" s="5" t="str">
-        <f>AL54+AM54+CK54+IF(AN54&gt;AP54,AN54-AP54,0)+IF(AO54&gt;AQ54,AO54-AQ54,0)</f>
-      </c>
-      <c r="AS54" s="5" t="str">
-        <f>AR54/60</f>
-      </c>
-      <c r="AT54" s="5" t="str">
-        <f>FLOOR(AS54/8,1)&amp;"."&amp;FLOOR(MOD(AS54,8),1)&amp;"."&amp;(MOD(AS54,8)-FLOOR(MOD(AS54,8),1))*60</f>
-      </c>
-      <c r="AU54" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="AV54" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="AW54" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="AX54" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="AY54" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="AZ54" s="5" t="str">
-        <f>INT(LEFT(AU54,1))</f>
-      </c>
-      <c r="BA54" s="5" t="str">
-        <f>INT(LEFT(AV54,1))</f>
-      </c>
-      <c r="BB54" s="5" t="str">
-        <f>INT(LEFT(AW54,1))</f>
-      </c>
-      <c r="BC54" s="5" t="str">
-        <f>INT(LEFT(AX54,1))</f>
-      </c>
-      <c r="BD54" s="5" t="str">
-        <f>INT(LEFT(AY54,1))</f>
-      </c>
-      <c r="BE54" s="5" t="str">
-        <f>SUM(AZ54,BA54,BB54,BC54,BD54)</f>
-      </c>
-      <c r="BF54" s="5" t="str">
-        <f>RIGHT(AU54,LEN(AU54)-2)</f>
-      </c>
-      <c r="BG54" s="5" t="str">
-        <f>RIGHT(AV54,LEN(AV54)-2)</f>
-      </c>
-      <c r="BH54" s="5" t="str">
-        <f>RIGHT(AW54,LEN(AW54)-2)</f>
-      </c>
-      <c r="BI54" s="5" t="str">
-        <f>RIGHT(AX54,LEN(AX54)-2)</f>
-      </c>
-      <c r="BJ54" s="5" t="str">
-        <f>RIGHT(AY54,LEN(AY54)-2)</f>
-      </c>
-      <c r="BK54" s="5" t="str">
-        <f>INT(LEFT(BF54,1))</f>
-      </c>
-      <c r="BL54" s="5" t="str">
-        <f>INT(LEFT(BG54,1))</f>
-      </c>
-      <c r="BM54" s="5" t="str">
-        <f>INT(LEFT(BH54,1))</f>
-      </c>
-      <c r="BN54" s="5" t="str">
-        <f>INT(LEFT(BI54,1))</f>
-      </c>
-      <c r="BO54" s="5" t="str">
-        <f>INT(LEFT(BJ54,1))</f>
-      </c>
-      <c r="BP54" s="5" t="str">
-        <f>SUM(BK54:BO54)</f>
-      </c>
-      <c r="BQ54" s="5" t="str">
-        <f>RIGHT(BF54,LEN(BF54)-2)+0</f>
-      </c>
-      <c r="BR54" s="5" t="str">
-        <f>RIGHT(BG54,LEN(BG54)-2)+0</f>
-      </c>
-      <c r="BS54" s="5" t="str">
-        <f>RIGHT(BH54,LEN(BH54)-2)+0</f>
-      </c>
-      <c r="BT54" s="5" t="str">
-        <f>RIGHT(BI54,LEN(BI54)-2)+0</f>
-      </c>
-      <c r="BU54" s="5" t="str">
-        <f>RIGHT(BJ54,LEN(BJ54)-2)+0</f>
-      </c>
-      <c r="BV54" s="5" t="str">
-        <f>SUM(BQ54:BU54)</f>
-      </c>
-      <c r="BW54" s="5" t="str">
-        <f>AZ54*8*60+BK54*60+BQ54</f>
-      </c>
-      <c r="BX54" s="5" t="str">
-        <f>BA54*8*60+BL54*60+BR54</f>
-      </c>
-      <c r="BY54" s="5" t="str">
-        <f>BB54*8*60+BM54*60+BS54</f>
-      </c>
-      <c r="BZ54" s="5" t="str">
-        <f>BC54*8*60+BN54*60+BT54</f>
-      </c>
-      <c r="CA54" s="5" t="str">
-        <f>BD54*8*60+BO54*60+BU54</f>
-      </c>
-      <c r="CB54" s="5" t="str">
-        <f>SUM(BW54:CA54)</f>
-      </c>
-      <c r="CC54" s="5" t="str">
-        <f>CB54/60</f>
-      </c>
-      <c r="CD54" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CE54" s="5" t="str">
-        <f>FLOOR(CC54/8,1)&amp;"."&amp;FLOOR(MOD(CC54,8),1)&amp;"."&amp;(MOD(CC54,8)-FLOOR(MOD(CC54,8),1))*60</f>
-      </c>
-      <c r="CF54" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="CG54" s="5" t="str">
-        <f>INT(LEFT(CF54,2))</f>
-      </c>
-      <c r="CH54" s="5" t="str">
-        <f>IF(LEFT(RIGHT(CF54,LEN(CF54)-2),1)=".",RIGHT(CF54,LEN(CF54)-3),RIGHT(CF54,LEN(CF54)-2))</f>
-      </c>
-      <c r="CI54" s="5" t="str">
-        <f>INT(LEFT(CH54,1))</f>
-      </c>
-      <c r="CJ54" s="5" t="str">
-        <f>RIGHT(CH54,LEN(CH54)-2)+0</f>
-      </c>
-      <c r="CK54" s="5" t="str">
-        <f>CG54*8*60+CI54*60+CJ54</f>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="I55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="J55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="K55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="L55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="M55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="N55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="O55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="P55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="R55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="S55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="T55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="U55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="V55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="W55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="X55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AG55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AN55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AO55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AP55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AQ55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AR55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AS55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AT55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AU55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AV55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AW55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AX55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AY55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AZ55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BA55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BB55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BC55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BD55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BE55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BF55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BG55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BH55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BI55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BJ55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BK55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BL55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BM55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BN55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BO55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BP55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BQ55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BR55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BS55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BT55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BU55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BV55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BW55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BX55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BY55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="BZ55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="CA55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="CB55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="CC55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="CD55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="CE55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="CF55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="CG55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="CH55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="CI55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="CJ55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="CK55" s="6" t="s">
+      <c r="A54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="O54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="R54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="S54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="T54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="U54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="V54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="W54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="X54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AN54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AR54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AY54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BD54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BE54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BF54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BI54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BJ54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BK54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BL54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BM54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BN54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BO54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BP54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BQ54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BR54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BS54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BT54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BU54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BV54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BW54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BX54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BY54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BZ54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CA54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CB54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CC54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CD54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CE54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CF54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CG54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CH54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CI54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CJ54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="CK54" s="6" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tested download of reports
</commit_message>
<xml_diff>
--- a/exceltocsv/public/reports/DTRSUMMARY.xlsx
+++ b/exceltocsv/public/reports/DTRSUMMARY.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="199" xml:space="preserve">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="201" xml:space="preserve">
   <si>
     <t>iRipple, Inc. | DTR Summary Sheet for the period May 09, 2015 to May 22, 2015</t>
   </si>
@@ -320,99 +320,108 @@
     <t>Enterprise - Ayagold</t>
   </si>
   <si>
+    <t>3.4.0</t>
+  </si>
+  <si>
+    <t>Bernardo, Gianilla Mae</t>
+  </si>
+  <si>
+    <t>0.0.30</t>
+  </si>
+  <si>
+    <t>2.4.0</t>
+  </si>
+  <si>
+    <t>Biana, Kristine Joy</t>
+  </si>
+  <si>
+    <t>Marketing &amp;amp; Hardware</t>
+  </si>
+  <si>
+    <t>0.1.0</t>
+  </si>
+  <si>
+    <t>Borlagdan, Aldrin</t>
+  </si>
+  <si>
+    <t>ATVI</t>
+  </si>
+  <si>
+    <t>4.0.0</t>
+  </si>
+  <si>
+    <t>Buena, Ian Christopher</t>
+  </si>
+  <si>
+    <t>0.2.45</t>
+  </si>
+  <si>
+    <t>Buenafe, Rajiv</t>
+  </si>
+  <si>
+    <t>10.0.0</t>
+  </si>
+  <si>
+    <t>Cansino, Oliver</t>
+  </si>
+  <si>
+    <t>Cataluna, Christian Gilbert</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>2.0.0</t>
+  </si>
+  <si>
     <t>4.4.0</t>
   </si>
   <si>
-    <t>Bernardo, Gianilla Mae</t>
-  </si>
-  <si>
-    <t>0.0.30</t>
-  </si>
-  <si>
-    <t>2.4.0</t>
-  </si>
-  <si>
-    <t>Biana, Kristine Joy</t>
-  </si>
-  <si>
-    <t>Marketing &amp;amp; Hardware</t>
-  </si>
-  <si>
-    <t>0.1.0</t>
+    <t>CaÃ±ete, Carol Ann</t>
+  </si>
+  <si>
+    <t>0.4.0</t>
+  </si>
+  <si>
+    <t>5.4.0</t>
+  </si>
+  <si>
+    <t>Cerbo, Jaycer</t>
+  </si>
+  <si>
+    <t>1.7.0</t>
+  </si>
+  <si>
+    <t>Ching, Mark Angelo</t>
+  </si>
+  <si>
+    <t>Imaghine</t>
+  </si>
+  <si>
+    <t>0.6.45</t>
+  </si>
+  <si>
+    <t>Cortez, Jomar</t>
+  </si>
+  <si>
+    <t>1.4.0</t>
+  </si>
+  <si>
+    <t>6.0.0</t>
+  </si>
+  <si>
+    <t>Cruz, Cesar</t>
+  </si>
+  <si>
+    <t>Delfin, Jonathan</t>
+  </si>
+  <si>
+    <t>International Business - PNG</t>
   </si>
   <si>
     <t>0.2.0</t>
   </si>
   <si>
-    <t>Borlagdan, Aldrin</t>
-  </si>
-  <si>
-    <t>ATVI</t>
-  </si>
-  <si>
-    <t>4.0.0</t>
-  </si>
-  <si>
-    <t>Buena, Ian Christopher</t>
-  </si>
-  <si>
-    <t>0.2.45</t>
-  </si>
-  <si>
-    <t>Buenafe, Rajiv</t>
-  </si>
-  <si>
-    <t>10.0.0</t>
-  </si>
-  <si>
-    <t>Cansino, Oliver</t>
-  </si>
-  <si>
-    <t>Cataluna, Christian Gilbert</t>
-  </si>
-  <si>
-    <t>Sales</t>
-  </si>
-  <si>
-    <t>CaÃ±ete, Carol Ann</t>
-  </si>
-  <si>
-    <t>Cerbo, Jaycer</t>
-  </si>
-  <si>
-    <t>1.7.0</t>
-  </si>
-  <si>
-    <t>Ching, Mark Angelo</t>
-  </si>
-  <si>
-    <t>Imaghine</t>
-  </si>
-  <si>
-    <t>0.6.45</t>
-  </si>
-  <si>
-    <t>Cortez, Jomar</t>
-  </si>
-  <si>
-    <t>5.4.0</t>
-  </si>
-  <si>
-    <t>2.0.0</t>
-  </si>
-  <si>
-    <t>Cruz, Cesar</t>
-  </si>
-  <si>
-    <t>1.4.0</t>
-  </si>
-  <si>
-    <t>Delfin, Jonathan</t>
-  </si>
-  <si>
-    <t>International Business - PNG</t>
-  </si>
-  <si>
     <t>Dino, Arvin</t>
   </si>
   <si>
@@ -449,30 +458,33 @@
     <t>0.1.30</t>
   </si>
   <si>
+    <t>0.6.30</t>
+  </si>
+  <si>
+    <t>Fadrilan, Liezl</t>
+  </si>
+  <si>
+    <t>Synext (Nexus)</t>
+  </si>
+  <si>
+    <t>9.0.0</t>
+  </si>
+  <si>
+    <t>Flores, Arianne Grace</t>
+  </si>
+  <si>
+    <t>0.5.0</t>
+  </si>
+  <si>
+    <t>1.2.0</t>
+  </si>
+  <si>
+    <t>Francisco, Roed Ronualdo </t>
+  </si>
+  <si>
     <t>0.6.0</t>
   </si>
   <si>
-    <t>Fadrilan, Liezl</t>
-  </si>
-  <si>
-    <t>Synext (Nexus)</t>
-  </si>
-  <si>
-    <t>9.0.0</t>
-  </si>
-  <si>
-    <t>Flores, Arianne Grace</t>
-  </si>
-  <si>
-    <t>0.5.0</t>
-  </si>
-  <si>
-    <t>1.2.0</t>
-  </si>
-  <si>
-    <t>Francisco, Roed Ronualdo </t>
-  </si>
-  <si>
     <t>Golo, Rianna Rae</t>
   </si>
   <si>
@@ -482,9 +494,6 @@
     <t>Hernandez, Paulyn Gean</t>
   </si>
   <si>
-    <t>0.4.0</t>
-  </si>
-  <si>
     <t>Javier, Victor </t>
   </si>
   <si>
@@ -518,13 +527,10 @@
     <t>Mendoza, Diana</t>
   </si>
   <si>
-    <t>0.6.30</t>
-  </si>
-  <si>
     <t>Muncal, Ardo</t>
   </si>
   <si>
-    <t>2.3.0</t>
+    <t>2.5.0</t>
   </si>
   <si>
     <t>Nagnal, Fracy</t>
@@ -2199,7 +2205,7 @@
         <v>81</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K7" s="5" t="str">
         <f>INT(LEFT(E7,2))</f>
@@ -4193,7 +4199,7 @@
         <f>FLOOR(AS14/8,1)&amp;"."&amp;FLOOR(MOD(AS14,8),1)&amp;"."&amp;(MOD(AS14,8)-FLOOR(MOD(AS14,8),1))*60</f>
       </c>
       <c r="AU14" s="5" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="AV14" s="5" t="s">
         <v>81</v>
@@ -4327,10 +4333,10 @@
         <v>12</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="D15" s="5" t="n">
         <v>1</v>
@@ -4573,7 +4579,7 @@
         <f>FLOOR(CC15/8,1)&amp;"."&amp;FLOOR(MOD(CC15,8),1)&amp;"."&amp;(MOD(CC15,8)-FLOOR(MOD(CC15,8),1))*60</f>
       </c>
       <c r="CF15" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="CG15" s="5" t="str">
         <f>INT(LEFT(CF15,2))</f>
@@ -4596,10 +4602,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D16" s="5" t="n">
         <v>1</v>
@@ -4608,7 +4614,7 @@
         <v>109</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>81</v>
@@ -4842,7 +4848,7 @@
         <f>FLOOR(CC16/8,1)&amp;"."&amp;FLOOR(MOD(CC16,8),1)&amp;"."&amp;(MOD(CC16,8)-FLOOR(MOD(CC16,8),1))*60</f>
       </c>
       <c r="CF16" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="CG16" s="5" t="str">
         <f>INT(LEFT(CF16,2))</f>
@@ -4865,7 +4871,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>84</v>
@@ -5111,7 +5117,7 @@
         <f>FLOOR(CC17/8,1)&amp;"."&amp;FLOOR(MOD(CC17,8),1)&amp;"."&amp;(MOD(CC17,8)-FLOOR(MOD(CC17,8),1))*60</f>
       </c>
       <c r="CF17" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="CG17" s="5" t="str">
         <f>INT(LEFT(CF17,2))</f>
@@ -5134,7 +5140,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>99</v>
@@ -5403,10 +5409,10 @@
         <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>119</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="D19" s="5" t="n">
         <v>0</v>
@@ -5421,13 +5427,13 @@
         <v>81</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>81</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="K19" s="5" t="str">
         <f>INT(LEFT(E19,2))</f>
@@ -5649,7 +5655,7 @@
         <f>FLOOR(CC19/8,1)&amp;"."&amp;FLOOR(MOD(CC19,8),1)&amp;"."&amp;(MOD(CC19,8)-FLOOR(MOD(CC19,8),1))*60</f>
       </c>
       <c r="CF19" s="5" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="CG19" s="5" t="str">
         <f>INT(LEFT(CF19,2))</f>
@@ -5672,7 +5678,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>97</v>
@@ -5687,7 +5693,7 @@
         <v>81</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>81</v>
+        <v>123</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>82</v>
@@ -5696,7 +5702,7 @@
         <v>81</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
       <c r="K20" s="5" t="str">
         <f>INT(LEFT(E20,2))</f>
@@ -5941,7 +5947,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>99</v>
@@ -6079,7 +6085,7 @@
         <v>81</v>
       </c>
       <c r="AV21" s="5" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AW21" s="5" t="s">
         <v>81</v>
@@ -6210,10 +6216,10 @@
         <v>19</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D22" s="5" t="n">
         <v>1</v>
@@ -6222,7 +6228,7 @@
         <v>95</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>81</v>
@@ -6456,7 +6462,7 @@
         <f>FLOOR(CC22/8,1)&amp;"."&amp;FLOOR(MOD(CC22,8),1)&amp;"."&amp;(MOD(CC22,8)-FLOOR(MOD(CC22,8),1))*60</f>
       </c>
       <c r="CF22" s="5" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="CG22" s="5" t="str">
         <f>INT(LEFT(CF22,2))</f>
@@ -6479,7 +6485,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>80</v>
@@ -6494,7 +6500,7 @@
         <v>81</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>86</v>
+        <v>131</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>82</v>
@@ -6503,7 +6509,7 @@
         <v>81</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="K23" s="5" t="str">
         <f>INT(LEFT(E23,2))</f>
@@ -6725,7 +6731,7 @@
         <f>FLOOR(CC23/8,1)&amp;"."&amp;FLOOR(MOD(CC23,8),1)&amp;"."&amp;(MOD(CC23,8)-FLOOR(MOD(CC23,8),1))*60</f>
       </c>
       <c r="CF23" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="CG23" s="5" t="str">
         <f>INT(LEFT(CF23,2))</f>
@@ -6748,7 +6754,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>99</v>
@@ -6763,7 +6769,7 @@
         <v>81</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>82</v>
@@ -6994,7 +7000,7 @@
         <f>FLOOR(CC24/8,1)&amp;"."&amp;FLOOR(MOD(CC24,8),1)&amp;"."&amp;(MOD(CC24,8)-FLOOR(MOD(CC24,8),1))*60</f>
       </c>
       <c r="CF24" s="5" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="CG24" s="5" t="str">
         <f>INT(LEFT(CF24,2))</f>
@@ -7017,10 +7023,10 @@
         <v>22</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D25" s="5" t="n">
         <v>0</v>
@@ -7152,7 +7158,7 @@
         <f>FLOOR(AS25/8,1)&amp;"."&amp;FLOOR(MOD(AS25,8),1)&amp;"."&amp;(MOD(AS25,8)-FLOOR(MOD(AS25,8),1))*60</f>
       </c>
       <c r="AU25" s="5" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="AV25" s="5" t="s">
         <v>81</v>
@@ -7286,10 +7292,10 @@
         <v>23</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D26" s="5" t="n">
         <v>0</v>
@@ -7298,7 +7304,7 @@
         <v>81</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>81</v>
@@ -7555,10 +7561,10 @@
         <v>24</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D27" s="5" t="n">
         <v>0</v>
@@ -7824,7 +7830,7 @@
         <v>25</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>80</v>
@@ -7836,7 +7842,7 @@
         <v>95</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>81</v>
@@ -7959,7 +7965,7 @@
         <f>FLOOR(AS28/8,1)&amp;"."&amp;FLOOR(MOD(AS28,8),1)&amp;"."&amp;(MOD(AS28,8)-FLOOR(MOD(AS28,8),1))*60</f>
       </c>
       <c r="AU28" s="5" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="AV28" s="5" t="s">
         <v>86</v>
@@ -8070,7 +8076,7 @@
         <f>FLOOR(CC28/8,1)&amp;"."&amp;FLOOR(MOD(CC28,8),1)&amp;"."&amp;(MOD(CC28,8)-FLOOR(MOD(CC28,8),1))*60</f>
       </c>
       <c r="CF28" s="5" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="CG28" s="5" t="str">
         <f>INT(LEFT(CF28,2))</f>
@@ -8093,10 +8099,10 @@
         <v>26</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D29" s="5" t="n">
         <v>0</v>
@@ -8362,19 +8368,19 @@
         <v>27</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D30" s="5" t="n">
         <v>3</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>81</v>
@@ -8497,7 +8503,7 @@
         <f>FLOOR(AS30/8,1)&amp;"."&amp;FLOOR(MOD(AS30,8),1)&amp;"."&amp;(MOD(AS30,8)-FLOOR(MOD(AS30,8),1))*60</f>
       </c>
       <c r="AU30" s="5" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="AV30" s="5" t="s">
         <v>81</v>
@@ -8631,10 +8637,10 @@
         <v>28</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D31" s="5" t="n">
         <v>0</v>
@@ -8877,7 +8883,7 @@
         <f>FLOOR(CC31/8,1)&amp;"."&amp;FLOOR(MOD(CC31,8),1)&amp;"."&amp;(MOD(CC31,8)-FLOOR(MOD(CC31,8),1))*60</f>
       </c>
       <c r="CF31" s="5" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="CG31" s="5" t="str">
         <f>INT(LEFT(CF31,2))</f>
@@ -8900,7 +8906,7 @@
         <v>29</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>90</v>
@@ -8915,7 +8921,7 @@
         <v>81</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>86</v>
+        <v>131</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>82</v>
@@ -8924,7 +8930,7 @@
         <v>81</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="K32" s="5" t="str">
         <f>INT(LEFT(E32,2))</f>
@@ -9035,10 +9041,10 @@
         <f>FLOOR(AS32/8,1)&amp;"."&amp;FLOOR(MOD(AS32,8),1)&amp;"."&amp;(MOD(AS32,8)-FLOOR(MOD(AS32,8),1))*60</f>
       </c>
       <c r="AU32" s="5" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="AV32" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="AW32" s="5" t="s">
         <v>81</v>
@@ -9146,7 +9152,7 @@
         <f>FLOOR(CC32/8,1)&amp;"."&amp;FLOOR(MOD(CC32,8),1)&amp;"."&amp;(MOD(CC32,8)-FLOOR(MOD(CC32,8),1))*60</f>
       </c>
       <c r="CF32" s="5" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
       <c r="CG32" s="5" t="str">
         <f>INT(LEFT(CF32,2))</f>
@@ -9169,7 +9175,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>99</v>
@@ -9307,7 +9313,7 @@
         <v>81</v>
       </c>
       <c r="AV33" s="5" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="AW33" s="5" t="s">
         <v>81</v>
@@ -9438,16 +9444,16 @@
         <v>31</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D34" s="5" t="n">
         <v>2</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>81</v>
@@ -9707,7 +9713,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>99</v>
@@ -9953,7 +9959,7 @@
         <f>FLOOR(CC35/8,1)&amp;"."&amp;FLOOR(MOD(CC35,8),1)&amp;"."&amp;(MOD(CC35,8)-FLOOR(MOD(CC35,8),1))*60</f>
       </c>
       <c r="CF35" s="5" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="CG35" s="5" t="str">
         <f>INT(LEFT(CF35,2))</f>
@@ -9976,10 +9982,10 @@
         <v>33</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D36" s="5" t="n">
         <v>0</v>
@@ -10222,7 +10228,7 @@
         <f>FLOOR(CC36/8,1)&amp;"."&amp;FLOOR(MOD(CC36,8),1)&amp;"."&amp;(MOD(CC36,8)-FLOOR(MOD(CC36,8),1))*60</f>
       </c>
       <c r="CF36" s="5" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="CG36" s="5" t="str">
         <f>INT(LEFT(CF36,2))</f>
@@ -10245,10 +10251,10 @@
         <v>34</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D37" s="5" t="n">
         <v>2</v>
@@ -10491,7 +10497,7 @@
         <f>FLOOR(CC37/8,1)&amp;"."&amp;FLOOR(MOD(CC37,8),1)&amp;"."&amp;(MOD(CC37,8)-FLOOR(MOD(CC37,8),1))*60</f>
       </c>
       <c r="CF37" s="5" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="CG37" s="5" t="str">
         <f>INT(LEFT(CF37,2))</f>
@@ -10514,10 +10520,10 @@
         <v>35</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D38" s="5" t="n">
         <v>0</v>
@@ -10760,7 +10766,7 @@
         <f>FLOOR(CC38/8,1)&amp;"."&amp;FLOOR(MOD(CC38,8),1)&amp;"."&amp;(MOD(CC38,8)-FLOOR(MOD(CC38,8),1))*60</f>
       </c>
       <c r="CF38" s="5" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="CG38" s="5" t="str">
         <f>INT(LEFT(CF38,2))</f>
@@ -10783,7 +10789,7 @@
         <v>36</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>84</v>
@@ -11052,16 +11058,16 @@
         <v>37</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D40" s="5" t="n">
         <v>4</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>81</v>
@@ -11187,7 +11193,7 @@
         <f>FLOOR(AS40/8,1)&amp;"."&amp;FLOOR(MOD(AS40,8),1)&amp;"."&amp;(MOD(AS40,8)-FLOOR(MOD(AS40,8),1))*60</f>
       </c>
       <c r="AU40" s="5" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="AV40" s="5" t="s">
         <v>81</v>
@@ -11321,16 +11327,16 @@
         <v>38</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D41" s="5" t="n">
         <v>7</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>81</v>
@@ -11567,7 +11573,7 @@
         <f>FLOOR(CC41/8,1)&amp;"."&amp;FLOOR(MOD(CC41,8),1)&amp;"."&amp;(MOD(CC41,8)-FLOOR(MOD(CC41,8),1))*60</f>
       </c>
       <c r="CF41" s="5" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="CG41" s="5" t="str">
         <f>INT(LEFT(CF41,2))</f>
@@ -11590,7 +11596,7 @@
         <v>39</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>97</v>
@@ -11599,7 +11605,7 @@
         <v>9</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>81</v>
@@ -11836,7 +11842,7 @@
         <f>FLOOR(CC42/8,1)&amp;"."&amp;FLOOR(MOD(CC42,8),1)&amp;"."&amp;(MOD(CC42,8)-FLOOR(MOD(CC42,8),1))*60</f>
       </c>
       <c r="CF42" s="5" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="CG42" s="5" t="str">
         <f>INT(LEFT(CF42,2))</f>
@@ -11859,16 +11865,16 @@
         <v>40</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D43" s="5" t="n">
         <v>5</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>81</v>
@@ -11994,7 +12000,7 @@
         <f>FLOOR(AS43/8,1)&amp;"."&amp;FLOOR(MOD(AS43,8),1)&amp;"."&amp;(MOD(AS43,8)-FLOOR(MOD(AS43,8),1))*60</f>
       </c>
       <c r="AU43" s="5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="AV43" s="5" t="s">
         <v>81</v>
@@ -12128,7 +12134,7 @@
         <v>41</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>84</v>
@@ -12374,7 +12380,7 @@
         <f>FLOOR(CC44/8,1)&amp;"."&amp;FLOOR(MOD(CC44,8),1)&amp;"."&amp;(MOD(CC44,8)-FLOOR(MOD(CC44,8),1))*60</f>
       </c>
       <c r="CF44" s="5" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="CG44" s="5" t="str">
         <f>INT(LEFT(CF44,2))</f>
@@ -12397,7 +12403,7 @@
         <v>42</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>99</v>
@@ -12532,7 +12538,7 @@
         <f>FLOOR(AS45/8,1)&amp;"."&amp;FLOOR(MOD(AS45,8),1)&amp;"."&amp;(MOD(AS45,8)-FLOOR(MOD(AS45,8),1))*60</f>
       </c>
       <c r="AU45" s="5" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="AV45" s="5" t="s">
         <v>81</v>
@@ -12643,7 +12649,7 @@
         <f>FLOOR(CC45/8,1)&amp;"."&amp;FLOOR(MOD(CC45,8),1)&amp;"."&amp;(MOD(CC45,8)-FLOOR(MOD(CC45,8),1))*60</f>
       </c>
       <c r="CF45" s="5" t="s">
-        <v>167</v>
+        <v>120</v>
       </c>
       <c r="CG45" s="5" t="str">
         <f>INT(LEFT(CF45,2))</f>
@@ -12666,10 +12672,10 @@
         <v>43</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D46" s="5" t="n">
         <v>0</v>
@@ -12935,10 +12941,10 @@
         <v>44</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D47" s="5" t="n">
         <v>1</v>
@@ -13181,7 +13187,7 @@
         <f>FLOOR(CC47/8,1)&amp;"."&amp;FLOOR(MOD(CC47,8),1)&amp;"."&amp;(MOD(CC47,8)-FLOOR(MOD(CC47,8),1))*60</f>
       </c>
       <c r="CF47" s="5" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="CG47" s="5" t="str">
         <f>INT(LEFT(CF47,2))</f>
@@ -13204,10 +13210,10 @@
         <v>45</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D48" s="5" t="n">
         <v>0</v>
@@ -13473,10 +13479,10 @@
         <v>46</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D49" s="5" t="n">
         <v>2</v>
@@ -13719,7 +13725,7 @@
         <f>FLOOR(CC49/8,1)&amp;"."&amp;FLOOR(MOD(CC49,8),1)&amp;"."&amp;(MOD(CC49,8)-FLOOR(MOD(CC49,8),1))*60</f>
       </c>
       <c r="CF49" s="5" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="CG49" s="5" t="str">
         <f>INT(LEFT(CF49,2))</f>
@@ -13742,16 +13748,16 @@
         <v>47</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D50" s="5" t="n">
         <v>4</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>81</v>
@@ -13988,7 +13994,7 @@
         <f>FLOOR(CC50/8,1)&amp;"."&amp;FLOOR(MOD(CC50,8),1)&amp;"."&amp;(MOD(CC50,8)-FLOOR(MOD(CC50,8),1))*60</f>
       </c>
       <c r="CF50" s="5" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="CG50" s="5" t="str">
         <f>INT(LEFT(CF50,2))</f>
@@ -14011,7 +14017,7 @@
         <v>48</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>99</v>
@@ -14020,7 +14026,7 @@
         <v>6</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>81</v>
@@ -14280,7 +14286,7 @@
         <v>49</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>102</v>
@@ -14289,7 +14295,7 @@
         <v>2</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>109</v>
@@ -14526,7 +14532,7 @@
         <f>FLOOR(CC52/8,1)&amp;"."&amp;FLOOR(MOD(CC52,8),1)&amp;"."&amp;(MOD(CC52,8)-FLOOR(MOD(CC52,8),1))*60</f>
       </c>
       <c r="CF52" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="CG52" s="5" t="str">
         <f>INT(LEFT(CF52,2))</f>
@@ -14549,7 +14555,7 @@
         <v>50</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>80</v>
@@ -14561,7 +14567,7 @@
         <v>81</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>81</v>
@@ -14573,7 +14579,7 @@
         <v>81</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="K53" s="5" t="str">
         <f>INT(LEFT(E53,2))</f>
@@ -14795,7 +14801,7 @@
         <f>FLOOR(CC53/8,1)&amp;"."&amp;FLOOR(MOD(CC53,8),1)&amp;"."&amp;(MOD(CC53,8)-FLOOR(MOD(CC53,8),1))*60</f>
       </c>
       <c r="CF53" s="5" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="CG53" s="5" t="str">
         <f>INT(LEFT(CF53,2))</f>
@@ -14818,7 +14824,7 @@
         <v>51</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>80</v>
@@ -15087,10 +15093,10 @@
         <v>52</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D55" s="5" t="n">
         <v>3</v>
@@ -15222,7 +15228,7 @@
         <f>FLOOR(AS55/8,1)&amp;"."&amp;FLOOR(MOD(AS55,8),1)&amp;"."&amp;(MOD(AS55,8)-FLOOR(MOD(AS55,8),1))*60</f>
       </c>
       <c r="AU55" s="5" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="AV55" s="5" t="s">
         <v>81</v>
@@ -15356,10 +15362,10 @@
         <v>53</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D56" s="5" t="n">
         <v>1</v>
@@ -15371,7 +15377,7 @@
         <v>81</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>81</v>
+        <v>123</v>
       </c>
       <c r="H56" s="5" t="s">
         <v>82</v>
@@ -15491,10 +15497,10 @@
         <f>FLOOR(AS56/8,1)&amp;"."&amp;FLOOR(MOD(AS56,8),1)&amp;"."&amp;(MOD(AS56,8)-FLOOR(MOD(AS56,8),1))*60</f>
       </c>
       <c r="AU56" s="5" t="s">
-        <v>190</v>
+        <v>126</v>
       </c>
       <c r="AV56" s="5" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="AW56" s="5" t="s">
         <v>81</v>
@@ -15602,7 +15608,7 @@
         <f>FLOOR(CC56/8,1)&amp;"."&amp;FLOOR(MOD(CC56,8),1)&amp;"."&amp;(MOD(CC56,8)-FLOOR(MOD(CC56,8),1))*60</f>
       </c>
       <c r="CF56" s="5" t="s">
-        <v>131</v>
+        <v>86</v>
       </c>
       <c r="CG56" s="5" t="str">
         <f>INT(LEFT(CF56,2))</f>
@@ -15625,22 +15631,22 @@
         <v>54</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>102</v>
       </c>
       <c r="D57" s="5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>185</v>
+        <v>94</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="H57" s="5" t="s">
         <v>82</v>
@@ -15649,7 +15655,7 @@
         <v>81</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="K57" s="5" t="str">
         <f>INT(LEFT(E57,2))</f>
@@ -15894,7 +15900,7 @@
         <v>55</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>102</v>
@@ -15909,7 +15915,7 @@
         <v>81</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>81</v>
+        <v>123</v>
       </c>
       <c r="H58" s="5" t="s">
         <v>82</v>
@@ -16140,7 +16146,7 @@
         <f>FLOOR(CC58/8,1)&amp;"."&amp;FLOOR(MOD(CC58,8),1)&amp;"."&amp;(MOD(CC58,8)-FLOOR(MOD(CC58,8),1))*60</f>
       </c>
       <c r="CF58" s="5" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="CG58" s="5" t="str">
         <f>INT(LEFT(CF58,2))</f>
@@ -16163,7 +16169,7 @@
         <v>56</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>90</v>
@@ -16432,16 +16438,16 @@
         <v>57</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D60" s="5" t="n">
         <v>3</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>81</v>
@@ -16678,7 +16684,7 @@
         <f>FLOOR(CC60/8,1)&amp;"."&amp;FLOOR(MOD(CC60,8),1)&amp;"."&amp;(MOD(CC60,8)-FLOOR(MOD(CC60,8),1))*60</f>
       </c>
       <c r="CF60" s="5" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="CG60" s="5" t="str">
         <f>INT(LEFT(CF60,2))</f>
@@ -16701,7 +16707,7 @@
         <v>58</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>108</v>
@@ -16947,7 +16953,7 @@
         <f>FLOOR(CC61/8,1)&amp;"."&amp;FLOOR(MOD(CC61,8),1)&amp;"."&amp;(MOD(CC61,8)-FLOOR(MOD(CC61,8),1))*60</f>
       </c>
       <c r="CF61" s="5" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="CG61" s="5" t="str">
         <f>INT(LEFT(CF61,2))</f>
@@ -16970,7 +16976,7 @@
         <v>59</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>80</v>
@@ -17216,7 +17222,7 @@
         <f>FLOOR(CC62/8,1)&amp;"."&amp;FLOOR(MOD(CC62,8),1)&amp;"."&amp;(MOD(CC62,8)-FLOOR(MOD(CC62,8),1))*60</f>
       </c>
       <c r="CF62" s="5" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="CG62" s="5" t="str">
         <f>INT(LEFT(CF62,2))</f>
@@ -17239,7 +17245,7 @@
         <v>60</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>99</v>
@@ -17485,7 +17491,7 @@
         <f>FLOOR(CC63/8,1)&amp;"."&amp;FLOOR(MOD(CC63,8),1)&amp;"."&amp;(MOD(CC63,8)-FLOOR(MOD(CC63,8),1))*60</f>
       </c>
       <c r="CF63" s="5" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="CG63" s="5" t="str">
         <f>INT(LEFT(CF63,2))</f>
@@ -17508,7 +17514,7 @@
         <v>61</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>90</v>
@@ -17754,7 +17760,7 @@
         <f>FLOOR(CC64/8,1)&amp;"."&amp;FLOOR(MOD(CC64,8),1)&amp;"."&amp;(MOD(CC64,8)-FLOOR(MOD(CC64,8),1))*60</f>
       </c>
       <c r="CF64" s="5" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="CG64" s="5" t="str">
         <f>INT(LEFT(CF64,2))</f>

</xml_diff>